<commit_message>
Cleaned up storm intervals
Intervals were overlapping after multiple storms needed to be combined.
Added and tuned up Q and S storm summary tables
</commit_message>
<xml_diff>
--- a/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
+++ b/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
@@ -393,7 +393,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -440,10 +440,10 @@
         <v>7.5</v>
       </c>
       <c s="2" r="E2" t="n">
-        <v>40927.5625</v>
+        <v>40941.25</v>
       </c>
       <c s="2" r="F2" t="n">
-        <v>40927.947916666664</v>
+        <v>40941.770833333336</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -460,10 +460,10 @@
         <v>9.25</v>
       </c>
       <c s="2" r="E3" t="n">
-        <v>40933.15625</v>
+        <v>40942.052083333336</v>
       </c>
       <c s="2" r="F3" t="n">
-        <v>40933.666666666664</v>
+        <v>40942.135416666664</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -480,10 +480,10 @@
         <v>12.25</v>
       </c>
       <c s="2" r="E4" t="n">
-        <v>40941.25</v>
+        <v>40942.135416666664</v>
       </c>
       <c s="2" r="F4" t="n">
-        <v>40941.770833333336</v>
+        <v>40942.229166666664</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -500,10 +500,10 @@
         <v>12.5</v>
       </c>
       <c s="2" r="E5" t="n">
-        <v>40942.052083333336</v>
+        <v>40942.229166666664</v>
       </c>
       <c s="2" r="F5" t="n">
-        <v>40942.135416666664</v>
+        <v>40942.322916666664</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -514,2269 +514,2197 @@
         <v>40942.052083333336</v>
       </c>
       <c s="2" r="C6" t="n">
-        <v>40942.229166666664</v>
+        <v>40942.895833333336</v>
       </c>
       <c r="D6" t="n">
         <v>2.0</v>
       </c>
       <c s="2" r="E6" t="n">
-        <v>40942.135416666664</v>
+        <v>40942.322916666664</v>
       </c>
       <c s="2" r="F6" t="n">
-        <v>40942.229166666664</v>
+        <v>40942.895833333336</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c s="1" r="A7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c s="2" r="B7" t="n">
-        <v>40942.135416666664</v>
+        <v>40944.416666666664</v>
       </c>
       <c s="2" r="C7" t="n">
-        <v>40942.322916666664</v>
+        <v>40944.895833333336</v>
       </c>
       <c r="D7" t="n">
-        <v>2.25</v>
+        <v>11.5</v>
       </c>
       <c s="2" r="E7" t="n">
-        <v>40942.229166666664</v>
+        <v>40976.6875</v>
       </c>
       <c s="2" r="F7" t="n">
-        <v>40942.322916666664</v>
+        <v>40976.854166666664</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c s="1" r="A8" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c s="2" r="B8" t="n">
-        <v>40942.229166666664</v>
+        <v>40944.958333333336</v>
       </c>
       <c s="2" r="C8" t="n">
-        <v>40942.895833333336</v>
+        <v>40947.0</v>
       </c>
       <c r="D8" t="n">
-        <v>2.25</v>
+        <v>49.0</v>
       </c>
       <c s="2" r="E8" t="n">
-        <v>40942.322916666664</v>
+        <v>40977.25</v>
       </c>
       <c s="2" r="F8" t="n">
-        <v>40942.895833333336</v>
+        <v>40977.583333333336</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c s="1" r="A9" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c s="2" r="B9" t="n">
-        <v>40944.416666666664</v>
+        <v>40962.864583333336</v>
       </c>
       <c s="2" r="C9" t="n">
-        <v>40944.895833333336</v>
+        <v>40963.21875</v>
       </c>
       <c r="D9" t="n">
-        <v>11.5</v>
+        <v>8.5</v>
       </c>
       <c s="2" r="E9" t="n">
-        <v>40944.958333333336</v>
+        <v>40984.416666666664</v>
       </c>
       <c s="2" r="F9" t="n">
-        <v>40947.0</v>
+        <v>40984.6875</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c s="1" r="A10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c s="2" r="B10" t="n">
-        <v>40944.958333333336</v>
+        <v>40976.6875</v>
       </c>
       <c s="2" r="C10" t="n">
-        <v>40947.0</v>
+        <v>40976.854166666664</v>
       </c>
       <c r="D10" t="n">
-        <v>49.0</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E10" t="n">
-        <v>40962.864583333336</v>
+        <v>40985.489583333336</v>
       </c>
       <c s="2" r="F10" t="n">
-        <v>40963.21875</v>
+        <v>40985.739583333336</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c s="1" r="A11" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c s="2" r="B11" t="n">
-        <v>40962.864583333336</v>
+        <v>40977.25</v>
       </c>
       <c s="2" r="C11" t="n">
-        <v>40963.21875</v>
+        <v>40977.583333333336</v>
       </c>
       <c r="D11" t="n">
-        <v>8.5</v>
+        <v>8.0</v>
       </c>
       <c s="2" r="E11" t="n">
-        <v>40976.6875</v>
+        <v>40989.84375</v>
       </c>
       <c s="2" r="F11" t="n">
-        <v>40976.854166666664</v>
+        <v>40990.145833333336</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c s="1" r="A12" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c s="2" r="B12" t="n">
-        <v>40976.6875</v>
+        <v>40984.416666666664</v>
       </c>
       <c s="2" r="C12" t="n">
-        <v>40976.854166666664</v>
+        <v>40984.6875</v>
       </c>
       <c r="D12" t="n">
-        <v>4.0</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E12" t="n">
-        <v>40977.25</v>
+        <v>40990.21875</v>
       </c>
       <c s="2" r="F12" t="n">
-        <v>40977.583333333336</v>
+        <v>40990.302083333336</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c s="1" r="A13" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c s="2" r="B13" t="n">
-        <v>40977.25</v>
+        <v>40985.489583333336</v>
       </c>
       <c s="2" r="C13" t="n">
-        <v>40977.583333333336</v>
+        <v>40985.739583333336</v>
       </c>
       <c r="D13" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E13" t="n">
-        <v>40984.416666666664</v>
+        <v>40990.90625</v>
       </c>
       <c s="2" r="F13" t="n">
-        <v>40984.6875</v>
+        <v>40991.322916666664</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c s="1" r="A14" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c s="2" r="B14" t="n">
-        <v>40984.416666666664</v>
+        <v>40989.84375</v>
       </c>
       <c s="2" r="C14" t="n">
-        <v>40984.6875</v>
+        <v>40990.145833333336</v>
       </c>
       <c r="D14" t="n">
-        <v>6.5</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E14" t="n">
-        <v>40985.489583333336</v>
+        <v>40993.145833333336</v>
       </c>
       <c s="2" r="F14" t="n">
-        <v>40985.739583333336</v>
+        <v>40993.947916666664</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c s="1" r="A15" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c s="2" r="B15" t="n">
-        <v>40985.489583333336</v>
+        <v>40990.21875</v>
       </c>
       <c s="2" r="C15" t="n">
-        <v>40985.739583333336</v>
+        <v>40990.302083333336</v>
       </c>
       <c r="D15" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E15" t="n">
-        <v>40989.84375</v>
+        <v>41031.677083333336</v>
       </c>
       <c s="2" r="F15" t="n">
-        <v>40990.145833333336</v>
+        <v>41031.75</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c s="1" r="A16" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c s="2" r="B16" t="n">
-        <v>40989.84375</v>
+        <v>40990.90625</v>
       </c>
       <c s="2" r="C16" t="n">
-        <v>40990.145833333336</v>
+        <v>40991.322916666664</v>
       </c>
       <c r="D16" t="n">
-        <v>7.25</v>
+        <v>10.0</v>
       </c>
       <c s="2" r="E16" t="n">
-        <v>40990.21875</v>
+        <v>41037.197916666664</v>
       </c>
       <c s="2" r="F16" t="n">
-        <v>40990.302083333336</v>
+        <v>41037.333333333336</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c s="1" r="A17" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c s="2" r="B17" t="n">
-        <v>40990.21875</v>
+        <v>40993.145833333336</v>
       </c>
       <c s="2" r="C17" t="n">
-        <v>40990.302083333336</v>
+        <v>40993.947916666664</v>
       </c>
       <c r="D17" t="n">
-        <v>2.0</v>
+        <v>19.25</v>
       </c>
       <c s="2" r="E17" t="n">
-        <v>40990.90625</v>
+        <v>41051.78125</v>
       </c>
       <c s="2" r="F17" t="n">
-        <v>40991.322916666664</v>
+        <v>41052.125</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c s="1" r="A18" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c s="2" r="B18" t="n">
-        <v>40990.90625</v>
+        <v>41031.677083333336</v>
       </c>
       <c s="2" r="C18" t="n">
-        <v>40991.322916666664</v>
+        <v>41031.75</v>
       </c>
       <c r="D18" t="n">
-        <v>10.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E18" t="n">
-        <v>40993.145833333336</v>
+        <v>41052.322916666664</v>
       </c>
       <c s="2" r="F18" t="n">
-        <v>40993.947916666664</v>
+        <v>41053.583333333336</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c s="1" r="A19" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c s="2" r="B19" t="n">
-        <v>40993.145833333336</v>
+        <v>41037.197916666664</v>
       </c>
       <c s="2" r="C19" t="n">
-        <v>40993.947916666664</v>
+        <v>41037.333333333336</v>
       </c>
       <c r="D19" t="n">
-        <v>19.25</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E19" t="n">
-        <v>41031.677083333336</v>
+        <v>41053.833333333336</v>
       </c>
       <c s="2" r="F19" t="n">
-        <v>41031.75</v>
+        <v>41054.708333333336</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c s="1" r="A20" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c s="2" r="B20" t="n">
-        <v>41031.677083333336</v>
+        <v>41051.78125</v>
       </c>
       <c s="2" r="C20" t="n">
-        <v>41031.75</v>
+        <v>41052.125</v>
       </c>
       <c r="D20" t="n">
-        <v>1.75</v>
+        <v>8.25</v>
       </c>
       <c s="2" r="E20" t="n">
-        <v>41037.197916666664</v>
+        <v>41055.0625</v>
       </c>
       <c s="2" r="F20" t="n">
-        <v>41037.333333333336</v>
+        <v>41055.708333333336</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c s="1" r="A21" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c s="2" r="B21" t="n">
-        <v>41037.197916666664</v>
+        <v>41052.322916666664</v>
       </c>
       <c s="2" r="C21" t="n">
-        <v>41037.333333333336</v>
+        <v>41053.583333333336</v>
       </c>
       <c r="D21" t="n">
-        <v>3.25</v>
+        <v>30.25</v>
       </c>
       <c s="2" r="E21" t="n">
-        <v>41051.78125</v>
+        <v>41063.427083333336</v>
       </c>
       <c s="2" r="F21" t="n">
-        <v>41052.125</v>
+        <v>41063.885416666664</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c s="1" r="A22" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c s="2" r="B22" t="n">
-        <v>41051.78125</v>
+        <v>41053.833333333336</v>
       </c>
       <c s="2" r="C22" t="n">
-        <v>41052.125</v>
+        <v>41054.708333333336</v>
       </c>
       <c r="D22" t="n">
-        <v>8.25</v>
+        <v>21.0</v>
       </c>
       <c s="2" r="E22" t="n">
-        <v>41052.322916666664</v>
+        <v>41064.010416666664</v>
       </c>
       <c s="2" r="F22" t="n">
-        <v>41053.583333333336</v>
+        <v>41064.46875</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c s="1" r="A23" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c s="2" r="B23" t="n">
-        <v>41052.322916666664</v>
+        <v>41055.0625</v>
       </c>
       <c s="2" r="C23" t="n">
-        <v>41053.583333333336</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="D23" t="n">
-        <v>30.25</v>
+        <v>15.5</v>
       </c>
       <c s="2" r="E23" t="n">
-        <v>41053.833333333336</v>
+        <v>41064.604166666664</v>
       </c>
       <c s="2" r="F23" t="n">
-        <v>41054.708333333336</v>
+        <v>41065.895833333336</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c s="1" r="A24" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c s="2" r="B24" t="n">
-        <v>41053.833333333336</v>
+        <v>41063.427083333336</v>
       </c>
       <c s="2" r="C24" t="n">
-        <v>41054.708333333336</v>
+        <v>41063.885416666664</v>
       </c>
       <c r="D24" t="n">
-        <v>21.0</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E24" t="n">
-        <v>41055.0625</v>
+        <v>41066.885416666664</v>
       </c>
       <c s="2" r="F24" t="n">
-        <v>41055.708333333336</v>
+        <v>41067.270833333336</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c s="1" r="A25" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c s="2" r="B25" t="n">
-        <v>41055.0625</v>
+        <v>41064.010416666664</v>
       </c>
       <c s="2" r="C25" t="n">
-        <v>41055.708333333336</v>
+        <v>41064.46875</v>
       </c>
       <c r="D25" t="n">
-        <v>15.5</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E25" t="n">
-        <v>41063.427083333336</v>
+        <v>41067.3125</v>
       </c>
       <c s="2" r="F25" t="n">
-        <v>41063.885416666664</v>
+        <v>41067.729166666664</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c s="1" r="A26" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c s="2" r="B26" t="n">
-        <v>41063.427083333336</v>
+        <v>41064.604166666664</v>
       </c>
       <c s="2" r="C26" t="n">
-        <v>41063.885416666664</v>
+        <v>41065.895833333336</v>
       </c>
       <c r="D26" t="n">
-        <v>11.0</v>
+        <v>31.0</v>
       </c>
       <c s="2" r="E26" t="n">
-        <v>41064.010416666664</v>
+        <v>41098.083333333336</v>
       </c>
       <c s="2" r="F26" t="n">
-        <v>41064.46875</v>
+        <v>41098.25</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c s="1" r="A27" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c s="2" r="B27" t="n">
-        <v>41064.010416666664</v>
+        <v>41066.885416666664</v>
       </c>
       <c s="2" r="C27" t="n">
-        <v>41064.46875</v>
+        <v>41067.270833333336</v>
       </c>
       <c r="D27" t="n">
-        <v>11.0</v>
+        <v>9.25</v>
       </c>
       <c s="2" r="E27" t="n">
-        <v>41064.604166666664</v>
+        <v>41117.09375</v>
       </c>
       <c s="2" r="F27" t="n">
-        <v>41065.895833333336</v>
+        <v>41117.1875</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c s="1" r="A28" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c s="2" r="B28" t="n">
-        <v>41064.604166666664</v>
+        <v>41067.3125</v>
       </c>
       <c s="2" r="C28" t="n">
-        <v>41065.895833333336</v>
+        <v>41067.729166666664</v>
       </c>
       <c r="D28" t="n">
-        <v>31.0</v>
+        <v>10.0</v>
       </c>
       <c s="2" r="E28" t="n">
-        <v>41066.885416666664</v>
+        <v>41117.854166666664</v>
       </c>
       <c s="2" r="F28" t="n">
-        <v>41067.270833333336</v>
+        <v>41117.927083333336</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c s="1" r="A29" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c s="2" r="B29" t="n">
-        <v>41066.885416666664</v>
+        <v>41098.083333333336</v>
       </c>
       <c s="2" r="C29" t="n">
-        <v>41067.270833333336</v>
+        <v>41098.25</v>
       </c>
       <c r="D29" t="n">
-        <v>9.25</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E29" t="n">
-        <v>41067.3125</v>
+        <v>41130.145833333336</v>
       </c>
       <c s="2" r="F29" t="n">
-        <v>41067.729166666664</v>
+        <v>41130.395833333336</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c s="1" r="A30" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c s="2" r="B30" t="n">
-        <v>41067.3125</v>
+        <v>41117.09375</v>
       </c>
       <c s="2" r="C30" t="n">
-        <v>41067.729166666664</v>
+        <v>41117.1875</v>
       </c>
       <c r="D30" t="n">
-        <v>10.0</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E30" t="n">
-        <v>41098.083333333336</v>
+        <v>41153.479166666664</v>
       </c>
       <c s="2" r="F30" t="n">
-        <v>41098.25</v>
+        <v>41155.270833333336</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c s="1" r="A31" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c s="2" r="B31" t="n">
-        <v>41098.083333333336</v>
+        <v>41117.854166666664</v>
       </c>
       <c s="2" r="C31" t="n">
-        <v>41098.25</v>
+        <v>41117.927083333336</v>
       </c>
       <c r="D31" t="n">
-        <v>4.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E31" t="n">
-        <v>41117.09375</v>
+        <v>41316.875</v>
       </c>
       <c s="2" r="F31" t="n">
-        <v>41117.1875</v>
+        <v>41317.53125</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c s="1" r="A32" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c s="2" r="B32" t="n">
-        <v>41117.09375</v>
+        <v>41130.145833333336</v>
       </c>
       <c s="2" r="C32" t="n">
-        <v>41117.1875</v>
+        <v>41130.395833333336</v>
       </c>
       <c r="D32" t="n">
-        <v>2.25</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E32" t="n">
-        <v>41117.854166666664</v>
+        <v>41338.78125</v>
       </c>
       <c s="2" r="F32" t="n">
-        <v>41117.927083333336</v>
+        <v>41339.083333333336</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c s="1" r="A33" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c s="2" r="B33" t="n">
-        <v>41117.854166666664</v>
+        <v>41153.479166666664</v>
       </c>
       <c s="2" r="C33" t="n">
-        <v>41117.927083333336</v>
+        <v>41155.270833333336</v>
       </c>
       <c r="D33" t="n">
-        <v>1.75</v>
+        <v>43.0</v>
       </c>
       <c s="2" r="E33" t="n">
-        <v>41130.145833333336</v>
+        <v>41339.385416666664</v>
       </c>
       <c s="2" r="F33" t="n">
-        <v>41130.395833333336</v>
+        <v>41339.916666666664</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c s="1" r="A34" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c s="2" r="B34" t="n">
-        <v>41130.145833333336</v>
+        <v>41316.875</v>
       </c>
       <c s="2" r="C34" t="n">
-        <v>41130.395833333336</v>
+        <v>41317.53125</v>
       </c>
       <c r="D34" t="n">
-        <v>6.0</v>
+        <v>15.75</v>
       </c>
       <c s="2" r="E34" t="n">
-        <v>41153.479166666664</v>
+        <v>41340.604166666664</v>
       </c>
       <c s="2" r="F34" t="n">
-        <v>41155.270833333336</v>
+        <v>41341.84375</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c s="1" r="A35" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c s="2" r="B35" t="n">
-        <v>41153.479166666664</v>
+        <v>41338.78125</v>
       </c>
       <c s="2" r="C35" t="n">
-        <v>41155.270833333336</v>
+        <v>41339.083333333336</v>
       </c>
       <c r="D35" t="n">
-        <v>43.0</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E35" t="n">
-        <v>41316.875</v>
+        <v>41344.09375</v>
       </c>
       <c s="2" r="F35" t="n">
-        <v>41317.53125</v>
+        <v>41344.791666666664</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c s="1" r="A36" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c s="2" r="B36" t="n">
-        <v>41316.875</v>
+        <v>41339.385416666664</v>
       </c>
       <c s="2" r="C36" t="n">
-        <v>41317.53125</v>
+        <v>41339.916666666664</v>
       </c>
       <c r="D36" t="n">
-        <v>15.75</v>
+        <v>12.75</v>
       </c>
       <c s="2" r="E36" t="n">
-        <v>41338.78125</v>
+        <v>41354.552083333336</v>
       </c>
       <c s="2" r="F36" t="n">
-        <v>41339.083333333336</v>
+        <v>41354.645833333336</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c s="1" r="A37" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c s="2" r="B37" t="n">
-        <v>41338.78125</v>
+        <v>41340.604166666664</v>
       </c>
       <c s="2" r="C37" t="n">
-        <v>41339.083333333336</v>
+        <v>41341.84375</v>
       </c>
       <c r="D37" t="n">
-        <v>7.25</v>
+        <v>29.75</v>
       </c>
       <c s="2" r="E37" t="n">
-        <v>41339.385416666664</v>
+        <v>41356.458333333336</v>
       </c>
       <c s="2" r="F37" t="n">
-        <v>41339.916666666664</v>
+        <v>41356.53125</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c s="1" r="A38" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c s="2" r="B38" t="n">
-        <v>41339.385416666664</v>
+        <v>41344.09375</v>
       </c>
       <c s="2" r="C38" t="n">
-        <v>41339.916666666664</v>
+        <v>41344.791666666664</v>
       </c>
       <c r="D38" t="n">
-        <v>12.75</v>
+        <v>16.75</v>
       </c>
       <c s="2" r="E38" t="n">
-        <v>41340.604166666664</v>
+        <v>41380.458333333336</v>
       </c>
       <c s="2" r="F38" t="n">
-        <v>41341.84375</v>
+        <v>41380.90625</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c s="1" r="A39" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c s="2" r="B39" t="n">
-        <v>41340.604166666664</v>
+        <v>41354.552083333336</v>
       </c>
       <c s="2" r="C39" t="n">
-        <v>41341.84375</v>
+        <v>41354.645833333336</v>
       </c>
       <c r="D39" t="n">
-        <v>29.75</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E39" t="n">
-        <v>41344.09375</v>
+        <v>41381.0</v>
       </c>
       <c s="2" r="F39" t="n">
-        <v>41344.791666666664</v>
+        <v>41381.697916666664</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c s="1" r="A40" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c s="2" r="B40" t="n">
-        <v>41344.09375</v>
+        <v>41356.458333333336</v>
       </c>
       <c s="2" r="C40" t="n">
-        <v>41344.791666666664</v>
+        <v>41356.53125</v>
       </c>
       <c r="D40" t="n">
-        <v>16.75</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E40" t="n">
-        <v>41354.552083333336</v>
+        <v>41384.1875</v>
       </c>
       <c s="2" r="F40" t="n">
-        <v>41354.645833333336</v>
+        <v>41384.604166666664</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c s="1" r="A41" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c s="2" r="B41" t="n">
-        <v>41354.552083333336</v>
+        <v>41380.458333333336</v>
       </c>
       <c s="2" r="C41" t="n">
-        <v>41354.645833333336</v>
+        <v>41380.90625</v>
       </c>
       <c r="D41" t="n">
-        <v>2.25</v>
+        <v>10.75</v>
       </c>
       <c s="2" r="E41" t="n">
-        <v>41356.458333333336</v>
+        <v>41387.5625</v>
       </c>
       <c s="2" r="F41" t="n">
-        <v>41356.53125</v>
+        <v>41388.3125</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c s="1" r="A42" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c s="2" r="B42" t="n">
-        <v>41356.458333333336</v>
+        <v>41381.0</v>
       </c>
       <c s="2" r="C42" t="n">
-        <v>41356.53125</v>
+        <v>41381.697916666664</v>
       </c>
       <c r="D42" t="n">
-        <v>1.75</v>
+        <v>16.75</v>
       </c>
       <c s="2" r="E42" t="n">
-        <v>41380.458333333336</v>
+        <v>41392.427083333336</v>
       </c>
       <c s="2" r="F42" t="n">
-        <v>41380.90625</v>
+        <v>41392.625</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c s="1" r="A43" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c s="2" r="B43" t="n">
-        <v>41380.458333333336</v>
+        <v>41384.1875</v>
       </c>
       <c s="2" r="C43" t="n">
-        <v>41380.90625</v>
+        <v>41384.604166666664</v>
       </c>
       <c r="D43" t="n">
-        <v>10.75</v>
+        <v>10.0</v>
       </c>
       <c s="2" r="E43" t="n">
-        <v>41381.0</v>
+        <v>41392.84375</v>
       </c>
       <c s="2" r="F43" t="n">
-        <v>41381.697916666664</v>
+        <v>41393.166666666664</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c s="1" r="A44" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c s="2" r="B44" t="n">
-        <v>41381.0</v>
+        <v>41387.5625</v>
       </c>
       <c s="2" r="C44" t="n">
-        <v>41381.697916666664</v>
+        <v>41388.3125</v>
       </c>
       <c r="D44" t="n">
-        <v>16.75</v>
+        <v>18.0</v>
       </c>
       <c s="2" r="E44" t="n">
-        <v>41384.1875</v>
+        <v>41394.625</v>
       </c>
       <c s="2" r="F44" t="n">
-        <v>41384.604166666664</v>
+        <v>41395.65625</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c s="1" r="A45" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c s="2" r="B45" t="n">
-        <v>41384.1875</v>
+        <v>41392.427083333336</v>
       </c>
       <c s="2" r="C45" t="n">
-        <v>41384.604166666664</v>
+        <v>41392.625</v>
       </c>
       <c r="D45" t="n">
-        <v>10.0</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E45" t="n">
-        <v>41387.5625</v>
+        <v>41405.604166666664</v>
       </c>
       <c s="2" r="F45" t="n">
-        <v>41388.3125</v>
+        <v>41405.677083333336</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c s="1" r="A46" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c s="2" r="B46" t="n">
-        <v>41387.5625</v>
+        <v>41392.84375</v>
       </c>
       <c s="2" r="C46" t="n">
-        <v>41388.3125</v>
+        <v>41393.166666666664</v>
       </c>
       <c r="D46" t="n">
-        <v>18.0</v>
+        <v>7.75</v>
       </c>
       <c s="2" r="E46" t="n">
-        <v>41392.427083333336</v>
+        <v>41430.239583333336</v>
       </c>
       <c s="2" r="F46" t="n">
-        <v>41392.625</v>
+        <v>41431.208333333336</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c s="1" r="A47" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c s="2" r="B47" t="n">
-        <v>41392.427083333336</v>
+        <v>41394.625</v>
       </c>
       <c s="2" r="C47" t="n">
-        <v>41392.625</v>
+        <v>41395.65625</v>
       </c>
       <c r="D47" t="n">
-        <v>4.75</v>
+        <v>24.75</v>
       </c>
       <c s="2" r="E47" t="n">
-        <v>41392.84375</v>
+        <v>41441.135416666664</v>
       </c>
       <c s="2" r="F47" t="n">
-        <v>41393.166666666664</v>
+        <v>41441.40625</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c s="1" r="A48" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c s="2" r="B48" t="n">
-        <v>41392.84375</v>
+        <v>41405.604166666664</v>
       </c>
       <c s="2" r="C48" t="n">
-        <v>41393.166666666664</v>
+        <v>41405.677083333336</v>
       </c>
       <c r="D48" t="n">
-        <v>7.75</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E48" t="n">
-        <v>41394.625</v>
+        <v>41472.145833333336</v>
       </c>
       <c s="2" r="F48" t="n">
-        <v>41395.65625</v>
+        <v>41472.229166666664</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c s="1" r="A49" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c s="2" r="B49" t="n">
-        <v>41394.625</v>
+        <v>41430.239583333336</v>
       </c>
       <c s="2" r="C49" t="n">
-        <v>41395.65625</v>
+        <v>41431.208333333336</v>
       </c>
       <c r="D49" t="n">
-        <v>24.75</v>
+        <v>23.25</v>
       </c>
       <c s="2" r="E49" t="n">
-        <v>41405.604166666664</v>
+        <v>41472.958333333336</v>
       </c>
       <c s="2" r="F49" t="n">
-        <v>41405.677083333336</v>
+        <v>41473.46875</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c s="1" r="A50" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c s="2" r="B50" t="n">
-        <v>41405.604166666664</v>
+        <v>41441.135416666664</v>
       </c>
       <c s="2" r="C50" t="n">
-        <v>41405.677083333336</v>
+        <v>41441.40625</v>
       </c>
       <c r="D50" t="n">
-        <v>1.75</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E50" t="n">
-        <v>41430.239583333336</v>
+        <v>41474.364583333336</v>
       </c>
       <c s="2" r="F50" t="n">
-        <v>41431.208333333336</v>
+        <v>41474.625</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c s="1" r="A51" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c s="2" r="B51" t="n">
-        <v>41430.239583333336</v>
+        <v>41472.145833333336</v>
       </c>
       <c s="2" r="C51" t="n">
-        <v>41431.208333333336</v>
+        <v>41472.229166666664</v>
       </c>
       <c r="D51" t="n">
-        <v>23.25</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E51" t="n">
-        <v>41441.135416666664</v>
+        <v>41474.625</v>
       </c>
       <c s="2" r="F51" t="n">
-        <v>41441.40625</v>
+        <v>41475.666666666664</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c s="1" r="A52" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c s="2" r="B52" t="n">
-        <v>41441.135416666664</v>
+        <v>41472.958333333336</v>
       </c>
       <c s="2" r="C52" t="n">
-        <v>41441.40625</v>
+        <v>41473.46875</v>
       </c>
       <c r="D52" t="n">
-        <v>6.5</v>
+        <v>12.25</v>
       </c>
       <c s="2" r="E52" t="n">
-        <v>41472.145833333336</v>
+        <v>41496.1875</v>
       </c>
       <c s="2" r="F52" t="n">
-        <v>41472.229166666664</v>
+        <v>41497.052083333336</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c s="1" r="A53" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c s="2" r="B53" t="n">
-        <v>41472.145833333336</v>
+        <v>41474.364583333336</v>
       </c>
       <c s="2" r="C53" t="n">
-        <v>41472.229166666664</v>
+        <v>41475.666666666664</v>
       </c>
       <c r="D53" t="n">
-        <v>2.0</v>
+        <v>6.25</v>
       </c>
       <c s="2" r="E53" t="n">
-        <v>41472.958333333336</v>
+        <v>41501.791666666664</v>
       </c>
       <c s="2" r="F53" t="n">
-        <v>41473.46875</v>
+        <v>41501.947916666664</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c s="1" r="A54" t="n">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c s="2" r="B54" t="n">
-        <v>41472.958333333336</v>
+        <v>41491.989583333336</v>
       </c>
       <c s="2" r="C54" t="n">
-        <v>41473.46875</v>
+        <v>41492.229166666664</v>
       </c>
       <c r="D54" t="n">
-        <v>12.25</v>
+        <v>5.75</v>
       </c>
       <c s="2" r="E54" t="n">
-        <v>41474.364583333336</v>
+        <v>41502.333333333336</v>
       </c>
       <c s="2" r="F54" t="n">
-        <v>41474.625</v>
+        <v>41504.677083333336</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c s="1" r="A55" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c s="2" r="B55" t="n">
-        <v>41474.364583333336</v>
+        <v>41496.1875</v>
       </c>
       <c s="2" r="C55" t="n">
-        <v>41475.666666666664</v>
+        <v>41497.052083333336</v>
       </c>
       <c r="D55" t="n">
-        <v>6.25</v>
+        <v>20.75</v>
       </c>
       <c s="2" r="E55" t="n">
-        <v>41474.625</v>
+        <v>41505.28125</v>
       </c>
       <c s="2" r="F55" t="n">
-        <v>41475.666666666664</v>
+        <v>41505.979166666664</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c s="1" r="A56" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c s="2" r="B56" t="n">
-        <v>41491.989583333336</v>
+        <v>41501.791666666664</v>
       </c>
       <c s="2" r="C56" t="n">
-        <v>41492.229166666664</v>
+        <v>41501.947916666664</v>
       </c>
       <c r="D56" t="n">
-        <v>5.75</v>
+        <v>3.75</v>
       </c>
       <c s="2" r="E56" t="n">
-        <v>41496.1875</v>
+        <v>41518.197916666664</v>
       </c>
       <c s="2" r="F56" t="n">
-        <v>41497.052083333336</v>
+        <v>41518.28125</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c s="1" r="A57" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c s="2" r="B57" t="n">
-        <v>41496.1875</v>
+        <v>41502.333333333336</v>
       </c>
       <c s="2" r="C57" t="n">
-        <v>41497.052083333336</v>
+        <v>41504.677083333336</v>
       </c>
       <c r="D57" t="n">
-        <v>20.75</v>
+        <v>56.25</v>
       </c>
       <c s="2" r="E57" t="n">
-        <v>41501.791666666664</v>
+        <v>41518.354166666664</v>
       </c>
       <c s="2" r="F57" t="n">
-        <v>41501.947916666664</v>
+        <v>41518.635416666664</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c s="1" r="A58" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c s="2" r="B58" t="n">
-        <v>41501.791666666664</v>
+        <v>41505.28125</v>
       </c>
       <c s="2" r="C58" t="n">
-        <v>41501.947916666664</v>
+        <v>41505.979166666664</v>
       </c>
       <c r="D58" t="n">
-        <v>3.75</v>
+        <v>16.75</v>
       </c>
       <c s="2" r="E58" t="n">
-        <v>41502.333333333336</v>
+        <v>41684.614583333336</v>
       </c>
       <c s="2" r="F58" t="n">
-        <v>41504.677083333336</v>
+        <v>41684.84375</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c s="1" r="A59" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c s="2" r="B59" t="n">
-        <v>41502.333333333336</v>
+        <v>41518.197916666664</v>
       </c>
       <c s="2" r="C59" t="n">
-        <v>41504.677083333336</v>
+        <v>41518.28125</v>
       </c>
       <c r="D59" t="n">
-        <v>56.25</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E59" t="n">
-        <v>41505.28125</v>
+        <v>41685.375</v>
       </c>
       <c s="2" r="F59" t="n">
-        <v>41505.979166666664</v>
+        <v>41685.479166666664</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c s="1" r="A60" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c s="2" r="B60" t="n">
-        <v>41505.28125</v>
+        <v>41518.354166666664</v>
       </c>
       <c s="2" r="C60" t="n">
-        <v>41505.979166666664</v>
+        <v>41518.635416666664</v>
       </c>
       <c r="D60" t="n">
-        <v>16.75</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E60" t="n">
-        <v>41518.197916666664</v>
+        <v>41688.760416666664</v>
       </c>
       <c s="2" r="F60" t="n">
-        <v>41518.28125</v>
+        <v>41688.833333333336</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c s="1" r="A61" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c s="2" r="B61" t="n">
-        <v>41518.197916666664</v>
+        <v>41684.614583333336</v>
       </c>
       <c s="2" r="C61" t="n">
-        <v>41518.28125</v>
+        <v>41684.84375</v>
       </c>
       <c r="D61" t="n">
-        <v>2.0</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E61" t="n">
-        <v>41518.354166666664</v>
+        <v>41690.46875</v>
       </c>
       <c s="2" r="F61" t="n">
-        <v>41518.635416666664</v>
+        <v>41690.791666666664</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c s="1" r="A62" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c s="2" r="B62" t="n">
-        <v>41518.354166666664</v>
+        <v>41685.375</v>
       </c>
       <c s="2" r="C62" t="n">
-        <v>41518.635416666664</v>
+        <v>41685.479166666664</v>
       </c>
       <c r="D62" t="n">
-        <v>6.75</v>
+        <v>2.5</v>
       </c>
       <c s="2" r="E62" t="n">
-        <v>41684.614583333336</v>
+        <v>41691.479166666664</v>
       </c>
       <c s="2" r="F62" t="n">
-        <v>41684.84375</v>
+        <v>41692.239583333336</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c s="1" r="A63" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c s="2" r="B63" t="n">
-        <v>41684.614583333336</v>
+        <v>41688.760416666664</v>
       </c>
       <c s="2" r="C63" t="n">
-        <v>41684.84375</v>
+        <v>41688.833333333336</v>
       </c>
       <c r="D63" t="n">
-        <v>5.5</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E63" t="n">
-        <v>41685.375</v>
+        <v>41692.322916666664</v>
       </c>
       <c s="2" r="F63" t="n">
-        <v>41685.479166666664</v>
+        <v>41692.40625</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c s="1" r="A64" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c s="2" r="B64" t="n">
-        <v>41685.375</v>
+        <v>41690.46875</v>
       </c>
       <c s="2" r="C64" t="n">
-        <v>41685.479166666664</v>
+        <v>41690.791666666664</v>
       </c>
       <c r="D64" t="n">
-        <v>2.5</v>
+        <v>7.75</v>
       </c>
       <c s="2" r="E64" t="n">
-        <v>41688.760416666664</v>
+        <v>41694.229166666664</v>
       </c>
       <c s="2" r="F64" t="n">
-        <v>41688.833333333336</v>
+        <v>41694.302083333336</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c s="1" r="A65" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c s="2" r="B65" t="n">
-        <v>41688.760416666664</v>
+        <v>41691.479166666664</v>
       </c>
       <c s="2" r="C65" t="n">
-        <v>41688.833333333336</v>
+        <v>41692.239583333336</v>
       </c>
       <c r="D65" t="n">
-        <v>1.75</v>
+        <v>18.25</v>
       </c>
       <c s="2" r="E65" t="n">
-        <v>41690.46875</v>
+        <v>41695.885416666664</v>
       </c>
       <c s="2" r="F65" t="n">
-        <v>41690.791666666664</v>
+        <v>41696.8125</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c s="1" r="A66" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c s="2" r="B66" t="n">
-        <v>41690.46875</v>
+        <v>41692.322916666664</v>
       </c>
       <c s="2" r="C66" t="n">
-        <v>41690.791666666664</v>
+        <v>41692.40625</v>
       </c>
       <c r="D66" t="n">
-        <v>7.75</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E66" t="n">
-        <v>41691.479166666664</v>
+        <v>41697.083333333336</v>
       </c>
       <c s="2" r="F66" t="n">
-        <v>41692.239583333336</v>
+        <v>41698.09375</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c s="1" r="A67" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c s="2" r="B67" t="n">
-        <v>41691.479166666664</v>
+        <v>41694.229166666664</v>
       </c>
       <c s="2" r="C67" t="n">
-        <v>41692.239583333336</v>
+        <v>41694.302083333336</v>
       </c>
       <c r="D67" t="n">
-        <v>18.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E67" t="n">
-        <v>41692.322916666664</v>
+        <v>41704.802083333336</v>
       </c>
       <c s="2" r="F67" t="n">
-        <v>41692.40625</v>
+        <v>41705.239583333336</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c s="1" r="A68" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c s="2" r="B68" t="n">
-        <v>41692.322916666664</v>
+        <v>41695.885416666664</v>
       </c>
       <c s="2" r="C68" t="n">
-        <v>41692.40625</v>
+        <v>41696.8125</v>
       </c>
       <c r="D68" t="n">
-        <v>2.0</v>
+        <v>22.25</v>
       </c>
       <c s="2" r="E68" t="n">
-        <v>41694.229166666664</v>
+        <v>41711.520833333336</v>
       </c>
       <c s="2" r="F68" t="n">
-        <v>41694.302083333336</v>
+        <v>41711.65625</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c s="1" r="A69" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c s="2" r="B69" t="n">
-        <v>41694.229166666664</v>
+        <v>41697.083333333336</v>
       </c>
       <c s="2" r="C69" t="n">
-        <v>41694.302083333336</v>
+        <v>41698.09375</v>
       </c>
       <c r="D69" t="n">
-        <v>1.75</v>
+        <v>24.25</v>
       </c>
       <c s="2" r="E69" t="n">
-        <v>41695.885416666664</v>
+        <v>41711.666666666664</v>
       </c>
       <c s="2" r="F69" t="n">
-        <v>41696.8125</v>
+        <v>41712.0</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c s="1" r="A70" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c s="2" r="B70" t="n">
-        <v>41695.885416666664</v>
+        <v>41704.802083333336</v>
       </c>
       <c s="2" r="C70" t="n">
-        <v>41696.8125</v>
+        <v>41705.239583333336</v>
       </c>
       <c r="D70" t="n">
-        <v>22.25</v>
+        <v>10.5</v>
       </c>
       <c s="2" r="E70" t="n">
-        <v>41697.083333333336</v>
+        <v>41712.020833333336</v>
       </c>
       <c s="2" r="F70" t="n">
-        <v>41698.09375</v>
+        <v>41712.40625</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c s="1" r="A71" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c s="2" r="B71" t="n">
-        <v>41697.083333333336</v>
+        <v>41711.520833333336</v>
       </c>
       <c s="2" r="C71" t="n">
-        <v>41698.09375</v>
+        <v>41711.65625</v>
       </c>
       <c r="D71" t="n">
-        <v>24.25</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E71" t="n">
-        <v>41704.802083333336</v>
+        <v>41712.75</v>
       </c>
       <c s="2" r="F71" t="n">
-        <v>41705.239583333336</v>
+        <v>41712.822916666664</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c s="1" r="A72" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c s="2" r="B72" t="n">
-        <v>41704.802083333336</v>
+        <v>41711.666666666664</v>
       </c>
       <c s="2" r="C72" t="n">
-        <v>41705.239583333336</v>
+        <v>41712.0</v>
       </c>
       <c r="D72" t="n">
-        <v>10.5</v>
+        <v>8.0</v>
       </c>
       <c s="2" r="E72" t="n">
-        <v>41711.520833333336</v>
+        <v>41730.364583333336</v>
       </c>
       <c s="2" r="F72" t="n">
-        <v>41711.65625</v>
+        <v>41730.4375</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c s="1" r="A73" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c s="2" r="B73" t="n">
-        <v>41711.520833333336</v>
+        <v>41712.020833333336</v>
       </c>
       <c s="2" r="C73" t="n">
-        <v>41711.65625</v>
+        <v>41712.40625</v>
       </c>
       <c r="D73" t="n">
-        <v>3.25</v>
+        <v>9.25</v>
       </c>
       <c s="2" r="E73" t="n">
-        <v>41711.666666666664</v>
+        <v>41735.520833333336</v>
       </c>
       <c s="2" r="F73" t="n">
-        <v>41712.0</v>
+        <v>41736.197916666664</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c s="1" r="A74" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c s="2" r="B74" t="n">
-        <v>41711.666666666664</v>
+        <v>41712.75</v>
       </c>
       <c s="2" r="C74" t="n">
-        <v>41712.0</v>
+        <v>41712.822916666664</v>
       </c>
       <c r="D74" t="n">
-        <v>8.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E74" t="n">
-        <v>41712.020833333336</v>
+        <v>41737.604166666664</v>
       </c>
       <c s="2" r="F74" t="n">
-        <v>41712.40625</v>
+        <v>41737.791666666664</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c s="1" r="A75" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c s="2" r="B75" t="n">
-        <v>41712.020833333336</v>
+        <v>41730.364583333336</v>
       </c>
       <c s="2" r="C75" t="n">
-        <v>41712.40625</v>
+        <v>41730.4375</v>
       </c>
       <c r="D75" t="n">
-        <v>9.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E75" t="n">
-        <v>41712.75</v>
+        <v>41738.979166666664</v>
       </c>
       <c s="2" r="F75" t="n">
-        <v>41712.822916666664</v>
+        <v>41739.197916666664</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c s="1" r="A76" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c s="2" r="B76" t="n">
-        <v>41712.75</v>
+        <v>41735.520833333336</v>
       </c>
       <c s="2" r="C76" t="n">
-        <v>41712.822916666664</v>
+        <v>41736.197916666664</v>
       </c>
       <c r="D76" t="n">
-        <v>1.75</v>
+        <v>16.25</v>
       </c>
       <c s="2" r="E76" t="n">
-        <v>41730.364583333336</v>
+        <v>41740.40625</v>
       </c>
       <c s="2" r="F76" t="n">
-        <v>41730.4375</v>
+        <v>41740.5</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c s="1" r="A77" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c s="2" r="B77" t="n">
-        <v>41730.364583333336</v>
+        <v>41737.604166666664</v>
       </c>
       <c s="2" r="C77" t="n">
-        <v>41730.4375</v>
+        <v>41737.791666666664</v>
       </c>
       <c r="D77" t="n">
-        <v>1.75</v>
+        <v>4.5</v>
       </c>
       <c s="2" r="E77" t="n">
-        <v>41735.520833333336</v>
+        <v>41746.625</v>
       </c>
       <c s="2" r="F77" t="n">
-        <v>41736.197916666664</v>
+        <v>41746.697916666664</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c s="1" r="A78" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c s="2" r="B78" t="n">
-        <v>41735.520833333336</v>
+        <v>41738.979166666664</v>
       </c>
       <c s="2" r="C78" t="n">
-        <v>41736.197916666664</v>
+        <v>41739.197916666664</v>
       </c>
       <c r="D78" t="n">
-        <v>16.25</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E78" t="n">
-        <v>41737.604166666664</v>
+        <v>41747.78125</v>
       </c>
       <c s="2" r="F78" t="n">
-        <v>41737.791666666664</v>
+        <v>41748.010416666664</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c s="1" r="A79" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c s="2" r="B79" t="n">
-        <v>41737.604166666664</v>
+        <v>41740.40625</v>
       </c>
       <c s="2" r="C79" t="n">
-        <v>41737.791666666664</v>
+        <v>41740.5</v>
       </c>
       <c r="D79" t="n">
-        <v>4.5</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E79" t="n">
-        <v>41738.979166666664</v>
+        <v>41748.28125</v>
       </c>
       <c s="2" r="F79" t="n">
-        <v>41739.197916666664</v>
+        <v>41749.489583333336</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c s="1" r="A80" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c s="2" r="B80" t="n">
-        <v>41738.979166666664</v>
+        <v>41746.625</v>
       </c>
       <c s="2" r="C80" t="n">
-        <v>41739.197916666664</v>
+        <v>41746.697916666664</v>
       </c>
       <c r="D80" t="n">
-        <v>5.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E80" t="n">
-        <v>41740.40625</v>
+        <v>41754.645833333336</v>
       </c>
       <c s="2" r="F80" t="n">
-        <v>41740.5</v>
+        <v>41755.020833333336</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c s="1" r="A81" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c s="2" r="B81" t="n">
-        <v>41740.40625</v>
+        <v>41747.78125</v>
       </c>
       <c s="2" r="C81" t="n">
-        <v>41740.5</v>
+        <v>41748.010416666664</v>
       </c>
       <c r="D81" t="n">
-        <v>2.25</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E81" t="n">
-        <v>41746.625</v>
+        <v>41755.458333333336</v>
       </c>
       <c s="2" r="F81" t="n">
-        <v>41746.697916666664</v>
+        <v>41755.53125</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c s="1" r="A82" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c s="2" r="B82" t="n">
-        <v>41746.625</v>
+        <v>41748.28125</v>
       </c>
       <c s="2" r="C82" t="n">
-        <v>41746.697916666664</v>
+        <v>41749.489583333336</v>
       </c>
       <c r="D82" t="n">
-        <v>1.75</v>
+        <v>29.0</v>
       </c>
       <c s="2" r="E82" t="n">
-        <v>41747.78125</v>
+        <v>41756.479166666664</v>
       </c>
       <c s="2" r="F82" t="n">
-        <v>41748.010416666664</v>
+        <v>41756.90625</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c s="1" r="A83" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c s="2" r="B83" t="n">
-        <v>41747.78125</v>
+        <v>41754.645833333336</v>
       </c>
       <c s="2" r="C83" t="n">
-        <v>41748.010416666664</v>
+        <v>41755.020833333336</v>
       </c>
       <c r="D83" t="n">
-        <v>5.5</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E83" t="n">
-        <v>41748.28125</v>
+        <v>41757.385416666664</v>
       </c>
       <c s="2" r="F83" t="n">
-        <v>41749.489583333336</v>
+        <v>41757.583333333336</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c s="1" r="A84" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c s="2" r="B84" t="n">
-        <v>41748.28125</v>
+        <v>41755.458333333336</v>
       </c>
       <c s="2" r="C84" t="n">
-        <v>41749.489583333336</v>
+        <v>41755.53125</v>
       </c>
       <c r="D84" t="n">
-        <v>29.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E84" t="n">
-        <v>41754.645833333336</v>
+        <v>41757.885416666664</v>
       </c>
       <c s="2" r="F84" t="n">
-        <v>41755.020833333336</v>
+        <v>41758.708333333336</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c s="1" r="A85" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c s="2" r="B85" t="n">
-        <v>41754.645833333336</v>
+        <v>41756.479166666664</v>
       </c>
       <c s="2" r="C85" t="n">
-        <v>41755.020833333336</v>
+        <v>41756.90625</v>
       </c>
       <c r="D85" t="n">
-        <v>9.0</v>
+        <v>10.25</v>
       </c>
       <c s="2" r="E85" t="n">
-        <v>41755.458333333336</v>
+        <v>41758.708333333336</v>
       </c>
       <c s="2" r="F85" t="n">
-        <v>41755.53125</v>
+        <v>41758.802083333336</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c s="1" r="A86" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="2" r="B86" t="n">
-        <v>41755.458333333336</v>
+        <v>41757.385416666664</v>
       </c>
       <c s="2" r="C86" t="n">
-        <v>41755.53125</v>
+        <v>41757.583333333336</v>
       </c>
       <c r="D86" t="n">
-        <v>1.75</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E86" t="n">
-        <v>41756.479166666664</v>
+        <v>41758.802083333336</v>
       </c>
       <c s="2" r="F86" t="n">
-        <v>41756.90625</v>
+        <v>41758.9375</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c s="1" r="A87" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c s="2" r="B87" t="n">
-        <v>41756.479166666664</v>
+        <v>41757.885416666664</v>
       </c>
       <c s="2" r="C87" t="n">
-        <v>41756.90625</v>
+        <v>41758.9375</v>
       </c>
       <c r="D87" t="n">
-        <v>10.25</v>
+        <v>19.75</v>
       </c>
       <c s="2" r="E87" t="n">
-        <v>41757.385416666664</v>
+        <v>41779.041666666664</v>
       </c>
       <c s="2" r="F87" t="n">
-        <v>41757.583333333336</v>
+        <v>41779.208333333336</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c s="1" r="A88" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c s="2" r="B88" t="n">
-        <v>41757.385416666664</v>
+        <v>41759.489583333336</v>
       </c>
       <c s="2" r="C88" t="n">
-        <v>41757.583333333336</v>
+        <v>41760.333333333336</v>
       </c>
       <c r="D88" t="n">
-        <v>4.75</v>
+        <v>20.25</v>
       </c>
       <c s="2" r="E88" t="n">
-        <v>41757.885416666664</v>
+        <v>41781.5625</v>
       </c>
       <c s="2" r="F88" t="n">
-        <v>41758.708333333336</v>
+        <v>41782.177083333336</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c s="1" r="A89" t="n">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c s="2" r="B89" t="n">
-        <v>41757.885416666664</v>
+        <v>41778.5625</v>
       </c>
       <c s="2" r="C89" t="n">
-        <v>41758.802083333336</v>
+        <v>41778.697916666664</v>
       </c>
       <c r="D89" t="n">
-        <v>19.75</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E89" t="n">
-        <v>41758.708333333336</v>
+        <v>41782.333333333336</v>
       </c>
       <c s="2" r="F89" t="n">
-        <v>41758.802083333336</v>
+        <v>41782.53125</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c s="1" r="A90" t="n">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c s="2" r="B90" t="n">
-        <v>41758.708333333336</v>
+        <v>41779.041666666664</v>
       </c>
       <c s="2" r="C90" t="n">
-        <v>41758.9375</v>
+        <v>41779.208333333336</v>
       </c>
       <c r="D90" t="n">
-        <v>2.25</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E90" t="n">
-        <v>41758.802083333336</v>
+        <v>41782.979166666664</v>
       </c>
       <c s="2" r="F90" t="n">
-        <v>41758.9375</v>
+        <v>41783.25</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c s="1" r="A91" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c s="2" r="B91" t="n">
-        <v>41759.489583333336</v>
+        <v>41781.5625</v>
       </c>
       <c s="2" r="C91" t="n">
-        <v>41760.333333333336</v>
+        <v>41782.177083333336</v>
       </c>
       <c r="D91" t="n">
-        <v>20.25</v>
+        <v>14.75</v>
       </c>
       <c s="2" r="E91" t="n">
-        <v>41778.5625</v>
+        <v>41783.375</v>
       </c>
       <c s="2" r="F91" t="n">
-        <v>41778.697916666664</v>
+        <v>41783.447916666664</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c s="1" r="A92" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c s="2" r="B92" t="n">
-        <v>41778.5625</v>
+        <v>41782.333333333336</v>
       </c>
       <c s="2" r="C92" t="n">
-        <v>41778.697916666664</v>
+        <v>41782.53125</v>
       </c>
       <c r="D92" t="n">
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E92" t="n">
-        <v>41779.041666666664</v>
+        <v>41788.59375</v>
       </c>
       <c s="2" r="F92" t="n">
-        <v>41779.208333333336</v>
+        <v>41788.729166666664</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c s="1" r="A93" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c s="2" r="B93" t="n">
-        <v>41779.041666666664</v>
+        <v>41782.979166666664</v>
       </c>
       <c s="2" r="C93" t="n">
-        <v>41779.208333333336</v>
+        <v>41783.25</v>
       </c>
       <c r="D93" t="n">
-        <v>4.0</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E93" t="n">
-        <v>41781.5625</v>
+        <v>41795.791666666664</v>
       </c>
       <c s="2" r="F93" t="n">
-        <v>41782.177083333336</v>
+        <v>41796.645833333336</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c s="1" r="A94" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c s="2" r="B94" t="n">
-        <v>41781.5625</v>
+        <v>41783.375</v>
       </c>
       <c s="2" r="C94" t="n">
-        <v>41782.177083333336</v>
+        <v>41783.447916666664</v>
       </c>
       <c r="D94" t="n">
-        <v>14.75</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E94" t="n">
-        <v>41782.333333333336</v>
+        <v>41807.041666666664</v>
       </c>
       <c s="2" r="F94" t="n">
-        <v>41782.53125</v>
+        <v>41807.40625</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c s="1" r="A95" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c s="2" r="B95" t="n">
-        <v>41782.333333333336</v>
+        <v>41788.59375</v>
       </c>
       <c s="2" r="C95" t="n">
-        <v>41782.53125</v>
+        <v>41788.729166666664</v>
       </c>
       <c r="D95" t="n">
-        <v>4.75</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E95" t="n">
-        <v>41782.979166666664</v>
+        <v>41823.4375</v>
       </c>
       <c s="2" r="F95" t="n">
-        <v>41783.25</v>
+        <v>41823.833333333336</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c s="1" r="A96" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c s="2" r="B96" t="n">
-        <v>41782.979166666664</v>
+        <v>41795.791666666664</v>
       </c>
       <c s="2" r="C96" t="n">
-        <v>41783.25</v>
+        <v>41796.645833333336</v>
       </c>
       <c r="D96" t="n">
-        <v>6.5</v>
+        <v>20.5</v>
       </c>
       <c s="2" r="E96" t="n">
-        <v>41783.375</v>
+        <v>41825.25</v>
       </c>
       <c s="2" r="F96" t="n">
-        <v>41783.447916666664</v>
+        <v>41825.760416666664</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c s="1" r="A97" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c s="2" r="B97" t="n">
-        <v>41783.375</v>
+        <v>41807.041666666664</v>
       </c>
       <c s="2" r="C97" t="n">
-        <v>41783.447916666664</v>
+        <v>41807.40625</v>
       </c>
       <c r="D97" t="n">
-        <v>1.75</v>
+        <v>8.75</v>
       </c>
       <c s="2" r="E97" t="n">
-        <v>41788.59375</v>
+        <v>41826.84375</v>
       </c>
       <c s="2" r="F97" t="n">
-        <v>41788.729166666664</v>
+        <v>41827.0</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c s="1" r="A98" t="n">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c s="2" r="B98" t="n">
-        <v>41788.59375</v>
+        <v>41823.4375</v>
       </c>
       <c s="2" r="C98" t="n">
-        <v>41788.729166666664</v>
+        <v>41823.833333333336</v>
       </c>
       <c r="D98" t="n">
-        <v>3.25</v>
+        <v>9.5</v>
       </c>
       <c s="2" r="E98" t="n">
-        <v>41795.791666666664</v>
+        <v>41849.25</v>
       </c>
       <c s="2" r="F98" t="n">
-        <v>41796.645833333336</v>
+        <v>41853.364583333336</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c s="1" r="A99" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c s="2" r="B99" t="n">
-        <v>41795.791666666664</v>
+        <v>41825.25</v>
       </c>
       <c s="2" r="C99" t="n">
-        <v>41796.645833333336</v>
+        <v>41825.760416666664</v>
       </c>
       <c r="D99" t="n">
-        <v>20.5</v>
+        <v>12.25</v>
       </c>
       <c s="2" r="E99" t="n">
-        <v>41807.041666666664</v>
+        <v>41853.364583333336</v>
       </c>
       <c s="2" r="F99" t="n">
-        <v>41807.40625</v>
+        <v>41854.6875</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c s="1" r="A100" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c s="2" r="B100" t="n">
-        <v>41807.041666666664</v>
+        <v>41826.84375</v>
       </c>
       <c s="2" r="C100" t="n">
-        <v>41807.40625</v>
+        <v>41827.0</v>
       </c>
       <c r="D100" t="n">
-        <v>8.75</v>
+        <v>3.75</v>
       </c>
       <c s="2" r="E100" t="n">
-        <v>41823.4375</v>
+        <v>41927.739583333336</v>
       </c>
       <c s="2" r="F100" t="n">
-        <v>41823.833333333336</v>
+        <v>41928.083333333336</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c s="1" r="A101" t="n">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c s="2" r="B101" t="n">
-        <v>41823.4375</v>
+        <v>41849.25</v>
       </c>
       <c s="2" r="C101" t="n">
-        <v>41823.833333333336</v>
+        <v>41854.6875</v>
       </c>
       <c r="D101" t="n">
-        <v>9.5</v>
+        <v>98.75</v>
       </c>
       <c s="2" r="E101" t="n">
-        <v>41825.25</v>
+        <v>41945.145833333336</v>
       </c>
       <c s="2" r="F101" t="n">
-        <v>41825.760416666664</v>
+        <v>41945.364583333336</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c s="1" r="A102" t="n">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c s="2" r="B102" t="n">
-        <v>41825.25</v>
+        <v>41927.53125</v>
       </c>
       <c s="2" r="C102" t="n">
-        <v>41825.760416666664</v>
+        <v>41927.6875</v>
       </c>
       <c r="D102" t="n">
-        <v>12.25</v>
+        <v>3.75</v>
       </c>
       <c s="2" r="E102" t="n">
-        <v>41826.84375</v>
+        <v>41946.71875</v>
       </c>
       <c s="2" r="F102" t="n">
-        <v>41827.0</v>
+        <v>41947.15625</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c s="1" r="A103" t="n">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c s="2" r="B103" t="n">
-        <v>41826.84375</v>
+        <v>41927.739583333336</v>
       </c>
       <c s="2" r="C103" t="n">
-        <v>41827.0</v>
+        <v>41928.083333333336</v>
       </c>
       <c r="D103" t="n">
-        <v>3.75</v>
+        <v>8.25</v>
       </c>
       <c s="2" r="E103" t="n">
-        <v>41849.25</v>
+        <v>41955.395833333336</v>
       </c>
       <c s="2" r="F103" t="n">
-        <v>41853.364583333336</v>
+        <v>41955.489583333336</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c s="1" r="A104" t="n">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c s="2" r="B104" t="n">
-        <v>41849.25</v>
+        <v>41945.145833333336</v>
       </c>
       <c s="2" r="C104" t="n">
-        <v>41854.6875</v>
+        <v>41945.364583333336</v>
       </c>
       <c r="D104" t="n">
-        <v>98.75</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E104" t="n">
-        <v>41853.364583333336</v>
+        <v>41955.71875</v>
       </c>
       <c s="2" r="F104" t="n">
-        <v>41854.6875</v>
+        <v>41956.020833333336</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c s="1" r="A105" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c s="2" r="B105" t="n">
-        <v>41927.53125</v>
+        <v>41946.71875</v>
       </c>
       <c s="2" r="C105" t="n">
-        <v>41927.6875</v>
+        <v>41947.15625</v>
       </c>
       <c r="D105" t="n">
-        <v>3.75</v>
+        <v>10.5</v>
       </c>
       <c s="2" r="E105" t="n">
-        <v>41927.739583333336</v>
+        <v>41959.0</v>
       </c>
       <c s="2" r="F105" t="n">
-        <v>41928.083333333336</v>
+        <v>41959.572916666664</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c s="1" r="A106" t="n">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c s="2" r="B106" t="n">
-        <v>41927.739583333336</v>
+        <v>41955.395833333336</v>
       </c>
       <c s="2" r="C106" t="n">
-        <v>41928.083333333336</v>
+        <v>41955.489583333336</v>
       </c>
       <c r="D106" t="n">
-        <v>8.25</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E106" t="n">
-        <v>41945.145833333336</v>
+        <v>41961.770833333336</v>
       </c>
       <c s="2" r="F106" t="n">
-        <v>41945.364583333336</v>
+        <v>41962.072916666664</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c s="1" r="A107" t="n">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c s="2" r="B107" t="n">
-        <v>41945.145833333336</v>
+        <v>41955.71875</v>
       </c>
       <c s="2" r="C107" t="n">
-        <v>41945.364583333336</v>
+        <v>41956.020833333336</v>
       </c>
       <c r="D107" t="n">
-        <v>5.25</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E107" t="n">
-        <v>41946.71875</v>
+        <v>41962.791666666664</v>
       </c>
       <c s="2" r="F107" t="n">
-        <v>41947.15625</v>
+        <v>41963.041666666664</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c s="1" r="A108" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c s="2" r="B108" t="n">
-        <v>41946.71875</v>
+        <v>41959.0</v>
       </c>
       <c s="2" r="C108" t="n">
-        <v>41947.15625</v>
+        <v>41959.572916666664</v>
       </c>
       <c r="D108" t="n">
-        <v>10.5</v>
+        <v>13.75</v>
       </c>
       <c s="2" r="E108" t="n">
-        <v>41955.395833333336</v>
+        <v>41965.8125</v>
       </c>
       <c s="2" r="F108" t="n">
-        <v>41955.489583333336</v>
+        <v>41966.729166666664</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c s="1" r="A109" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c s="2" r="B109" t="n">
-        <v>41955.395833333336</v>
+        <v>41961.770833333336</v>
       </c>
       <c s="2" r="C109" t="n">
-        <v>41955.489583333336</v>
+        <v>41962.072916666664</v>
       </c>
       <c r="D109" t="n">
-        <v>2.25</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E109" t="n">
-        <v>41955.71875</v>
+        <v>41967.885416666664</v>
       </c>
       <c s="2" r="F109" t="n">
-        <v>41956.020833333336</v>
+        <v>41968.1875</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c s="1" r="A110" t="n">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c s="2" r="B110" t="n">
-        <v>41955.71875</v>
+        <v>41962.791666666664</v>
       </c>
       <c s="2" r="C110" t="n">
-        <v>41956.020833333336</v>
+        <v>41963.041666666664</v>
       </c>
       <c r="D110" t="n">
-        <v>7.25</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E110" t="n">
-        <v>41959.0</v>
+        <v>41977.84375</v>
       </c>
       <c s="2" r="F110" t="n">
-        <v>41959.572916666664</v>
+        <v>41978.697916666664</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c s="1" r="A111" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c s="2" r="B111" t="n">
-        <v>41959.0</v>
+        <v>41965.8125</v>
       </c>
       <c s="2" r="C111" t="n">
-        <v>41959.572916666664</v>
+        <v>41966.729166666664</v>
       </c>
       <c r="D111" t="n">
-        <v>13.75</v>
+        <v>22.0</v>
       </c>
       <c s="2" r="E111" t="n">
-        <v>41961.770833333336</v>
+        <v>41982.427083333336</v>
       </c>
       <c s="2" r="F111" t="n">
-        <v>41962.072916666664</v>
+        <v>41983.03125</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c s="1" r="A112" t="n">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c s="2" r="B112" t="n">
-        <v>41961.770833333336</v>
+        <v>41967.885416666664</v>
       </c>
       <c s="2" r="C112" t="n">
-        <v>41962.072916666664</v>
+        <v>41968.1875</v>
       </c>
       <c r="D112" t="n">
         <v>7.25</v>
       </c>
       <c s="2" r="E112" t="n">
-        <v>41962.791666666664</v>
+        <v>41992.010416666664</v>
       </c>
       <c s="2" r="F112" t="n">
-        <v>41963.041666666664</v>
+        <v>41992.885416666664</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c s="1" r="A113" t="n">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c s="2" r="B113" t="n">
-        <v>41962.791666666664</v>
+        <v>41977.84375</v>
       </c>
       <c s="2" r="C113" t="n">
-        <v>41963.041666666664</v>
+        <v>41978.697916666664</v>
       </c>
       <c r="D113" t="n">
-        <v>6.0</v>
+        <v>20.5</v>
       </c>
       <c s="2" r="E113" t="n">
-        <v>41965.8125</v>
+        <v>41994.020833333336</v>
       </c>
       <c s="2" r="F113" t="n">
-        <v>41966.729166666664</v>
+        <v>41996.09375</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c s="1" r="A114" t="n">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c s="2" r="B114" t="n">
-        <v>41965.8125</v>
+        <v>41982.427083333336</v>
       </c>
       <c s="2" r="C114" t="n">
-        <v>41966.729166666664</v>
+        <v>41983.03125</v>
       </c>
       <c r="D114" t="n">
-        <v>22.0</v>
-      </c>
-      <c s="2" r="E114" t="n">
-        <v>41967.885416666664</v>
-      </c>
-      <c s="2" r="F114" t="n">
-        <v>41968.1875</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c s="1" r="A115" t="n">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c s="2" r="B115" t="n">
-        <v>41967.885416666664</v>
+        <v>41992.010416666664</v>
       </c>
       <c s="2" r="C115" t="n">
-        <v>41968.1875</v>
+        <v>41992.885416666664</v>
       </c>
       <c r="D115" t="n">
-        <v>7.25</v>
-      </c>
-      <c s="2" r="E115" t="n">
-        <v>41977.84375</v>
-      </c>
-      <c s="2" r="F115" t="n">
-        <v>41978.697916666664</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c s="1" r="A116" t="n">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c s="2" r="B116" t="n">
-        <v>41977.84375</v>
+        <v>41994.020833333336</v>
       </c>
       <c s="2" r="C116" t="n">
-        <v>41978.697916666664</v>
+        <v>41996.09375</v>
       </c>
       <c r="D116" t="n">
-        <v>20.5</v>
-      </c>
-      <c s="2" r="E116" t="n">
-        <v>41982.427083333336</v>
-      </c>
-      <c s="2" r="F116" t="n">
-        <v>41983.03125</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c s="1" r="A117" t="n">
-        <v>119</v>
-      </c>
-      <c s="2" r="B117" t="n">
-        <v>41982.427083333336</v>
-      </c>
-      <c s="2" r="C117" t="n">
-        <v>41983.03125</v>
-      </c>
-      <c r="D117" t="n">
-        <v>14.5</v>
-      </c>
-      <c s="2" r="E117" t="n">
-        <v>41992.010416666664</v>
-      </c>
-      <c s="2" r="F117" t="n">
-        <v>41992.885416666664</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c s="1" r="A118" t="n">
-        <v>120</v>
-      </c>
-      <c s="2" r="B118" t="n">
-        <v>41992.010416666664</v>
-      </c>
-      <c s="2" r="C118" t="n">
-        <v>41992.885416666664</v>
-      </c>
-      <c r="D118" t="n">
-        <v>21.0</v>
-      </c>
-      <c s="2" r="E118" t="n">
-        <v>41994.020833333336</v>
-      </c>
-      <c s="2" r="F118" t="n">
-        <v>41996.09375</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c s="1" r="A119" t="n">
-        <v>121</v>
-      </c>
-      <c s="2" r="B119" t="n">
-        <v>41994.020833333336</v>
-      </c>
-      <c s="2" r="C119" t="n">
-        <v>41996.09375</v>
-      </c>
-      <c r="D119" t="n">
         <v>49.75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a quick and dirty Change over time
</commit_message>
<xml_diff>
--- a/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
+++ b/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
@@ -396,7 +396,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -1712,7 +1712,7 @@
         <v>16.75</v>
       </c>
       <c s="2" r="E57" t="n">
-        <v>41684.614583333336</v>
+        <v>41684.625</v>
       </c>
       <c s="2" r="F57" t="n">
         <v>41684.84375</v>
@@ -1772,13 +1772,13 @@
         <v>63</v>
       </c>
       <c s="2" r="B60" t="n">
-        <v>41684.614583333336</v>
+        <v>41684.625</v>
       </c>
       <c s="2" r="C60" t="n">
         <v>41684.84375</v>
       </c>
       <c r="D60" t="n">
-        <v>5.5</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E60" t="n">
         <v>41690.46875</v>
@@ -1787,7 +1787,7 @@
         <v>41690.791666666664</v>
       </c>
       <c r="G60" t="n">
-        <v>19800000000000</v>
+        <v>18900000000000</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2999,6 +2999,12 @@
       <c r="D113" t="n">
         <v>14.5</v>
       </c>
+      <c s="2" r="E113" t="n">
+        <v>42005.354166666664</v>
+      </c>
+      <c s="2" r="F113" t="n">
+        <v>42005.895833333336</v>
+      </c>
       <c r="G113" t="n">
         <v>52200000000000</v>
       </c>
@@ -3016,6 +3022,12 @@
       <c r="D114" t="n">
         <v>21.0</v>
       </c>
+      <c s="2" r="E114" t="n">
+        <v>42006.5625</v>
+      </c>
+      <c s="2" r="F114" t="n">
+        <v>42006.854166666664</v>
+      </c>
       <c r="G114" t="n">
         <v>75600000000000</v>
       </c>
@@ -3033,8 +3045,111 @@
       <c r="D115" t="n">
         <v>49.75</v>
       </c>
+      <c s="2" r="E115" t="n">
+        <v>42008.8125</v>
+      </c>
+      <c s="2" r="F115" t="n">
+        <v>42008.947916666664</v>
+      </c>
       <c r="G115" t="n">
         <v>179100000000000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c s="1" r="A116" t="n">
+        <v>122</v>
+      </c>
+      <c s="2" r="B116" t="n">
+        <v>42005.354166666664</v>
+      </c>
+      <c s="2" r="C116" t="n">
+        <v>42005.895833333336</v>
+      </c>
+      <c r="D116" t="n">
+        <v>13.0</v>
+      </c>
+      <c s="2" r="E116" t="n">
+        <v>42009.125</v>
+      </c>
+      <c s="2" r="F116" t="n">
+        <v>42009.364583333336</v>
+      </c>
+      <c r="G116" t="n">
+        <v>46800000000000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c s="1" r="A117" t="n">
+        <v>123</v>
+      </c>
+      <c s="2" r="B117" t="n">
+        <v>42006.5625</v>
+      </c>
+      <c s="2" r="C117" t="n">
+        <v>42006.854166666664</v>
+      </c>
+      <c r="D117" t="n">
+        <v>7.0</v>
+      </c>
+      <c s="2" r="E117" t="n">
+        <v>42013.489583333336</v>
+      </c>
+      <c s="2" r="F117" t="n">
+        <v>42014.375</v>
+      </c>
+      <c r="G117" t="n">
+        <v>25200000000000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c s="1" r="A118" t="n">
+        <v>124</v>
+      </c>
+      <c s="2" r="B118" t="n">
+        <v>42008.8125</v>
+      </c>
+      <c s="2" r="C118" t="n">
+        <v>42008.947916666664</v>
+      </c>
+      <c r="D118" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="G118" t="n">
+        <v>11700000000000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c s="1" r="A119" t="n">
+        <v>125</v>
+      </c>
+      <c s="2" r="B119" t="n">
+        <v>42009.125</v>
+      </c>
+      <c s="2" r="C119" t="n">
+        <v>42009.364583333336</v>
+      </c>
+      <c r="D119" t="n">
+        <v>5.75</v>
+      </c>
+      <c r="G119" t="n">
+        <v>20700000000000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c s="1" r="A120" t="n">
+        <v>126</v>
+      </c>
+      <c s="2" r="B120" t="n">
+        <v>42013.489583333336</v>
+      </c>
+      <c s="2" r="C120" t="n">
+        <v>42014.375</v>
+      </c>
+      <c r="D120" t="n">
+        <v>21.25</v>
+      </c>
+      <c r="G120" t="n">
+        <v>76500000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new data up to June
haven't QC'ed yet
</commit_message>
<xml_diff>
--- a/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
+++ b/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
@@ -396,7 +396,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -438,22 +438,22 @@
         <v>0</v>
       </c>
       <c s="2" r="B2" t="n">
-        <v>40927.020833333336</v>
+        <v>40927.03125</v>
       </c>
       <c s="2" r="C2" t="n">
-        <v>40927.333333333336</v>
+        <v>40927.28125</v>
       </c>
       <c r="D2" t="n">
-        <v>7.5</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E2" t="n">
-        <v>40941.25</v>
+        <v>40941.260416666664</v>
       </c>
       <c s="2" r="F2" t="n">
-        <v>40941.770833333336</v>
+        <v>40941.666666666664</v>
       </c>
       <c r="G2" t="n">
-        <v>27000000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -461,22 +461,22 @@
         <v>1</v>
       </c>
       <c s="2" r="B3" t="n">
-        <v>40927.5625</v>
+        <v>40927.572916666664</v>
       </c>
       <c s="2" r="C3" t="n">
-        <v>40927.947916666664</v>
+        <v>40927.885416666664</v>
       </c>
       <c r="D3" t="n">
-        <v>9.25</v>
+        <v>7.5</v>
       </c>
       <c s="2" r="E3" t="n">
-        <v>40942.052083333336</v>
+        <v>40942.322916666664</v>
       </c>
       <c s="2" r="F3" t="n">
-        <v>40942.135416666664</v>
+        <v>40942.8125</v>
       </c>
       <c r="G3" t="n">
-        <v>33300000000000</v>
+        <v>27000000000000</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -484,22 +484,22 @@
         <v>3</v>
       </c>
       <c s="2" r="B4" t="n">
-        <v>40941.25</v>
+        <v>40941.260416666664</v>
       </c>
       <c s="2" r="C4" t="n">
-        <v>40941.770833333336</v>
+        <v>40941.666666666664</v>
       </c>
       <c r="D4" t="n">
-        <v>12.5</v>
+        <v>9.75</v>
       </c>
       <c s="2" r="E4" t="n">
-        <v>40942.229166666664</v>
+        <v>40944.96875</v>
       </c>
       <c s="2" r="F4" t="n">
-        <v>40942.322916666664</v>
+        <v>40946.833333333336</v>
       </c>
       <c r="G4" t="n">
-        <v>45000000000000</v>
+        <v>35100000000000</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -507,1537 +507,1537 @@
         <v>4</v>
       </c>
       <c s="2" r="B5" t="n">
-        <v>40942.052083333336</v>
+        <v>40942.322916666664</v>
       </c>
       <c s="2" r="C5" t="n">
-        <v>40942.895833333336</v>
+        <v>40942.8125</v>
       </c>
       <c r="D5" t="n">
-        <v>20.25</v>
+        <v>11.75</v>
       </c>
       <c s="2" r="E5" t="n">
-        <v>40942.322916666664</v>
+        <v>40962.875</v>
       </c>
       <c s="2" r="F5" t="n">
-        <v>40942.895833333336</v>
+        <v>40963.15625</v>
       </c>
       <c r="G5" t="n">
-        <v>72900000000000</v>
+        <v>42300000000000</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c s="1" r="A6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c s="2" r="B6" t="n">
         <v>40944.416666666664</v>
       </c>
       <c s="2" r="C6" t="n">
-        <v>40944.895833333336</v>
+        <v>40944.822916666664</v>
       </c>
       <c r="D6" t="n">
-        <v>11.5</v>
+        <v>9.75</v>
       </c>
       <c s="2" r="E6" t="n">
         <v>40976.6875</v>
       </c>
       <c s="2" r="F6" t="n">
-        <v>40976.854166666664</v>
+        <v>40976.822916666664</v>
       </c>
       <c r="G6" t="n">
-        <v>41400000000000</v>
+        <v>35100000000000</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c s="1" r="A7" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c s="2" r="B7" t="n">
-        <v>40944.958333333336</v>
+        <v>40944.96875</v>
       </c>
       <c s="2" r="C7" t="n">
-        <v>40947.0</v>
+        <v>40946.833333333336</v>
       </c>
       <c r="D7" t="n">
-        <v>49.0</v>
+        <v>44.75</v>
       </c>
       <c s="2" r="E7" t="n">
         <v>40977.25</v>
       </c>
       <c s="2" r="F7" t="n">
-        <v>40977.583333333336</v>
+        <v>40977.541666666664</v>
       </c>
       <c r="G7" t="n">
-        <v>176400000000000</v>
+        <v>161100000000000</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c s="1" r="A8" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c s="2" r="B8" t="n">
-        <v>40962.864583333336</v>
+        <v>40962.875</v>
       </c>
       <c s="2" r="C8" t="n">
-        <v>40963.21875</v>
+        <v>40963.15625</v>
       </c>
       <c r="D8" t="n">
-        <v>8.5</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E8" t="n">
-        <v>40984.416666666664</v>
+        <v>40984.427083333336</v>
       </c>
       <c s="2" r="F8" t="n">
-        <v>40984.6875</v>
+        <v>40984.59375</v>
       </c>
       <c r="G8" t="n">
-        <v>30600000000000</v>
+        <v>24300000000000</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c s="1" r="A9" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c s="2" r="B9" t="n">
         <v>40976.6875</v>
       </c>
       <c s="2" r="C9" t="n">
-        <v>40976.854166666664</v>
+        <v>40976.822916666664</v>
       </c>
       <c r="D9" t="n">
-        <v>4.0</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E9" t="n">
         <v>40985.489583333336</v>
       </c>
       <c s="2" r="F9" t="n">
-        <v>40985.739583333336</v>
+        <v>40985.71875</v>
       </c>
       <c r="G9" t="n">
-        <v>14400000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c s="1" r="A10" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c s="2" r="B10" t="n">
         <v>40977.25</v>
       </c>
       <c s="2" r="C10" t="n">
-        <v>40977.583333333336</v>
+        <v>40977.541666666664</v>
       </c>
       <c r="D10" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c s="2" r="E10" t="n">
         <v>40989.84375</v>
       </c>
       <c s="2" r="F10" t="n">
-        <v>40990.145833333336</v>
+        <v>40990.09375</v>
       </c>
       <c r="G10" t="n">
-        <v>28800000000000</v>
+        <v>25200000000000</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c s="1" r="A11" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c s="2" r="B11" t="n">
-        <v>40984.416666666664</v>
+        <v>40984.427083333336</v>
       </c>
       <c s="2" r="C11" t="n">
-        <v>40984.6875</v>
+        <v>40984.59375</v>
       </c>
       <c r="D11" t="n">
-        <v>6.5</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E11" t="n">
-        <v>40990.21875</v>
+        <v>40990.90625</v>
       </c>
       <c s="2" r="F11" t="n">
-        <v>40990.302083333336</v>
+        <v>40991.260416666664</v>
       </c>
       <c r="G11" t="n">
-        <v>23400000000000</v>
+        <v>14400000000000</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c s="1" r="A12" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c s="2" r="B12" t="n">
         <v>40985.489583333336</v>
       </c>
       <c s="2" r="C12" t="n">
-        <v>40985.739583333336</v>
+        <v>40985.71875</v>
       </c>
       <c r="D12" t="n">
-        <v>6.0</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E12" t="n">
-        <v>40990.90625</v>
+        <v>40993.145833333336</v>
       </c>
       <c s="2" r="F12" t="n">
-        <v>40991.322916666664</v>
+        <v>40993.854166666664</v>
       </c>
       <c r="G12" t="n">
-        <v>21600000000000</v>
+        <v>19800000000000</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c s="1" r="A13" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c s="2" r="B13" t="n">
         <v>40989.84375</v>
       </c>
       <c s="2" r="C13" t="n">
-        <v>40990.145833333336</v>
+        <v>40990.09375</v>
       </c>
       <c r="D13" t="n">
-        <v>7.25</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E13" t="n">
-        <v>40993.145833333336</v>
+        <v>41037.197916666664</v>
       </c>
       <c s="2" r="F13" t="n">
-        <v>40993.947916666664</v>
+        <v>41037.322916666664</v>
       </c>
       <c r="G13" t="n">
-        <v>26100000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c s="1" r="A14" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c s="2" r="B14" t="n">
-        <v>40990.21875</v>
+        <v>40990.90625</v>
       </c>
       <c s="2" r="C14" t="n">
-        <v>40990.302083333336</v>
+        <v>40991.260416666664</v>
       </c>
       <c r="D14" t="n">
-        <v>2.0</v>
+        <v>8.5</v>
       </c>
       <c s="2" r="E14" t="n">
-        <v>41031.677083333336</v>
+        <v>41051.78125</v>
       </c>
       <c s="2" r="F14" t="n">
-        <v>41031.75</v>
+        <v>41052.083333333336</v>
       </c>
       <c r="G14" t="n">
-        <v>7200000000000</v>
+        <v>30600000000000</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c s="1" r="A15" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c s="2" r="B15" t="n">
-        <v>40990.90625</v>
+        <v>40993.145833333336</v>
       </c>
       <c s="2" r="C15" t="n">
-        <v>40991.322916666664</v>
+        <v>40993.854166666664</v>
       </c>
       <c r="D15" t="n">
-        <v>10.0</v>
+        <v>17.0</v>
       </c>
       <c s="2" r="E15" t="n">
-        <v>41037.197916666664</v>
+        <v>41052.333333333336</v>
       </c>
       <c s="2" r="F15" t="n">
-        <v>41037.333333333336</v>
+        <v>41053.479166666664</v>
       </c>
       <c r="G15" t="n">
-        <v>36000000000000</v>
+        <v>61200000000000</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c s="1" r="A16" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c s="2" r="B16" t="n">
-        <v>40993.145833333336</v>
+        <v>41037.197916666664</v>
       </c>
       <c s="2" r="C16" t="n">
-        <v>40993.947916666664</v>
+        <v>41037.322916666664</v>
       </c>
       <c r="D16" t="n">
-        <v>19.25</v>
+        <v>3.0</v>
       </c>
       <c s="2" r="E16" t="n">
-        <v>41051.78125</v>
+        <v>41053.854166666664</v>
       </c>
       <c s="2" r="F16" t="n">
-        <v>41052.125</v>
+        <v>41054.65625</v>
       </c>
       <c r="G16" t="n">
-        <v>69300000000000</v>
+        <v>10800000000000</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c s="1" r="A17" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c s="2" r="B17" t="n">
-        <v>41031.677083333336</v>
+        <v>41051.78125</v>
       </c>
       <c s="2" r="C17" t="n">
-        <v>41031.75</v>
+        <v>41052.083333333336</v>
       </c>
       <c r="D17" t="n">
-        <v>1.75</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E17" t="n">
-        <v>41052.322916666664</v>
+        <v>41055.0625</v>
       </c>
       <c s="2" r="F17" t="n">
-        <v>41053.583333333336</v>
+        <v>41055.645833333336</v>
       </c>
       <c r="G17" t="n">
-        <v>6300000000000</v>
+        <v>26100000000000</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c s="1" r="A18" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c s="2" r="B18" t="n">
-        <v>41037.197916666664</v>
+        <v>41052.333333333336</v>
       </c>
       <c s="2" r="C18" t="n">
-        <v>41037.333333333336</v>
+        <v>41053.479166666664</v>
       </c>
       <c r="D18" t="n">
-        <v>3.25</v>
+        <v>27.5</v>
       </c>
       <c s="2" r="E18" t="n">
-        <v>41053.833333333336</v>
+        <v>41063.4375</v>
       </c>
       <c s="2" r="F18" t="n">
-        <v>41054.708333333336</v>
+        <v>41063.84375</v>
       </c>
       <c r="G18" t="n">
-        <v>11700000000000</v>
+        <v>99000000000000</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c s="1" r="A19" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c s="2" r="B19" t="n">
-        <v>41051.78125</v>
+        <v>41053.854166666664</v>
       </c>
       <c s="2" r="C19" t="n">
-        <v>41052.125</v>
+        <v>41054.65625</v>
       </c>
       <c r="D19" t="n">
-        <v>8.25</v>
+        <v>19.25</v>
       </c>
       <c s="2" r="E19" t="n">
-        <v>41055.0625</v>
+        <v>41064.010416666664</v>
       </c>
       <c s="2" r="F19" t="n">
-        <v>41055.708333333336</v>
+        <v>41064.46875</v>
       </c>
       <c r="G19" t="n">
-        <v>29700000000000</v>
+        <v>69300000000000</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c s="1" r="A20" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c s="2" r="B20" t="n">
-        <v>41052.322916666664</v>
+        <v>41055.0625</v>
       </c>
       <c s="2" r="C20" t="n">
-        <v>41053.583333333336</v>
+        <v>41055.645833333336</v>
       </c>
       <c r="D20" t="n">
-        <v>30.25</v>
+        <v>14.0</v>
       </c>
       <c s="2" r="E20" t="n">
-        <v>41063.427083333336</v>
+        <v>41064.604166666664</v>
       </c>
       <c s="2" r="F20" t="n">
-        <v>41063.885416666664</v>
+        <v>41065.770833333336</v>
       </c>
       <c r="G20" t="n">
-        <v>108900000000000</v>
+        <v>50400000000000</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c s="1" r="A21" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c s="2" r="B21" t="n">
-        <v>41053.833333333336</v>
+        <v>41063.4375</v>
       </c>
       <c s="2" r="C21" t="n">
-        <v>41054.708333333336</v>
+        <v>41063.84375</v>
       </c>
       <c r="D21" t="n">
-        <v>21.0</v>
+        <v>9.75</v>
       </c>
       <c s="2" r="E21" t="n">
-        <v>41064.010416666664</v>
+        <v>41066.885416666664</v>
       </c>
       <c s="2" r="F21" t="n">
-        <v>41064.46875</v>
+        <v>41067.020833333336</v>
       </c>
       <c r="G21" t="n">
-        <v>75600000000000</v>
+        <v>35100000000000</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c s="1" r="A22" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c s="2" r="B22" t="n">
-        <v>41055.0625</v>
+        <v>41064.010416666664</v>
       </c>
       <c s="2" r="C22" t="n">
-        <v>41055.708333333336</v>
+        <v>41064.46875</v>
       </c>
       <c r="D22" t="n">
-        <v>15.5</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E22" t="n">
-        <v>41064.604166666664</v>
+        <v>41067.333333333336</v>
       </c>
       <c s="2" r="F22" t="n">
-        <v>41065.895833333336</v>
+        <v>41067.614583333336</v>
       </c>
       <c r="G22" t="n">
-        <v>55800000000000</v>
+        <v>39600000000000</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c s="1" r="A23" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c s="2" r="B23" t="n">
-        <v>41063.427083333336</v>
+        <v>41064.604166666664</v>
       </c>
       <c s="2" r="C23" t="n">
-        <v>41063.885416666664</v>
+        <v>41065.770833333336</v>
       </c>
       <c r="D23" t="n">
-        <v>11.0</v>
+        <v>28.0</v>
       </c>
       <c s="2" r="E23" t="n">
-        <v>41066.885416666664</v>
+        <v>41098.083333333336</v>
       </c>
       <c s="2" r="F23" t="n">
-        <v>41067.270833333336</v>
+        <v>41098.229166666664</v>
       </c>
       <c r="G23" t="n">
-        <v>39600000000000</v>
+        <v>100800000000000</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c s="1" r="A24" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c s="2" r="B24" t="n">
-        <v>41064.010416666664</v>
+        <v>41066.885416666664</v>
       </c>
       <c s="2" r="C24" t="n">
-        <v>41064.46875</v>
+        <v>41067.020833333336</v>
       </c>
       <c r="D24" t="n">
-        <v>11.0</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E24" t="n">
-        <v>41067.3125</v>
+        <v>41130.145833333336</v>
       </c>
       <c s="2" r="F24" t="n">
-        <v>41067.729166666664</v>
+        <v>41130.364583333336</v>
       </c>
       <c r="G24" t="n">
-        <v>39600000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c s="1" r="A25" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c s="2" r="B25" t="n">
-        <v>41064.604166666664</v>
+        <v>41067.333333333336</v>
       </c>
       <c s="2" r="C25" t="n">
-        <v>41065.895833333336</v>
+        <v>41067.614583333336</v>
       </c>
       <c r="D25" t="n">
-        <v>31.0</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E25" t="n">
-        <v>41098.083333333336</v>
+        <v>41153.479166666664</v>
       </c>
       <c s="2" r="F25" t="n">
-        <v>41098.25</v>
+        <v>41155.15625</v>
       </c>
       <c r="G25" t="n">
-        <v>111600000000000</v>
+        <v>24300000000000</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c s="1" r="A26" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c s="2" r="B26" t="n">
-        <v>41066.885416666664</v>
+        <v>41098.083333333336</v>
       </c>
       <c s="2" r="C26" t="n">
-        <v>41067.270833333336</v>
+        <v>41098.229166666664</v>
       </c>
       <c r="D26" t="n">
-        <v>9.25</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E26" t="n">
-        <v>41117.09375</v>
+        <v>41316.875</v>
       </c>
       <c s="2" r="F26" t="n">
-        <v>41117.1875</v>
+        <v>41317.458333333336</v>
       </c>
       <c r="G26" t="n">
-        <v>33300000000000</v>
+        <v>12600000000000</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c s="1" r="A27" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c s="2" r="B27" t="n">
-        <v>41067.3125</v>
+        <v>41130.145833333336</v>
       </c>
       <c s="2" r="C27" t="n">
-        <v>41067.729166666664</v>
+        <v>41130.364583333336</v>
       </c>
       <c r="D27" t="n">
-        <v>10.0</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E27" t="n">
-        <v>41117.854166666664</v>
+        <v>41338.78125</v>
       </c>
       <c s="2" r="F27" t="n">
-        <v>41117.927083333336</v>
+        <v>41339.041666666664</v>
       </c>
       <c r="G27" t="n">
-        <v>36000000000000</v>
+        <v>18900000000000</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c s="1" r="A28" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c s="2" r="B28" t="n">
-        <v>41098.083333333336</v>
+        <v>41153.479166666664</v>
       </c>
       <c s="2" r="C28" t="n">
-        <v>41098.25</v>
+        <v>41155.15625</v>
       </c>
       <c r="D28" t="n">
-        <v>4.0</v>
+        <v>40.25</v>
       </c>
       <c s="2" r="E28" t="n">
-        <v>41130.145833333336</v>
+        <v>41339.385416666664</v>
       </c>
       <c s="2" r="F28" t="n">
-        <v>41130.395833333336</v>
+        <v>41339.895833333336</v>
       </c>
       <c r="G28" t="n">
-        <v>14400000000000</v>
+        <v>144900000000000</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c s="1" r="A29" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c s="2" r="B29" t="n">
-        <v>41117.09375</v>
+        <v>41316.875</v>
       </c>
       <c s="2" r="C29" t="n">
-        <v>41117.1875</v>
+        <v>41317.458333333336</v>
       </c>
       <c r="D29" t="n">
-        <v>2.25</v>
+        <v>14.0</v>
       </c>
       <c s="2" r="E29" t="n">
-        <v>41153.479166666664</v>
+        <v>41340.604166666664</v>
       </c>
       <c s="2" r="F29" t="n">
-        <v>41155.270833333336</v>
+        <v>41341.760416666664</v>
       </c>
       <c r="G29" t="n">
-        <v>8100000000000</v>
+        <v>50400000000000</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c s="1" r="A30" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c s="2" r="B30" t="n">
-        <v>41117.854166666664</v>
+        <v>41338.78125</v>
       </c>
       <c s="2" r="C30" t="n">
-        <v>41117.927083333336</v>
+        <v>41339.041666666664</v>
       </c>
       <c r="D30" t="n">
-        <v>1.75</v>
+        <v>6.25</v>
       </c>
       <c s="2" r="E30" t="n">
-        <v>41316.875</v>
+        <v>41344.104166666664</v>
       </c>
       <c s="2" r="F30" t="n">
-        <v>41317.53125</v>
+        <v>41344.625</v>
       </c>
       <c r="G30" t="n">
-        <v>6300000000000</v>
+        <v>22500000000000</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c s="1" r="A31" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c s="2" r="B31" t="n">
-        <v>41130.145833333336</v>
+        <v>41339.385416666664</v>
       </c>
       <c s="2" r="C31" t="n">
-        <v>41130.395833333336</v>
+        <v>41339.895833333336</v>
       </c>
       <c r="D31" t="n">
-        <v>6.0</v>
+        <v>12.25</v>
       </c>
       <c s="2" r="E31" t="n">
-        <v>41338.78125</v>
+        <v>41354.552083333336</v>
       </c>
       <c s="2" r="F31" t="n">
-        <v>41339.083333333336</v>
+        <v>41354.635416666664</v>
       </c>
       <c r="G31" t="n">
-        <v>21600000000000</v>
+        <v>44100000000000</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c s="1" r="A32" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c s="2" r="B32" t="n">
-        <v>41153.479166666664</v>
+        <v>41340.604166666664</v>
       </c>
       <c s="2" r="C32" t="n">
-        <v>41155.270833333336</v>
+        <v>41341.760416666664</v>
       </c>
       <c r="D32" t="n">
-        <v>43.0</v>
+        <v>27.75</v>
       </c>
       <c s="2" r="E32" t="n">
-        <v>41339.385416666664</v>
+        <v>41380.46875</v>
       </c>
       <c s="2" r="F32" t="n">
-        <v>41339.916666666664</v>
+        <v>41380.875</v>
       </c>
       <c r="G32" t="n">
-        <v>154800000000000</v>
+        <v>99900000000000</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c s="1" r="A33" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c s="2" r="B33" t="n">
-        <v>41316.875</v>
+        <v>41344.104166666664</v>
       </c>
       <c s="2" r="C33" t="n">
-        <v>41317.53125</v>
+        <v>41344.625</v>
       </c>
       <c r="D33" t="n">
-        <v>15.75</v>
+        <v>12.5</v>
       </c>
       <c s="2" r="E33" t="n">
-        <v>41340.604166666664</v>
+        <v>41381.010416666664</v>
       </c>
       <c s="2" r="F33" t="n">
-        <v>41341.84375</v>
+        <v>41381.604166666664</v>
       </c>
       <c r="G33" t="n">
-        <v>56700000000000</v>
+        <v>45000000000000</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c s="1" r="A34" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c s="2" r="B34" t="n">
-        <v>41338.78125</v>
+        <v>41354.552083333336</v>
       </c>
       <c s="2" r="C34" t="n">
-        <v>41339.083333333336</v>
+        <v>41354.635416666664</v>
       </c>
       <c r="D34" t="n">
-        <v>7.25</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E34" t="n">
-        <v>41344.09375</v>
+        <v>41384.197916666664</v>
       </c>
       <c s="2" r="F34" t="n">
-        <v>41344.791666666664</v>
+        <v>41384.552083333336</v>
       </c>
       <c r="G34" t="n">
-        <v>26100000000000</v>
+        <v>7200000000000</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c s="1" r="A35" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c s="2" r="B35" t="n">
-        <v>41339.385416666664</v>
+        <v>41380.46875</v>
       </c>
       <c s="2" r="C35" t="n">
-        <v>41339.916666666664</v>
+        <v>41380.875</v>
       </c>
       <c r="D35" t="n">
-        <v>12.75</v>
+        <v>9.75</v>
       </c>
       <c s="2" r="E35" t="n">
-        <v>41354.552083333336</v>
+        <v>41387.5625</v>
       </c>
       <c s="2" r="F35" t="n">
-        <v>41354.645833333336</v>
+        <v>41388.25</v>
       </c>
       <c r="G35" t="n">
-        <v>45900000000000</v>
+        <v>35100000000000</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c s="1" r="A36" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c s="2" r="B36" t="n">
-        <v>41340.604166666664</v>
+        <v>41381.010416666664</v>
       </c>
       <c s="2" r="C36" t="n">
-        <v>41341.84375</v>
+        <v>41381.604166666664</v>
       </c>
       <c r="D36" t="n">
-        <v>29.75</v>
+        <v>14.25</v>
       </c>
       <c s="2" r="E36" t="n">
-        <v>41356.458333333336</v>
+        <v>41392.427083333336</v>
       </c>
       <c s="2" r="F36" t="n">
-        <v>41356.53125</v>
+        <v>41392.59375</v>
       </c>
       <c r="G36" t="n">
-        <v>107100000000000</v>
+        <v>51300000000000</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c s="1" r="A37" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c s="2" r="B37" t="n">
-        <v>41344.09375</v>
+        <v>41384.197916666664</v>
       </c>
       <c s="2" r="C37" t="n">
-        <v>41344.791666666664</v>
+        <v>41384.552083333336</v>
       </c>
       <c r="D37" t="n">
-        <v>16.75</v>
+        <v>8.5</v>
       </c>
       <c s="2" r="E37" t="n">
-        <v>41380.458333333336</v>
+        <v>41392.84375</v>
       </c>
       <c s="2" r="F37" t="n">
-        <v>41380.90625</v>
+        <v>41393.125</v>
       </c>
       <c r="G37" t="n">
-        <v>60300000000000</v>
+        <v>30600000000000</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c s="1" r="A38" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c s="2" r="B38" t="n">
-        <v>41354.552083333336</v>
+        <v>41387.5625</v>
       </c>
       <c s="2" r="C38" t="n">
-        <v>41354.645833333336</v>
+        <v>41388.25</v>
       </c>
       <c r="D38" t="n">
-        <v>2.25</v>
+        <v>16.5</v>
       </c>
       <c s="2" r="E38" t="n">
-        <v>41381.0</v>
+        <v>41394.625</v>
       </c>
       <c s="2" r="F38" t="n">
-        <v>41381.697916666664</v>
+        <v>41395.59375</v>
       </c>
       <c r="G38" t="n">
-        <v>8100000000000</v>
+        <v>59400000000000</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c s="1" r="A39" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c s="2" r="B39" t="n">
-        <v>41356.458333333336</v>
+        <v>41392.427083333336</v>
       </c>
       <c s="2" r="C39" t="n">
-        <v>41356.53125</v>
+        <v>41392.59375</v>
       </c>
       <c r="D39" t="n">
-        <v>1.75</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E39" t="n">
-        <v>41384.1875</v>
+        <v>41430.25</v>
       </c>
       <c s="2" r="F39" t="n">
-        <v>41384.604166666664</v>
+        <v>41431.145833333336</v>
       </c>
       <c r="G39" t="n">
-        <v>6300000000000</v>
+        <v>14400000000000</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c s="1" r="A40" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c s="2" r="B40" t="n">
-        <v>41380.458333333336</v>
+        <v>41392.84375</v>
       </c>
       <c s="2" r="C40" t="n">
-        <v>41380.90625</v>
+        <v>41393.125</v>
       </c>
       <c r="D40" t="n">
-        <v>10.75</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E40" t="n">
-        <v>41387.5625</v>
+        <v>41441.135416666664</v>
       </c>
       <c s="2" r="F40" t="n">
-        <v>41388.3125</v>
+        <v>41441.385416666664</v>
       </c>
       <c r="G40" t="n">
-        <v>38700000000000</v>
+        <v>24300000000000</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c s="1" r="A41" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c s="2" r="B41" t="n">
-        <v>41381.0</v>
+        <v>41394.625</v>
       </c>
       <c s="2" r="C41" t="n">
-        <v>41381.697916666664</v>
+        <v>41395.59375</v>
       </c>
       <c r="D41" t="n">
-        <v>16.75</v>
+        <v>23.25</v>
       </c>
       <c s="2" r="E41" t="n">
-        <v>41392.427083333336</v>
+        <v>41472.958333333336</v>
       </c>
       <c s="2" r="F41" t="n">
-        <v>41392.625</v>
+        <v>41473.427083333336</v>
       </c>
       <c r="G41" t="n">
-        <v>60300000000000</v>
+        <v>83700000000000</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c s="1" r="A42" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c s="2" r="B42" t="n">
-        <v>41384.1875</v>
+        <v>41430.25</v>
       </c>
       <c s="2" r="C42" t="n">
-        <v>41384.604166666664</v>
+        <v>41431.145833333336</v>
       </c>
       <c r="D42" t="n">
-        <v>10.0</v>
+        <v>21.5</v>
       </c>
       <c s="2" r="E42" t="n">
-        <v>41392.84375</v>
+        <v>41474.385416666664</v>
       </c>
       <c s="2" r="F42" t="n">
-        <v>41393.166666666664</v>
+        <v>41474.604166666664</v>
       </c>
       <c r="G42" t="n">
-        <v>36000000000000</v>
+        <v>77400000000000</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c s="1" r="A43" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c s="2" r="B43" t="n">
-        <v>41387.5625</v>
+        <v>41441.135416666664</v>
       </c>
       <c s="2" r="C43" t="n">
-        <v>41388.3125</v>
+        <v>41441.385416666664</v>
       </c>
       <c r="D43" t="n">
-        <v>18.0</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E43" t="n">
-        <v>41394.625</v>
+        <v>41474.635416666664</v>
       </c>
       <c s="2" r="F43" t="n">
-        <v>41395.65625</v>
+        <v>41475.614583333336</v>
       </c>
       <c r="G43" t="n">
-        <v>64800000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c s="1" r="A44" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c s="2" r="B44" t="n">
-        <v>41392.427083333336</v>
+        <v>41472.958333333336</v>
       </c>
       <c s="2" r="C44" t="n">
-        <v>41392.625</v>
+        <v>41473.427083333336</v>
       </c>
       <c r="D44" t="n">
-        <v>4.75</v>
+        <v>11.25</v>
       </c>
       <c s="2" r="E44" t="n">
-        <v>41405.604166666664</v>
+        <v>41492.0</v>
       </c>
       <c s="2" r="F44" t="n">
-        <v>41405.677083333336</v>
+        <v>41492.197916666664</v>
       </c>
       <c r="G44" t="n">
-        <v>17100000000000</v>
+        <v>40500000000000</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c s="1" r="A45" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c s="2" r="B45" t="n">
-        <v>41392.84375</v>
+        <v>41474.385416666664</v>
       </c>
       <c s="2" r="C45" t="n">
-        <v>41393.166666666664</v>
+        <v>41474.604166666664</v>
       </c>
       <c r="D45" t="n">
-        <v>7.75</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E45" t="n">
-        <v>41430.239583333336</v>
+        <v>41496.1875</v>
       </c>
       <c s="2" r="F45" t="n">
-        <v>41431.208333333336</v>
+        <v>41497.0</v>
       </c>
       <c r="G45" t="n">
-        <v>27900000000000</v>
+        <v>18900000000000</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c s="1" r="A46" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c s="2" r="B46" t="n">
-        <v>41394.625</v>
+        <v>41474.635416666664</v>
       </c>
       <c s="2" r="C46" t="n">
-        <v>41395.65625</v>
+        <v>41475.614583333336</v>
       </c>
       <c r="D46" t="n">
-        <v>24.75</v>
+        <v>23.5</v>
       </c>
       <c s="2" r="E46" t="n">
-        <v>41441.135416666664</v>
+        <v>41501.791666666664</v>
       </c>
       <c s="2" r="F46" t="n">
-        <v>41441.40625</v>
+        <v>41501.9375</v>
       </c>
       <c r="G46" t="n">
-        <v>89100000000000</v>
+        <v>84600000000000</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c s="1" r="A47" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c s="2" r="B47" t="n">
-        <v>41405.604166666664</v>
+        <v>41492.0</v>
       </c>
       <c s="2" r="C47" t="n">
-        <v>41405.677083333336</v>
+        <v>41492.197916666664</v>
       </c>
       <c r="D47" t="n">
-        <v>1.75</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E47" t="n">
-        <v>41472.145833333336</v>
+        <v>41502.333333333336</v>
       </c>
       <c s="2" r="F47" t="n">
-        <v>41472.229166666664</v>
+        <v>41504.583333333336</v>
       </c>
       <c r="G47" t="n">
-        <v>6300000000000</v>
+        <v>17100000000000</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c s="1" r="A48" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c s="2" r="B48" t="n">
-        <v>41430.239583333336</v>
+        <v>41496.1875</v>
       </c>
       <c s="2" r="C48" t="n">
-        <v>41431.208333333336</v>
+        <v>41497.0</v>
       </c>
       <c r="D48" t="n">
-        <v>23.25</v>
+        <v>19.5</v>
       </c>
       <c s="2" r="E48" t="n">
-        <v>41472.958333333336</v>
+        <v>41505.28125</v>
       </c>
       <c s="2" r="F48" t="n">
-        <v>41473.46875</v>
+        <v>41505.854166666664</v>
       </c>
       <c r="G48" t="n">
-        <v>83700000000000</v>
+        <v>70200000000000</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c s="1" r="A49" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c s="2" r="B49" t="n">
-        <v>41441.135416666664</v>
+        <v>41501.791666666664</v>
       </c>
       <c s="2" r="C49" t="n">
-        <v>41441.40625</v>
+        <v>41501.9375</v>
       </c>
       <c r="D49" t="n">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E49" t="n">
-        <v>41474.364583333336</v>
+        <v>41518.197916666664</v>
       </c>
       <c s="2" r="F49" t="n">
-        <v>41474.625</v>
+        <v>41518.270833333336</v>
       </c>
       <c r="G49" t="n">
-        <v>23400000000000</v>
+        <v>12600000000000</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c s="1" r="A50" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c s="2" r="B50" t="n">
-        <v>41472.145833333336</v>
+        <v>41502.333333333336</v>
       </c>
       <c s="2" r="C50" t="n">
-        <v>41472.229166666664</v>
+        <v>41504.583333333336</v>
       </c>
       <c r="D50" t="n">
-        <v>2.0</v>
+        <v>54.0</v>
       </c>
       <c s="2" r="E50" t="n">
-        <v>41474.625</v>
+        <v>41518.354166666664</v>
       </c>
       <c s="2" r="F50" t="n">
-        <v>41475.666666666664</v>
+        <v>41518.583333333336</v>
       </c>
       <c r="G50" t="n">
-        <v>7200000000000</v>
+        <v>194400000000000</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c s="1" r="A51" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c s="2" r="B51" t="n">
-        <v>41472.958333333336</v>
+        <v>41505.28125</v>
       </c>
       <c s="2" r="C51" t="n">
-        <v>41473.46875</v>
+        <v>41505.854166666664</v>
       </c>
       <c r="D51" t="n">
-        <v>12.25</v>
+        <v>13.75</v>
       </c>
       <c s="2" r="E51" t="n">
-        <v>41496.1875</v>
+        <v>41684.625</v>
       </c>
       <c s="2" r="F51" t="n">
-        <v>41497.052083333336</v>
+        <v>41684.822916666664</v>
       </c>
       <c r="G51" t="n">
-        <v>44100000000000</v>
+        <v>49500000000000</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c s="1" r="A52" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c s="2" r="B52" t="n">
-        <v>41474.364583333336</v>
+        <v>41518.197916666664</v>
       </c>
       <c s="2" r="C52" t="n">
-        <v>41475.666666666664</v>
+        <v>41518.270833333336</v>
       </c>
       <c r="D52" t="n">
-        <v>31.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E52" t="n">
-        <v>41501.791666666664</v>
+        <v>41690.46875</v>
       </c>
       <c s="2" r="F52" t="n">
-        <v>41501.947916666664</v>
+        <v>41690.75</v>
       </c>
       <c r="G52" t="n">
-        <v>112500000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c s="1" r="A53" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c s="2" r="B53" t="n">
-        <v>41491.989583333336</v>
+        <v>41518.354166666664</v>
       </c>
       <c s="2" r="C53" t="n">
-        <v>41492.229166666664</v>
+        <v>41518.583333333336</v>
       </c>
       <c r="D53" t="n">
-        <v>5.75</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E53" t="n">
-        <v>41502.333333333336</v>
+        <v>41691.479166666664</v>
       </c>
       <c s="2" r="F53" t="n">
-        <v>41504.677083333336</v>
+        <v>41692.145833333336</v>
       </c>
       <c r="G53" t="n">
-        <v>20700000000000</v>
+        <v>19800000000000</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c s="1" r="A54" t="n">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c s="2" r="B54" t="n">
-        <v>41496.1875</v>
+        <v>41684.625</v>
       </c>
       <c s="2" r="C54" t="n">
-        <v>41497.052083333336</v>
+        <v>41684.822916666664</v>
       </c>
       <c r="D54" t="n">
-        <v>20.75</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E54" t="n">
-        <v>41505.28125</v>
+        <v>41695.885416666664</v>
       </c>
       <c s="2" r="F54" t="n">
-        <v>41505.979166666664</v>
+        <v>41696.697916666664</v>
       </c>
       <c r="G54" t="n">
-        <v>74700000000000</v>
+        <v>17100000000000</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c s="1" r="A55" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c s="2" r="B55" t="n">
-        <v>41501.791666666664</v>
+        <v>41690.46875</v>
       </c>
       <c s="2" r="C55" t="n">
-        <v>41501.947916666664</v>
+        <v>41690.75</v>
       </c>
       <c r="D55" t="n">
-        <v>3.75</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E55" t="n">
-        <v>41518.197916666664</v>
+        <v>41697.083333333336</v>
       </c>
       <c s="2" r="F55" t="n">
-        <v>41518.28125</v>
+        <v>41697.572916666664</v>
       </c>
       <c r="G55" t="n">
-        <v>13500000000000</v>
+        <v>24300000000000</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c s="1" r="A56" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c s="2" r="B56" t="n">
-        <v>41502.333333333336</v>
+        <v>41691.479166666664</v>
       </c>
       <c s="2" r="C56" t="n">
-        <v>41504.677083333336</v>
+        <v>41692.145833333336</v>
       </c>
       <c r="D56" t="n">
-        <v>56.25</v>
+        <v>16.0</v>
       </c>
       <c s="2" r="E56" t="n">
-        <v>41518.354166666664</v>
+        <v>41697.677083333336</v>
       </c>
       <c s="2" r="F56" t="n">
-        <v>41518.635416666664</v>
+        <v>41698.010416666664</v>
       </c>
       <c r="G56" t="n">
-        <v>202500000000000</v>
+        <v>57600000000000</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c s="1" r="A57" t="n">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c s="2" r="B57" t="n">
-        <v>41505.28125</v>
+        <v>41695.885416666664</v>
       </c>
       <c s="2" r="C57" t="n">
-        <v>41505.979166666664</v>
+        <v>41696.697916666664</v>
       </c>
       <c r="D57" t="n">
-        <v>16.75</v>
+        <v>19.5</v>
       </c>
       <c s="2" r="E57" t="n">
-        <v>41684.625</v>
+        <v>41704.822916666664</v>
       </c>
       <c s="2" r="F57" t="n">
-        <v>41684.84375</v>
+        <v>41705.197916666664</v>
       </c>
       <c r="G57" t="n">
-        <v>60300000000000</v>
+        <v>70200000000000</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c s="1" r="A58" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c s="2" r="B58" t="n">
-        <v>41518.197916666664</v>
+        <v>41697.083333333336</v>
       </c>
       <c s="2" r="C58" t="n">
-        <v>41518.28125</v>
+        <v>41697.572916666664</v>
       </c>
       <c r="D58" t="n">
-        <v>2.0</v>
+        <v>11.75</v>
       </c>
       <c s="2" r="E58" t="n">
-        <v>41685.375</v>
+        <v>41711.520833333336</v>
       </c>
       <c s="2" r="F58" t="n">
-        <v>41685.479166666664</v>
+        <v>41711.635416666664</v>
       </c>
       <c r="G58" t="n">
-        <v>7200000000000</v>
+        <v>42300000000000</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c s="1" r="A59" t="n">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c s="2" r="B59" t="n">
-        <v>41518.354166666664</v>
+        <v>41697.677083333336</v>
       </c>
       <c s="2" r="C59" t="n">
-        <v>41518.635416666664</v>
+        <v>41698.010416666664</v>
       </c>
       <c r="D59" t="n">
-        <v>6.75</v>
+        <v>8.0</v>
       </c>
       <c s="2" r="E59" t="n">
-        <v>41688.760416666664</v>
+        <v>41711.666666666664</v>
       </c>
       <c s="2" r="F59" t="n">
-        <v>41688.833333333336</v>
+        <v>41711.791666666664</v>
       </c>
       <c r="G59" t="n">
-        <v>24300000000000</v>
+        <v>28800000000000</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c s="1" r="A60" t="n">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c s="2" r="B60" t="n">
-        <v>41684.625</v>
+        <v>41704.822916666664</v>
       </c>
       <c s="2" r="C60" t="n">
-        <v>41684.84375</v>
+        <v>41705.197916666664</v>
       </c>
       <c r="D60" t="n">
-        <v>5.25</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E60" t="n">
-        <v>41690.46875</v>
+        <v>41711.833333333336</v>
       </c>
       <c s="2" r="F60" t="n">
-        <v>41690.791666666664</v>
+        <v>41711.947916666664</v>
       </c>
       <c r="G60" t="n">
-        <v>18900000000000</v>
+        <v>32400000000000</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c s="1" r="A61" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c s="2" r="B61" t="n">
-        <v>41685.375</v>
+        <v>41711.520833333336</v>
       </c>
       <c s="2" r="C61" t="n">
-        <v>41685.479166666664</v>
+        <v>41711.635416666664</v>
       </c>
       <c r="D61" t="n">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c s="2" r="E61" t="n">
-        <v>41691.479166666664</v>
+        <v>41712.020833333336</v>
       </c>
       <c s="2" r="F61" t="n">
-        <v>41692.239583333336</v>
+        <v>41712.354166666664</v>
       </c>
       <c r="G61" t="n">
-        <v>9000000000000</v>
+        <v>9900000000000</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c s="1" r="A62" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c s="2" r="B62" t="n">
-        <v>41688.760416666664</v>
+        <v>41711.666666666664</v>
       </c>
       <c s="2" r="C62" t="n">
-        <v>41688.833333333336</v>
+        <v>41711.791666666664</v>
       </c>
       <c r="D62" t="n">
-        <v>1.75</v>
+        <v>3.0</v>
       </c>
       <c s="2" r="E62" t="n">
-        <v>41692.322916666664</v>
+        <v>41735.520833333336</v>
       </c>
       <c s="2" r="F62" t="n">
-        <v>41692.40625</v>
+        <v>41735.989583333336</v>
       </c>
       <c r="G62" t="n">
-        <v>6300000000000</v>
+        <v>10800000000000</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c s="1" r="A63" t="n">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c s="2" r="B63" t="n">
-        <v>41690.46875</v>
+        <v>41711.833333333336</v>
       </c>
       <c s="2" r="C63" t="n">
-        <v>41690.791666666664</v>
+        <v>41711.947916666664</v>
       </c>
       <c r="D63" t="n">
-        <v>7.75</v>
+        <v>2.75</v>
       </c>
       <c s="2" r="E63" t="n">
-        <v>41694.229166666664</v>
+        <v>41737.604166666664</v>
       </c>
       <c s="2" r="F63" t="n">
-        <v>41694.302083333336</v>
+        <v>41737.770833333336</v>
       </c>
       <c r="G63" t="n">
-        <v>27900000000000</v>
+        <v>9900000000000</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c s="1" r="A64" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c s="2" r="B64" t="n">
-        <v>41691.479166666664</v>
+        <v>41712.020833333336</v>
       </c>
       <c s="2" r="C64" t="n">
-        <v>41692.239583333336</v>
+        <v>41712.354166666664</v>
       </c>
       <c r="D64" t="n">
-        <v>18.25</v>
+        <v>8.0</v>
       </c>
       <c s="2" r="E64" t="n">
-        <v>41695.885416666664</v>
+        <v>41738.989583333336</v>
       </c>
       <c s="2" r="F64" t="n">
-        <v>41696.8125</v>
+        <v>41739.15625</v>
       </c>
       <c r="G64" t="n">
-        <v>65700000000000</v>
+        <v>28800000000000</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c s="1" r="A65" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c s="2" r="B65" t="n">
-        <v>41692.322916666664</v>
+        <v>41735.520833333336</v>
       </c>
       <c s="2" r="C65" t="n">
-        <v>41692.40625</v>
+        <v>41735.989583333336</v>
       </c>
       <c r="D65" t="n">
-        <v>2.0</v>
+        <v>11.25</v>
       </c>
       <c s="2" r="E65" t="n">
-        <v>41697.083333333336</v>
+        <v>41747.791666666664</v>
       </c>
       <c s="2" r="F65" t="n">
-        <v>41698.09375</v>
+        <v>41747.979166666664</v>
       </c>
       <c r="G65" t="n">
-        <v>7200000000000</v>
+        <v>40500000000000</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c s="1" r="A66" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c s="2" r="B66" t="n">
-        <v>41694.229166666664</v>
+        <v>41737.604166666664</v>
       </c>
       <c s="2" r="C66" t="n">
-        <v>41694.302083333336</v>
+        <v>41737.770833333336</v>
       </c>
       <c r="D66" t="n">
-        <v>1.75</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E66" t="n">
-        <v>41704.802083333336</v>
+        <v>41748.28125</v>
       </c>
       <c s="2" r="F66" t="n">
-        <v>41705.239583333336</v>
+        <v>41748.9375</v>
       </c>
       <c r="G66" t="n">
-        <v>6300000000000</v>
+        <v>14400000000000</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c s="1" r="A67" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c s="2" r="B67" t="n">
-        <v>41695.885416666664</v>
+        <v>41738.989583333336</v>
       </c>
       <c s="2" r="C67" t="n">
-        <v>41696.8125</v>
+        <v>41739.15625</v>
       </c>
       <c r="D67" t="n">
-        <v>22.25</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E67" t="n">
-        <v>41711.520833333336</v>
+        <v>41748.9375</v>
       </c>
       <c s="2" r="F67" t="n">
-        <v>41711.65625</v>
+        <v>41749.40625</v>
       </c>
       <c r="G67" t="n">
-        <v>80100000000000</v>
+        <v>14400000000000</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c s="1" r="A68" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c s="2" r="B68" t="n">
-        <v>41697.083333333336</v>
+        <v>41747.791666666664</v>
       </c>
       <c s="2" r="C68" t="n">
-        <v>41698.09375</v>
+        <v>41747.979166666664</v>
       </c>
       <c r="D68" t="n">
-        <v>24.25</v>
+        <v>4.5</v>
       </c>
       <c s="2" r="E68" t="n">
-        <v>41711.666666666664</v>
+        <v>41756.489583333336</v>
       </c>
       <c s="2" r="F68" t="n">
-        <v>41712.0</v>
+        <v>41756.822916666664</v>
       </c>
       <c r="G68" t="n">
-        <v>87300000000000</v>
+        <v>16200000000000</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c s="1" r="A69" t="n">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c s="2" r="B69" t="n">
-        <v>41704.802083333336</v>
+        <v>41748.28125</v>
       </c>
       <c s="2" r="C69" t="n">
-        <v>41705.239583333336</v>
+        <v>41749.40625</v>
       </c>
       <c r="D69" t="n">
-        <v>10.5</v>
+        <v>27.0</v>
       </c>
       <c s="2" r="E69" t="n">
-        <v>41712.020833333336</v>
+        <v>41757.385416666664</v>
       </c>
       <c s="2" r="F69" t="n">
-        <v>41712.40625</v>
+        <v>41757.53125</v>
       </c>
       <c r="G69" t="n">
-        <v>37800000000000</v>
+        <v>97200000000000</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c s="1" r="A70" t="n">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c s="2" r="B70" t="n">
-        <v>41711.520833333336</v>
+        <v>41754.65625</v>
       </c>
       <c s="2" r="C70" t="n">
-        <v>41711.65625</v>
+        <v>41754.802083333336</v>
       </c>
       <c r="D70" t="n">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E70" t="n">
-        <v>41712.75</v>
+        <v>41757.885416666664</v>
       </c>
       <c s="2" r="F70" t="n">
-        <v>41712.822916666664</v>
+        <v>41758.5625</v>
       </c>
       <c r="G70" t="n">
-        <v>11700000000000</v>
+        <v>12600000000000</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c s="1" r="A71" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c s="2" r="B71" t="n">
-        <v>41711.666666666664</v>
+        <v>41756.489583333336</v>
       </c>
       <c s="2" r="C71" t="n">
-        <v>41712.0</v>
+        <v>41756.822916666664</v>
       </c>
       <c r="D71" t="n">
         <v>8.0</v>
       </c>
       <c s="2" r="E71" t="n">
-        <v>41730.364583333336</v>
+        <v>41759.489583333336</v>
       </c>
       <c s="2" r="F71" t="n">
-        <v>41730.4375</v>
+        <v>41760.197916666664</v>
       </c>
       <c r="G71" t="n">
         <v>28800000000000</v>
@@ -2045,1111 +2045,1686 @@
     </row>
     <row r="72" spans="1:7">
       <c s="1" r="A72" t="n">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c s="2" r="B72" t="n">
-        <v>41712.020833333336</v>
+        <v>41757.385416666664</v>
       </c>
       <c s="2" r="C72" t="n">
-        <v>41712.40625</v>
+        <v>41757.53125</v>
       </c>
       <c r="D72" t="n">
-        <v>9.25</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E72" t="n">
-        <v>41735.520833333336</v>
+        <v>41778.5625</v>
       </c>
       <c s="2" r="F72" t="n">
-        <v>41736.197916666664</v>
+        <v>41778.677083333336</v>
       </c>
       <c r="G72" t="n">
-        <v>33300000000000</v>
+        <v>12600000000000</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c s="1" r="A73" t="n">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c s="2" r="B73" t="n">
-        <v>41712.75</v>
+        <v>41757.885416666664</v>
       </c>
       <c s="2" r="C73" t="n">
-        <v>41712.822916666664</v>
+        <v>41758.5625</v>
       </c>
       <c r="D73" t="n">
-        <v>1.75</v>
+        <v>16.25</v>
       </c>
       <c s="2" r="E73" t="n">
-        <v>41737.604166666664</v>
+        <v>41779.041666666664</v>
       </c>
       <c s="2" r="F73" t="n">
-        <v>41737.791666666664</v>
+        <v>41779.1875</v>
       </c>
       <c r="G73" t="n">
-        <v>6300000000000</v>
+        <v>58500000000000</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c s="1" r="A74" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c s="2" r="B74" t="n">
-        <v>41730.364583333336</v>
+        <v>41759.489583333336</v>
       </c>
       <c s="2" r="C74" t="n">
-        <v>41730.4375</v>
+        <v>41760.197916666664</v>
       </c>
       <c r="D74" t="n">
-        <v>1.75</v>
+        <v>17.0</v>
       </c>
       <c s="2" r="E74" t="n">
-        <v>41738.979166666664</v>
+        <v>41781.5625</v>
       </c>
       <c s="2" r="F74" t="n">
-        <v>41739.197916666664</v>
+        <v>41782.104166666664</v>
       </c>
       <c r="G74" t="n">
-        <v>6300000000000</v>
+        <v>61200000000000</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c s="1" r="A75" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c s="2" r="B75" t="n">
-        <v>41735.520833333336</v>
+        <v>41778.5625</v>
       </c>
       <c s="2" r="C75" t="n">
-        <v>41736.197916666664</v>
+        <v>41778.677083333336</v>
       </c>
       <c r="D75" t="n">
-        <v>16.25</v>
+        <v>2.75</v>
       </c>
       <c s="2" r="E75" t="n">
-        <v>41740.40625</v>
+        <v>41795.802083333336</v>
       </c>
       <c s="2" r="F75" t="n">
-        <v>41740.5</v>
+        <v>41796.604166666664</v>
       </c>
       <c r="G75" t="n">
-        <v>58500000000000</v>
+        <v>9900000000000</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c s="1" r="A76" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c s="2" r="B76" t="n">
-        <v>41737.604166666664</v>
+        <v>41779.041666666664</v>
       </c>
       <c s="2" r="C76" t="n">
-        <v>41737.791666666664</v>
+        <v>41779.1875</v>
       </c>
       <c r="D76" t="n">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E76" t="n">
-        <v>41746.625</v>
+        <v>41807.072916666664</v>
       </c>
       <c s="2" r="F76" t="n">
-        <v>41746.697916666664</v>
+        <v>41807.354166666664</v>
       </c>
       <c r="G76" t="n">
-        <v>16200000000000</v>
+        <v>12600000000000</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c s="1" r="A77" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c s="2" r="B77" t="n">
-        <v>41738.979166666664</v>
+        <v>41781.5625</v>
       </c>
       <c s="2" r="C77" t="n">
-        <v>41739.197916666664</v>
+        <v>41782.104166666664</v>
       </c>
       <c r="D77" t="n">
-        <v>5.25</v>
+        <v>13.0</v>
       </c>
       <c s="2" r="E77" t="n">
-        <v>41747.78125</v>
+        <v>41823.4375</v>
       </c>
       <c s="2" r="F77" t="n">
-        <v>41748.010416666664</v>
+        <v>41823.8125</v>
       </c>
       <c r="G77" t="n">
-        <v>18900000000000</v>
+        <v>46800000000000</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c s="1" r="A78" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c s="2" r="B78" t="n">
-        <v>41740.40625</v>
+        <v>41795.802083333336</v>
       </c>
       <c s="2" r="C78" t="n">
-        <v>41740.5</v>
+        <v>41796.604166666664</v>
       </c>
       <c r="D78" t="n">
-        <v>2.25</v>
+        <v>19.25</v>
       </c>
       <c s="2" r="E78" t="n">
-        <v>41748.28125</v>
+        <v>41825.25</v>
       </c>
       <c s="2" r="F78" t="n">
-        <v>41749.489583333336</v>
+        <v>41825.729166666664</v>
       </c>
       <c r="G78" t="n">
-        <v>8100000000000</v>
+        <v>69300000000000</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c s="1" r="A79" t="n">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c s="2" r="B79" t="n">
-        <v>41746.625</v>
+        <v>41807.072916666664</v>
       </c>
       <c s="2" r="C79" t="n">
-        <v>41746.697916666664</v>
+        <v>41807.354166666664</v>
       </c>
       <c r="D79" t="n">
-        <v>1.75</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E79" t="n">
-        <v>41754.645833333336</v>
+        <v>41826.84375</v>
       </c>
       <c s="2" r="F79" t="n">
-        <v>41755.020833333336</v>
+        <v>41826.979166666664</v>
       </c>
       <c r="G79" t="n">
-        <v>6300000000000</v>
+        <v>24300000000000</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c s="1" r="A80" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c s="2" r="B80" t="n">
-        <v>41747.78125</v>
+        <v>41823.4375</v>
       </c>
       <c s="2" r="C80" t="n">
-        <v>41748.010416666664</v>
+        <v>41823.8125</v>
       </c>
       <c r="D80" t="n">
-        <v>5.5</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E80" t="n">
-        <v>41755.458333333336</v>
+        <v>41849.25</v>
       </c>
       <c s="2" r="F80" t="n">
-        <v>41755.53125</v>
+        <v>41853.125</v>
       </c>
       <c r="G80" t="n">
-        <v>19800000000000</v>
+        <v>32400000000000</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c s="1" r="A81" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c s="2" r="B81" t="n">
-        <v>41748.28125</v>
+        <v>41825.25</v>
       </c>
       <c s="2" r="C81" t="n">
-        <v>41749.489583333336</v>
+        <v>41825.729166666664</v>
       </c>
       <c r="D81" t="n">
-        <v>29.0</v>
+        <v>11.5</v>
       </c>
       <c s="2" r="E81" t="n">
-        <v>41756.479166666664</v>
+        <v>41853.385416666664</v>
       </c>
       <c s="2" r="F81" t="n">
-        <v>41756.90625</v>
+        <v>41853.458333333336</v>
       </c>
       <c r="G81" t="n">
-        <v>104400000000000</v>
+        <v>41400000000000</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c s="1" r="A82" t="n">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c s="2" r="B82" t="n">
-        <v>41754.645833333336</v>
+        <v>41826.84375</v>
       </c>
       <c s="2" r="C82" t="n">
-        <v>41755.020833333336</v>
+        <v>41826.979166666664</v>
       </c>
       <c r="D82" t="n">
-        <v>9.0</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E82" t="n">
-        <v>41757.385416666664</v>
+        <v>41853.541666666664</v>
       </c>
       <c s="2" r="F82" t="n">
-        <v>41757.583333333336</v>
+        <v>41854.53125</v>
       </c>
       <c r="G82" t="n">
-        <v>32400000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c s="1" r="A83" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c s="2" r="B83" t="n">
-        <v>41755.458333333336</v>
+        <v>41849.25</v>
       </c>
       <c s="2" r="C83" t="n">
-        <v>41755.53125</v>
+        <v>41853.125</v>
       </c>
       <c r="D83" t="n">
-        <v>1.75</v>
+        <v>93.0</v>
       </c>
       <c s="2" r="E83" t="n">
-        <v>41757.885416666664</v>
+        <v>41927.53125</v>
       </c>
       <c s="2" r="F83" t="n">
-        <v>41758.708333333336</v>
+        <v>41927.677083333336</v>
       </c>
       <c r="G83" t="n">
-        <v>6300000000000</v>
+        <v>334800000000000</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c s="1" r="A84" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c s="2" r="B84" t="n">
-        <v>41756.479166666664</v>
+        <v>41853.385416666664</v>
       </c>
       <c s="2" r="C84" t="n">
-        <v>41756.90625</v>
+        <v>41853.458333333336</v>
       </c>
       <c r="D84" t="n">
-        <v>10.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E84" t="n">
-        <v>41758.708333333336</v>
+        <v>41927.739583333336</v>
       </c>
       <c s="2" r="F84" t="n">
-        <v>41758.802083333336</v>
+        <v>41928.041666666664</v>
       </c>
       <c r="G84" t="n">
-        <v>36900000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c s="1" r="A85" t="n">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c s="2" r="B85" t="n">
-        <v>41757.385416666664</v>
+        <v>41853.541666666664</v>
       </c>
       <c s="2" r="C85" t="n">
-        <v>41757.583333333336</v>
+        <v>41854.53125</v>
       </c>
       <c r="D85" t="n">
-        <v>4.75</v>
+        <v>23.75</v>
       </c>
       <c s="2" r="E85" t="n">
-        <v>41758.802083333336</v>
+        <v>41945.15625</v>
       </c>
       <c s="2" r="F85" t="n">
-        <v>41758.9375</v>
+        <v>41945.354166666664</v>
       </c>
       <c r="G85" t="n">
-        <v>17100000000000</v>
+        <v>85500000000000</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c s="1" r="A86" t="n">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c s="2" r="B86" t="n">
-        <v>41757.885416666664</v>
+        <v>41927.53125</v>
       </c>
       <c s="2" r="C86" t="n">
-        <v>41758.9375</v>
+        <v>41927.677083333336</v>
       </c>
       <c r="D86" t="n">
-        <v>25.25</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E86" t="n">
-        <v>41779.041666666664</v>
+        <v>41946.71875</v>
       </c>
       <c s="2" r="F86" t="n">
-        <v>41779.208333333336</v>
+        <v>41947.114583333336</v>
       </c>
       <c r="G86" t="n">
-        <v>90900000000000</v>
+        <v>12600000000000</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c s="1" r="A87" t="n">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c s="2" r="B87" t="n">
-        <v>41759.489583333336</v>
+        <v>41927.739583333336</v>
       </c>
       <c s="2" r="C87" t="n">
-        <v>41760.333333333336</v>
+        <v>41928.041666666664</v>
       </c>
       <c r="D87" t="n">
-        <v>20.25</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E87" t="n">
-        <v>41781.5625</v>
+        <v>41955.395833333336</v>
       </c>
       <c s="2" r="F87" t="n">
-        <v>41782.177083333336</v>
+        <v>41955.479166666664</v>
       </c>
       <c r="G87" t="n">
-        <v>72900000000000</v>
+        <v>26100000000000</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c s="1" r="A88" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c s="2" r="B88" t="n">
-        <v>41778.5625</v>
+        <v>41945.15625</v>
       </c>
       <c s="2" r="C88" t="n">
-        <v>41778.697916666664</v>
+        <v>41945.354166666664</v>
       </c>
       <c r="D88" t="n">
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E88" t="n">
-        <v>41782.333333333336</v>
+        <v>41955.729166666664</v>
       </c>
       <c s="2" r="F88" t="n">
-        <v>41782.53125</v>
+        <v>41955.979166666664</v>
       </c>
       <c r="G88" t="n">
-        <v>11700000000000</v>
+        <v>17100000000000</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c s="1" r="A89" t="n">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c s="2" r="B89" t="n">
-        <v>41779.041666666664</v>
+        <v>41946.71875</v>
       </c>
       <c s="2" r="C89" t="n">
-        <v>41779.208333333336</v>
+        <v>41947.114583333336</v>
       </c>
       <c r="D89" t="n">
-        <v>4.0</v>
+        <v>9.5</v>
       </c>
       <c s="2" r="E89" t="n">
-        <v>41782.979166666664</v>
+        <v>41959.0</v>
       </c>
       <c s="2" r="F89" t="n">
-        <v>41783.25</v>
+        <v>41959.520833333336</v>
       </c>
       <c r="G89" t="n">
-        <v>14400000000000</v>
+        <v>34200000000000</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c s="1" r="A90" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c s="2" r="B90" t="n">
-        <v>41781.5625</v>
+        <v>41955.395833333336</v>
       </c>
       <c s="2" r="C90" t="n">
-        <v>41782.177083333336</v>
+        <v>41955.479166666664</v>
       </c>
       <c r="D90" t="n">
-        <v>14.75</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E90" t="n">
-        <v>41783.375</v>
+        <v>41961.770833333336</v>
       </c>
       <c s="2" r="F90" t="n">
-        <v>41783.447916666664</v>
+        <v>41962.020833333336</v>
       </c>
       <c r="G90" t="n">
-        <v>53100000000000</v>
+        <v>7200000000000</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c s="1" r="A91" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c s="2" r="B91" t="n">
-        <v>41782.333333333336</v>
+        <v>41955.729166666664</v>
       </c>
       <c s="2" r="C91" t="n">
-        <v>41782.53125</v>
+        <v>41955.979166666664</v>
       </c>
       <c r="D91" t="n">
-        <v>4.75</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E91" t="n">
-        <v>41788.59375</v>
+        <v>41962.822916666664</v>
       </c>
       <c s="2" r="F91" t="n">
-        <v>41788.729166666664</v>
+        <v>41962.96875</v>
       </c>
       <c r="G91" t="n">
-        <v>17100000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c s="1" r="A92" t="n">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c s="2" r="B92" t="n">
-        <v>41782.979166666664</v>
+        <v>41959.0</v>
       </c>
       <c s="2" r="C92" t="n">
-        <v>41783.25</v>
+        <v>41959.520833333336</v>
       </c>
       <c r="D92" t="n">
-        <v>6.5</v>
+        <v>12.5</v>
       </c>
       <c s="2" r="E92" t="n">
-        <v>41795.791666666664</v>
+        <v>41965.8125</v>
       </c>
       <c s="2" r="F92" t="n">
-        <v>41796.645833333336</v>
+        <v>41966.6875</v>
       </c>
       <c r="G92" t="n">
-        <v>23400000000000</v>
+        <v>45000000000000</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c s="1" r="A93" t="n">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c s="2" r="B93" t="n">
-        <v>41783.375</v>
+        <v>41961.770833333336</v>
       </c>
       <c s="2" r="C93" t="n">
-        <v>41783.447916666664</v>
+        <v>41962.020833333336</v>
       </c>
       <c r="D93" t="n">
-        <v>1.75</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E93" t="n">
-        <v>41807.041666666664</v>
+        <v>41967.90625</v>
       </c>
       <c s="2" r="F93" t="n">
-        <v>41807.40625</v>
+        <v>41968.145833333336</v>
       </c>
       <c r="G93" t="n">
-        <v>6300000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c s="1" r="A94" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c s="2" r="B94" t="n">
-        <v>41788.59375</v>
+        <v>41962.822916666664</v>
       </c>
       <c s="2" r="C94" t="n">
-        <v>41788.729166666664</v>
+        <v>41962.96875</v>
       </c>
       <c r="D94" t="n">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E94" t="n">
-        <v>41823.4375</v>
+        <v>41977.84375</v>
       </c>
       <c s="2" r="F94" t="n">
-        <v>41823.833333333336</v>
+        <v>41978.666666666664</v>
       </c>
       <c r="G94" t="n">
-        <v>11700000000000</v>
+        <v>12600000000000</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c s="1" r="A95" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c s="2" r="B95" t="n">
-        <v>41795.791666666664</v>
+        <v>41965.8125</v>
       </c>
       <c s="2" r="C95" t="n">
-        <v>41796.645833333336</v>
+        <v>41966.6875</v>
       </c>
       <c r="D95" t="n">
-        <v>20.5</v>
+        <v>21.0</v>
       </c>
       <c s="2" r="E95" t="n">
-        <v>41825.25</v>
+        <v>41982.427083333336</v>
       </c>
       <c s="2" r="F95" t="n">
-        <v>41825.760416666664</v>
+        <v>41982.927083333336</v>
       </c>
       <c r="G95" t="n">
-        <v>73800000000000</v>
+        <v>75600000000000</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c s="1" r="A96" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c s="2" r="B96" t="n">
-        <v>41807.041666666664</v>
+        <v>41967.90625</v>
       </c>
       <c s="2" r="C96" t="n">
-        <v>41807.40625</v>
+        <v>41968.145833333336</v>
       </c>
       <c r="D96" t="n">
-        <v>8.75</v>
+        <v>5.75</v>
       </c>
       <c s="2" r="E96" t="n">
-        <v>41826.84375</v>
+        <v>41992.020833333336</v>
       </c>
       <c s="2" r="F96" t="n">
-        <v>41827.0</v>
+        <v>41992.59375</v>
       </c>
       <c r="G96" t="n">
-        <v>31500000000000</v>
+        <v>20700000000000</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c s="1" r="A97" t="n">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c s="2" r="B97" t="n">
-        <v>41823.4375</v>
+        <v>41977.84375</v>
       </c>
       <c s="2" r="C97" t="n">
-        <v>41823.833333333336</v>
+        <v>41978.666666666664</v>
       </c>
       <c r="D97" t="n">
-        <v>9.5</v>
+        <v>19.75</v>
       </c>
       <c s="2" r="E97" t="n">
-        <v>41849.25</v>
+        <v>41992.614583333336</v>
       </c>
       <c s="2" r="F97" t="n">
-        <v>41853.364583333336</v>
+        <v>41992.833333333336</v>
       </c>
       <c r="G97" t="n">
-        <v>34200000000000</v>
+        <v>71100000000000</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c s="1" r="A98" t="n">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c s="2" r="B98" t="n">
-        <v>41825.25</v>
+        <v>41982.427083333336</v>
       </c>
       <c s="2" r="C98" t="n">
-        <v>41825.760416666664</v>
+        <v>41982.927083333336</v>
       </c>
       <c r="D98" t="n">
-        <v>12.25</v>
+        <v>12.0</v>
       </c>
       <c s="2" r="E98" t="n">
-        <v>41853.364583333336</v>
+        <v>41994.020833333336</v>
       </c>
       <c s="2" r="F98" t="n">
-        <v>41854.6875</v>
+        <v>41994.385416666664</v>
       </c>
       <c r="G98" t="n">
-        <v>44100000000000</v>
+        <v>43200000000000</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c s="1" r="A99" t="n">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c s="2" r="B99" t="n">
-        <v>41826.84375</v>
+        <v>41992.020833333336</v>
       </c>
       <c s="2" r="C99" t="n">
-        <v>41827.0</v>
+        <v>41992.59375</v>
       </c>
       <c r="D99" t="n">
-        <v>3.75</v>
+        <v>13.75</v>
       </c>
       <c s="2" r="E99" t="n">
-        <v>41927.739583333336</v>
+        <v>41994.40625</v>
       </c>
       <c s="2" r="F99" t="n">
-        <v>41928.083333333336</v>
+        <v>41996.020833333336</v>
       </c>
       <c r="G99" t="n">
-        <v>13500000000000</v>
+        <v>49500000000000</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c s="1" r="A100" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c s="2" r="B100" t="n">
-        <v>41849.25</v>
+        <v>41992.614583333336</v>
       </c>
       <c s="2" r="C100" t="n">
-        <v>41854.6875</v>
+        <v>41992.833333333336</v>
       </c>
       <c r="D100" t="n">
-        <v>130.5</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E100" t="n">
-        <v>41945.145833333336</v>
+        <v>42005.354166666664</v>
       </c>
       <c s="2" r="F100" t="n">
-        <v>41945.364583333336</v>
+        <v>42005.854166666664</v>
       </c>
       <c r="G100" t="n">
-        <v>469800000000000</v>
+        <v>18900000000000</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c s="1" r="A101" t="n">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c s="2" r="B101" t="n">
-        <v>41927.53125</v>
+        <v>41994.020833333336</v>
       </c>
       <c s="2" r="C101" t="n">
-        <v>41927.6875</v>
+        <v>41994.385416666664</v>
       </c>
       <c r="D101" t="n">
-        <v>3.75</v>
+        <v>8.75</v>
       </c>
       <c s="2" r="E101" t="n">
-        <v>41946.71875</v>
+        <v>42006.5625</v>
       </c>
       <c s="2" r="F101" t="n">
-        <v>41947.15625</v>
+        <v>42006.791666666664</v>
       </c>
       <c r="G101" t="n">
-        <v>13500000000000</v>
+        <v>31500000000000</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c s="1" r="A102" t="n">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c s="2" r="B102" t="n">
-        <v>41927.739583333336</v>
+        <v>41994.40625</v>
       </c>
       <c s="2" r="C102" t="n">
-        <v>41928.083333333336</v>
+        <v>41996.020833333336</v>
       </c>
       <c r="D102" t="n">
-        <v>8.25</v>
+        <v>38.75</v>
       </c>
       <c s="2" r="E102" t="n">
-        <v>41955.395833333336</v>
+        <v>42008.8125</v>
       </c>
       <c s="2" r="F102" t="n">
-        <v>41955.489583333336</v>
+        <v>42008.916666666664</v>
       </c>
       <c r="G102" t="n">
-        <v>29700000000000</v>
+        <v>139500000000000</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c s="1" r="A103" t="n">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c s="2" r="B103" t="n">
-        <v>41945.145833333336</v>
+        <v>42005.354166666664</v>
       </c>
       <c s="2" r="C103" t="n">
-        <v>41945.364583333336</v>
+        <v>42005.854166666664</v>
       </c>
       <c r="D103" t="n">
-        <v>5.25</v>
+        <v>12.0</v>
       </c>
       <c s="2" r="E103" t="n">
-        <v>41955.71875</v>
+        <v>42009.135416666664</v>
       </c>
       <c s="2" r="F103" t="n">
-        <v>41956.020833333336</v>
+        <v>42009.3125</v>
       </c>
       <c r="G103" t="n">
-        <v>18900000000000</v>
+        <v>43200000000000</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c s="1" r="A104" t="n">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c s="2" r="B104" t="n">
-        <v>41946.71875</v>
+        <v>42006.5625</v>
       </c>
       <c s="2" r="C104" t="n">
-        <v>41947.15625</v>
+        <v>42006.791666666664</v>
       </c>
       <c r="D104" t="n">
-        <v>10.5</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E104" t="n">
-        <v>41959.0</v>
+        <v>42013.489583333336</v>
       </c>
       <c s="2" r="F104" t="n">
-        <v>41959.572916666664</v>
+        <v>42014.375</v>
       </c>
       <c r="G104" t="n">
-        <v>37800000000000</v>
+        <v>19800000000000</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c s="1" r="A105" t="n">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c s="2" r="B105" t="n">
-        <v>41955.395833333336</v>
+        <v>42008.8125</v>
       </c>
       <c s="2" r="C105" t="n">
-        <v>41955.489583333336</v>
+        <v>42008.916666666664</v>
       </c>
       <c r="D105" t="n">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c s="2" r="E105" t="n">
-        <v>41961.770833333336</v>
+        <v>42024.416666666664</v>
       </c>
       <c s="2" r="F105" t="n">
-        <v>41962.072916666664</v>
+        <v>42024.916666666664</v>
       </c>
       <c r="G105" t="n">
-        <v>8100000000000</v>
+        <v>9000000000000</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c s="1" r="A106" t="n">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c s="2" r="B106" t="n">
-        <v>41955.71875</v>
+        <v>42009.135416666664</v>
       </c>
       <c s="2" r="C106" t="n">
-        <v>41956.020833333336</v>
+        <v>42009.3125</v>
       </c>
       <c r="D106" t="n">
-        <v>7.25</v>
+        <v>4.25</v>
       </c>
       <c s="2" r="E106" t="n">
-        <v>41962.791666666664</v>
+        <v>42025.21875</v>
       </c>
       <c s="2" r="F106" t="n">
-        <v>41963.041666666664</v>
+        <v>42026.010416666664</v>
       </c>
       <c r="G106" t="n">
-        <v>26100000000000</v>
+        <v>15300000000000</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c s="1" r="A107" t="n">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c s="2" r="B107" t="n">
-        <v>41959.0</v>
+        <v>42013.489583333336</v>
       </c>
       <c s="2" r="C107" t="n">
-        <v>41959.572916666664</v>
+        <v>42014.375</v>
       </c>
       <c r="D107" t="n">
-        <v>13.75</v>
+        <v>21.25</v>
       </c>
       <c s="2" r="E107" t="n">
-        <v>41965.8125</v>
+        <v>42031.09375</v>
       </c>
       <c s="2" r="F107" t="n">
-        <v>41966.729166666664</v>
+        <v>42031.302083333336</v>
       </c>
       <c r="G107" t="n">
-        <v>49500000000000</v>
+        <v>76500000000000</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c s="1" r="A108" t="n">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c s="2" r="B108" t="n">
-        <v>41961.770833333336</v>
+        <v>42024.416666666664</v>
       </c>
       <c s="2" r="C108" t="n">
-        <v>41962.072916666664</v>
+        <v>42024.916666666664</v>
       </c>
       <c r="D108" t="n">
-        <v>7.25</v>
+        <v>12.0</v>
       </c>
       <c s="2" r="E108" t="n">
-        <v>41967.885416666664</v>
+        <v>42033.65625</v>
       </c>
       <c s="2" r="F108" t="n">
-        <v>41968.1875</v>
+        <v>42034.9375</v>
       </c>
       <c r="G108" t="n">
-        <v>26100000000000</v>
+        <v>43200000000000</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c s="1" r="A109" t="n">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c s="2" r="B109" t="n">
-        <v>41962.791666666664</v>
+        <v>42025.21875</v>
       </c>
       <c s="2" r="C109" t="n">
-        <v>41963.041666666664</v>
+        <v>42026.010416666664</v>
       </c>
       <c r="D109" t="n">
-        <v>6.0</v>
+        <v>19.0</v>
       </c>
       <c s="2" r="E109" t="n">
-        <v>41977.84375</v>
+        <v>42034.96875</v>
       </c>
       <c s="2" r="F109" t="n">
-        <v>41978.697916666664</v>
+        <v>42035.416666666664</v>
       </c>
       <c r="G109" t="n">
-        <v>21600000000000</v>
+        <v>68400000000000</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c s="1" r="A110" t="n">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c s="2" r="B110" t="n">
-        <v>41965.8125</v>
+        <v>42031.09375</v>
       </c>
       <c s="2" r="C110" t="n">
-        <v>41966.729166666664</v>
+        <v>42031.302083333336</v>
       </c>
       <c r="D110" t="n">
-        <v>22.0</v>
+        <v>5.0</v>
       </c>
       <c s="2" r="E110" t="n">
-        <v>41982.427083333336</v>
+        <v>42035.520833333336</v>
       </c>
       <c s="2" r="F110" t="n">
-        <v>41983.03125</v>
+        <v>42036.770833333336</v>
       </c>
       <c r="G110" t="n">
-        <v>79200000000000</v>
+        <v>18000000000000</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c s="1" r="A111" t="n">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c s="2" r="B111" t="n">
-        <v>41967.885416666664</v>
+        <v>42033.65625</v>
       </c>
       <c s="2" r="C111" t="n">
-        <v>41968.1875</v>
+        <v>42034.9375</v>
       </c>
       <c r="D111" t="n">
-        <v>7.25</v>
+        <v>30.75</v>
       </c>
       <c s="2" r="E111" t="n">
-        <v>41992.010416666664</v>
+        <v>42036.770833333336</v>
       </c>
       <c s="2" r="F111" t="n">
-        <v>41992.885416666664</v>
+        <v>42036.864583333336</v>
       </c>
       <c r="G111" t="n">
-        <v>26100000000000</v>
+        <v>110700000000000</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c s="1" r="A112" t="n">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c s="2" r="B112" t="n">
-        <v>41977.84375</v>
+        <v>42034.96875</v>
       </c>
       <c s="2" r="C112" t="n">
-        <v>41978.697916666664</v>
+        <v>42035.416666666664</v>
       </c>
       <c r="D112" t="n">
-        <v>20.5</v>
+        <v>10.75</v>
       </c>
       <c s="2" r="E112" t="n">
-        <v>41994.020833333336</v>
+        <v>42043.395833333336</v>
       </c>
       <c s="2" r="F112" t="n">
-        <v>41996.09375</v>
+        <v>42043.9375</v>
       </c>
       <c r="G112" t="n">
-        <v>73800000000000</v>
+        <v>38700000000000</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c s="1" r="A113" t="n">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c s="2" r="B113" t="n">
-        <v>41982.427083333336</v>
+        <v>42035.520833333336</v>
       </c>
       <c s="2" r="C113" t="n">
-        <v>41983.03125</v>
+        <v>42036.864583333336</v>
       </c>
       <c r="D113" t="n">
-        <v>14.5</v>
+        <v>32.25</v>
       </c>
       <c s="2" r="E113" t="n">
-        <v>42005.354166666664</v>
+        <v>42044.9375</v>
       </c>
       <c s="2" r="F113" t="n">
-        <v>42005.895833333336</v>
+        <v>42045.697916666664</v>
       </c>
       <c r="G113" t="n">
-        <v>52200000000000</v>
+        <v>116100000000000</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c s="1" r="A114" t="n">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c s="2" r="B114" t="n">
-        <v>41992.010416666664</v>
+        <v>42040.53125</v>
       </c>
       <c s="2" r="C114" t="n">
-        <v>41992.885416666664</v>
+        <v>42040.791666666664</v>
       </c>
       <c r="D114" t="n">
-        <v>21.0</v>
+        <v>6.25</v>
       </c>
       <c s="2" r="E114" t="n">
-        <v>42006.5625</v>
+        <v>42051.15625</v>
       </c>
       <c s="2" r="F114" t="n">
-        <v>42006.854166666664</v>
+        <v>42051.239583333336</v>
       </c>
       <c r="G114" t="n">
-        <v>75600000000000</v>
+        <v>22500000000000</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c s="1" r="A115" t="n">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c s="2" r="B115" t="n">
-        <v>41994.020833333336</v>
+        <v>42043.395833333336</v>
       </c>
       <c s="2" r="C115" t="n">
-        <v>41996.09375</v>
+        <v>42043.9375</v>
       </c>
       <c r="D115" t="n">
-        <v>49.75</v>
+        <v>13.0</v>
       </c>
       <c s="2" r="E115" t="n">
-        <v>42008.8125</v>
+        <v>42051.270833333336</v>
       </c>
       <c s="2" r="F115" t="n">
-        <v>42008.947916666664</v>
+        <v>42051.604166666664</v>
       </c>
       <c r="G115" t="n">
-        <v>179100000000000</v>
+        <v>46800000000000</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c s="1" r="A116" t="n">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c s="2" r="B116" t="n">
-        <v>42005.354166666664</v>
+        <v>42044.9375</v>
       </c>
       <c s="2" r="C116" t="n">
-        <v>42005.895833333336</v>
+        <v>42045.697916666664</v>
       </c>
       <c r="D116" t="n">
-        <v>13.0</v>
+        <v>18.25</v>
       </c>
       <c s="2" r="E116" t="n">
-        <v>42009.125</v>
+        <v>42051.6875</v>
       </c>
       <c s="2" r="F116" t="n">
-        <v>42009.364583333336</v>
+        <v>42051.78125</v>
       </c>
       <c r="G116" t="n">
-        <v>46800000000000</v>
+        <v>65700000000000</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c s="1" r="A117" t="n">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c s="2" r="B117" t="n">
-        <v>42006.5625</v>
+        <v>42051.15625</v>
       </c>
       <c s="2" r="C117" t="n">
-        <v>42006.854166666664</v>
+        <v>42051.239583333336</v>
       </c>
       <c r="D117" t="n">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E117" t="n">
-        <v>42013.489583333336</v>
+        <v>42052.125</v>
       </c>
       <c s="2" r="F117" t="n">
-        <v>42014.375</v>
+        <v>42052.21875</v>
       </c>
       <c r="G117" t="n">
-        <v>25200000000000</v>
+        <v>7200000000000</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c s="1" r="A118" t="n">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c s="2" r="B118" t="n">
-        <v>42008.8125</v>
+        <v>42051.270833333336</v>
       </c>
       <c s="2" r="C118" t="n">
-        <v>42008.947916666664</v>
+        <v>42051.604166666664</v>
       </c>
       <c r="D118" t="n">
-        <v>3.25</v>
+        <v>8.0</v>
+      </c>
+      <c s="2" r="E118" t="n">
+        <v>42056.75</v>
+      </c>
+      <c s="2" r="F118" t="n">
+        <v>42056.895833333336</v>
       </c>
       <c r="G118" t="n">
-        <v>11700000000000</v>
+        <v>28800000000000</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c s="1" r="A119" t="n">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c s="2" r="B119" t="n">
-        <v>42009.125</v>
+        <v>42051.6875</v>
       </c>
       <c s="2" r="C119" t="n">
-        <v>42009.364583333336</v>
+        <v>42051.78125</v>
       </c>
       <c r="D119" t="n">
-        <v>5.75</v>
+        <v>2.25</v>
+      </c>
+      <c s="2" r="E119" t="n">
+        <v>42057.052083333336</v>
+      </c>
+      <c s="2" r="F119" t="n">
+        <v>42057.677083333336</v>
       </c>
       <c r="G119" t="n">
-        <v>20700000000000</v>
+        <v>8100000000000</v>
       </c>
     </row>
     <row r="120" spans="1:7">
       <c s="1" r="A120" t="n">
+        <v>121</v>
+      </c>
+      <c s="2" r="B120" t="n">
+        <v>42052.125</v>
+      </c>
+      <c s="2" r="C120" t="n">
+        <v>42052.21875</v>
+      </c>
+      <c r="D120" t="n">
+        <v>2.25</v>
+      </c>
+      <c s="2" r="E120" t="n">
+        <v>42079.916666666664</v>
+      </c>
+      <c s="2" r="F120" t="n">
+        <v>42080.229166666664</v>
+      </c>
+      <c r="G120" t="n">
+        <v>8100000000000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c s="1" r="A121" t="n">
+        <v>122</v>
+      </c>
+      <c s="2" r="B121" t="n">
+        <v>42056.75</v>
+      </c>
+      <c s="2" r="C121" t="n">
+        <v>42056.895833333336</v>
+      </c>
+      <c r="D121" t="n">
+        <v>3.5</v>
+      </c>
+      <c s="2" r="E121" t="n">
+        <v>42085.4375</v>
+      </c>
+      <c s="2" r="F121" t="n">
+        <v>42085.645833333336</v>
+      </c>
+      <c r="G121" t="n">
+        <v>12600000000000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c s="1" r="A122" t="n">
+        <v>123</v>
+      </c>
+      <c s="2" r="B122" t="n">
+        <v>42057.052083333336</v>
+      </c>
+      <c s="2" r="C122" t="n">
+        <v>42057.677083333336</v>
+      </c>
+      <c r="D122" t="n">
+        <v>15.0</v>
+      </c>
+      <c s="2" r="E122" t="n">
+        <v>42087.0</v>
+      </c>
+      <c s="2" r="F122" t="n">
+        <v>42087.177083333336</v>
+      </c>
+      <c r="G122" t="n">
+        <v>54000000000000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c s="1" r="A123" t="n">
+        <v>124</v>
+      </c>
+      <c s="2" r="B123" t="n">
+        <v>42079.916666666664</v>
+      </c>
+      <c s="2" r="C123" t="n">
+        <v>42080.229166666664</v>
+      </c>
+      <c r="D123" t="n">
+        <v>7.5</v>
+      </c>
+      <c s="2" r="E123" t="n">
+        <v>42088.5</v>
+      </c>
+      <c s="2" r="F123" t="n">
+        <v>42089.083333333336</v>
+      </c>
+      <c r="G123" t="n">
+        <v>27000000000000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c s="1" r="A124" t="n">
+        <v>125</v>
+      </c>
+      <c s="2" r="B124" t="n">
+        <v>42085.4375</v>
+      </c>
+      <c s="2" r="C124" t="n">
+        <v>42085.645833333336</v>
+      </c>
+      <c r="D124" t="n">
+        <v>5.0</v>
+      </c>
+      <c s="2" r="E124" t="n">
+        <v>42089.739583333336</v>
+      </c>
+      <c s="2" r="F124" t="n">
+        <v>42090.145833333336</v>
+      </c>
+      <c r="G124" t="n">
+        <v>18000000000000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c s="1" r="A125" t="n">
         <v>126</v>
       </c>
-      <c s="2" r="B120" t="n">
-        <v>42013.489583333336</v>
-      </c>
-      <c s="2" r="C120" t="n">
-        <v>42014.375</v>
-      </c>
-      <c r="D120" t="n">
-        <v>21.25</v>
-      </c>
-      <c r="G120" t="n">
-        <v>76500000000000</v>
+      <c s="2" r="B125" t="n">
+        <v>42087.0</v>
+      </c>
+      <c s="2" r="C125" t="n">
+        <v>42087.177083333336</v>
+      </c>
+      <c r="D125" t="n">
+        <v>4.25</v>
+      </c>
+      <c s="2" r="E125" t="n">
+        <v>42092.96875</v>
+      </c>
+      <c s="2" r="F125" t="n">
+        <v>42093.083333333336</v>
+      </c>
+      <c r="G125" t="n">
+        <v>15300000000000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c s="1" r="A126" t="n">
+        <v>127</v>
+      </c>
+      <c s="2" r="B126" t="n">
+        <v>42088.5</v>
+      </c>
+      <c s="2" r="C126" t="n">
+        <v>42089.083333333336</v>
+      </c>
+      <c r="D126" t="n">
+        <v>14.0</v>
+      </c>
+      <c s="2" r="E126" t="n">
+        <v>42095.489583333336</v>
+      </c>
+      <c s="2" r="F126" t="n">
+        <v>42095.822916666664</v>
+      </c>
+      <c r="G126" t="n">
+        <v>50400000000000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c s="1" r="A127" t="n">
+        <v>128</v>
+      </c>
+      <c s="2" r="B127" t="n">
+        <v>42089.739583333336</v>
+      </c>
+      <c s="2" r="C127" t="n">
+        <v>42090.145833333336</v>
+      </c>
+      <c r="D127" t="n">
+        <v>9.75</v>
+      </c>
+      <c s="2" r="E127" t="n">
+        <v>42096.729166666664</v>
+      </c>
+      <c s="2" r="F127" t="n">
+        <v>42097.260416666664</v>
+      </c>
+      <c r="G127" t="n">
+        <v>35100000000000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c s="1" r="A128" t="n">
+        <v>129</v>
+      </c>
+      <c s="2" r="B128" t="n">
+        <v>42092.96875</v>
+      </c>
+      <c s="2" r="C128" t="n">
+        <v>42093.083333333336</v>
+      </c>
+      <c r="D128" t="n">
+        <v>2.75</v>
+      </c>
+      <c s="2" r="E128" t="n">
+        <v>42097.260416666664</v>
+      </c>
+      <c s="2" r="F128" t="n">
+        <v>42097.333333333336</v>
+      </c>
+      <c r="G128" t="n">
+        <v>9900000000000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c s="1" r="A129" t="n">
+        <v>130</v>
+      </c>
+      <c s="2" r="B129" t="n">
+        <v>42095.489583333336</v>
+      </c>
+      <c s="2" r="C129" t="n">
+        <v>42095.822916666664</v>
+      </c>
+      <c r="D129" t="n">
+        <v>8.0</v>
+      </c>
+      <c s="2" r="E129" t="n">
+        <v>42116.739583333336</v>
+      </c>
+      <c s="2" r="F129" t="n">
+        <v>42117.697916666664</v>
+      </c>
+      <c r="G129" t="n">
+        <v>28800000000000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c s="1" r="A130" t="n">
+        <v>131</v>
+      </c>
+      <c s="2" r="B130" t="n">
+        <v>42096.729166666664</v>
+      </c>
+      <c s="2" r="C130" t="n">
+        <v>42097.333333333336</v>
+      </c>
+      <c r="D130" t="n">
+        <v>14.5</v>
+      </c>
+      <c s="2" r="E130" t="n">
+        <v>42118.510416666664</v>
+      </c>
+      <c s="2" r="F130" t="n">
+        <v>42118.645833333336</v>
+      </c>
+      <c r="G130" t="n">
+        <v>52200000000000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c s="1" r="A131" t="n">
+        <v>133</v>
+      </c>
+      <c s="2" r="B131" t="n">
+        <v>42112.458333333336</v>
+      </c>
+      <c s="2" r="C131" t="n">
+        <v>42112.875</v>
+      </c>
+      <c r="D131" t="n">
+        <v>10.0</v>
+      </c>
+      <c s="2" r="E131" t="n">
+        <v>42128.0</v>
+      </c>
+      <c s="2" r="F131" t="n">
+        <v>42128.59375</v>
+      </c>
+      <c r="G131" t="n">
+        <v>36000000000000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c s="1" r="A132" t="n">
+        <v>134</v>
+      </c>
+      <c s="2" r="B132" t="n">
+        <v>42116.739583333336</v>
+      </c>
+      <c s="2" r="C132" t="n">
+        <v>42117.697916666664</v>
+      </c>
+      <c r="D132" t="n">
+        <v>23.0</v>
+      </c>
+      <c s="2" r="E132" t="n">
+        <v>42130.541666666664</v>
+      </c>
+      <c s="2" r="F132" t="n">
+        <v>42130.791666666664</v>
+      </c>
+      <c r="G132" t="n">
+        <v>82800000000000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c s="1" r="A133" t="n">
+        <v>135</v>
+      </c>
+      <c s="2" r="B133" t="n">
+        <v>42118.510416666664</v>
+      </c>
+      <c s="2" r="C133" t="n">
+        <v>42118.645833333336</v>
+      </c>
+      <c r="D133" t="n">
+        <v>3.25</v>
+      </c>
+      <c s="2" r="E133" t="n">
+        <v>42130.875</v>
+      </c>
+      <c s="2" r="F133" t="n">
+        <v>42131.489583333336</v>
+      </c>
+      <c r="G133" t="n">
+        <v>11700000000000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c s="1" r="A134" t="n">
+        <v>136</v>
+      </c>
+      <c s="2" r="B134" t="n">
+        <v>42128.0</v>
+      </c>
+      <c s="2" r="C134" t="n">
+        <v>42128.59375</v>
+      </c>
+      <c r="D134" t="n">
+        <v>14.25</v>
+      </c>
+      <c s="2" r="E134" t="n">
+        <v>42131.489583333336</v>
+      </c>
+      <c s="2" r="F134" t="n">
+        <v>42132.416666666664</v>
+      </c>
+      <c r="G134" t="n">
+        <v>51300000000000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c s="1" r="A135" t="n">
+        <v>137</v>
+      </c>
+      <c s="2" r="B135" t="n">
+        <v>42130.541666666664</v>
+      </c>
+      <c s="2" r="C135" t="n">
+        <v>42130.791666666664</v>
+      </c>
+      <c r="D135" t="n">
+        <v>6.0</v>
+      </c>
+      <c s="2" r="E135" t="n">
+        <v>42139.697916666664</v>
+      </c>
+      <c s="2" r="F135" t="n">
+        <v>42139.864583333336</v>
+      </c>
+      <c r="G135" t="n">
+        <v>21600000000000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c s="1" r="A136" t="n">
+        <v>138</v>
+      </c>
+      <c s="2" r="B136" t="n">
+        <v>42130.875</v>
+      </c>
+      <c s="2" r="C136" t="n">
+        <v>42132.416666666664</v>
+      </c>
+      <c r="D136" t="n">
+        <v>37.0</v>
+      </c>
+      <c s="2" r="E136" t="n">
+        <v>42140.979166666664</v>
+      </c>
+      <c s="2" r="F136" t="n">
+        <v>42142.177083333336</v>
+      </c>
+      <c r="G136" t="n">
+        <v>133200000000000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c s="1" r="A137" t="n">
+        <v>140</v>
+      </c>
+      <c s="2" r="B137" t="n">
+        <v>42135.989583333336</v>
+      </c>
+      <c s="2" r="C137" t="n">
+        <v>42136.177083333336</v>
+      </c>
+      <c r="D137" t="n">
+        <v>4.5</v>
+      </c>
+      <c s="2" r="E137" t="n">
+        <v>42145.9375</v>
+      </c>
+      <c s="2" r="F137" t="n">
+        <v>42148.0625</v>
+      </c>
+      <c r="G137" t="n">
+        <v>16200000000000</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c s="1" r="A138" t="n">
+        <v>141</v>
+      </c>
+      <c s="2" r="B138" t="n">
+        <v>42139.697916666664</v>
+      </c>
+      <c s="2" r="C138" t="n">
+        <v>42139.864583333336</v>
+      </c>
+      <c r="D138" t="n">
+        <v>4.0</v>
+      </c>
+      <c s="2" r="E138" t="n">
+        <v>42148.604166666664</v>
+      </c>
+      <c s="2" r="F138" t="n">
+        <v>42149.21875</v>
+      </c>
+      <c r="G138" t="n">
+        <v>14400000000000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c s="1" r="A139" t="n">
+        <v>142</v>
+      </c>
+      <c s="2" r="B139" t="n">
+        <v>42140.979166666664</v>
+      </c>
+      <c s="2" r="C139" t="n">
+        <v>42142.177083333336</v>
+      </c>
+      <c r="D139" t="n">
+        <v>28.75</v>
+      </c>
+      <c s="2" r="E139" t="n">
+        <v>42149.541666666664</v>
+      </c>
+      <c s="2" r="F139" t="n">
+        <v>42150.104166666664</v>
+      </c>
+      <c r="G139" t="n">
+        <v>103500000000000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c s="1" r="A140" t="n">
+        <v>143</v>
+      </c>
+      <c s="2" r="B140" t="n">
+        <v>42145.9375</v>
+      </c>
+      <c s="2" r="C140" t="n">
+        <v>42148.0625</v>
+      </c>
+      <c r="D140" t="n">
+        <v>51.0</v>
+      </c>
+      <c s="2" r="E140" t="n">
+        <v>42167.375</v>
+      </c>
+      <c s="2" r="F140" t="n">
+        <v>42169.177083333336</v>
+      </c>
+      <c r="G140" t="n">
+        <v>183600000000000</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c s="1" r="A141" t="n">
+        <v>144</v>
+      </c>
+      <c s="2" r="B141" t="n">
+        <v>42148.604166666664</v>
+      </c>
+      <c s="2" r="C141" t="n">
+        <v>42149.21875</v>
+      </c>
+      <c r="D141" t="n">
+        <v>14.75</v>
+      </c>
+      <c s="2" r="E141" t="n">
+        <v>42170.322916666664</v>
+      </c>
+      <c s="2" r="F141" t="n">
+        <v>42170.854166666664</v>
+      </c>
+      <c r="G141" t="n">
+        <v>53100000000000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c s="1" r="A142" t="n">
+        <v>145</v>
+      </c>
+      <c s="2" r="B142" t="n">
+        <v>42149.541666666664</v>
+      </c>
+      <c s="2" r="C142" t="n">
+        <v>42150.104166666664</v>
+      </c>
+      <c r="D142" t="n">
+        <v>13.5</v>
+      </c>
+      <c s="2" r="E142" t="n">
+        <v>42173.010416666664</v>
+      </c>
+      <c s="2" r="F142" t="n">
+        <v>42173.96875</v>
+      </c>
+      <c r="G142" t="n">
+        <v>48600000000000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c s="1" r="A143" t="n">
+        <v>146</v>
+      </c>
+      <c s="2" r="B143" t="n">
+        <v>42167.375</v>
+      </c>
+      <c s="2" r="C143" t="n">
+        <v>42169.177083333336</v>
+      </c>
+      <c r="D143" t="n">
+        <v>43.25</v>
+      </c>
+      <c r="G143" t="n">
+        <v>155700000000000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c s="1" r="A144" t="n">
+        <v>147</v>
+      </c>
+      <c s="2" r="B144" t="n">
+        <v>42170.322916666664</v>
+      </c>
+      <c s="2" r="C144" t="n">
+        <v>42170.854166666664</v>
+      </c>
+      <c r="D144" t="n">
+        <v>12.75</v>
+      </c>
+      <c r="G144" t="n">
+        <v>45900000000000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c s="1" r="A145" t="n">
+        <v>148</v>
+      </c>
+      <c s="2" r="B145" t="n">
+        <v>42173.010416666664</v>
+      </c>
+      <c s="2" r="C145" t="n">
+        <v>42173.96875</v>
+      </c>
+      <c r="D145" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="G145" t="n">
+        <v>82800000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished revision for Trent
Just need to proofread
</commit_message>
<xml_diff>
--- a/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
+++ b/Data/Q/StormIntervals/DAM_StormIntervals.xlsx
@@ -396,7 +396,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -438,22 +438,22 @@
         <v>0</v>
       </c>
       <c s="2" r="B2" t="n">
-        <v>40927.03125</v>
+        <v>40927.020833333336</v>
       </c>
       <c s="2" r="C2" t="n">
-        <v>40927.28125</v>
+        <v>40927.333333333336</v>
       </c>
       <c r="D2" t="n">
-        <v>6.0</v>
+        <v>7.5</v>
       </c>
       <c s="2" r="E2" t="n">
-        <v>40941.260416666664</v>
+        <v>40941.25</v>
       </c>
       <c s="2" r="F2" t="n">
-        <v>40941.666666666664</v>
+        <v>40941.770833333336</v>
       </c>
       <c r="G2" t="n">
-        <v>21600000000000</v>
+        <v>27000000000000</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -461,22 +461,22 @@
         <v>1</v>
       </c>
       <c s="2" r="B3" t="n">
-        <v>40927.572916666664</v>
+        <v>40927.5625</v>
       </c>
       <c s="2" r="C3" t="n">
-        <v>40927.885416666664</v>
+        <v>40927.947916666664</v>
       </c>
       <c r="D3" t="n">
-        <v>7.5</v>
+        <v>9.25</v>
       </c>
       <c s="2" r="E3" t="n">
-        <v>40942.322916666664</v>
+        <v>40942.052083333336</v>
       </c>
       <c s="2" r="F3" t="n">
-        <v>40942.8125</v>
+        <v>40942.135416666664</v>
       </c>
       <c r="G3" t="n">
-        <v>27000000000000</v>
+        <v>33300000000000</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -484,22 +484,22 @@
         <v>3</v>
       </c>
       <c s="2" r="B4" t="n">
-        <v>40941.260416666664</v>
+        <v>40941.25</v>
       </c>
       <c s="2" r="C4" t="n">
-        <v>40941.666666666664</v>
+        <v>40941.770833333336</v>
       </c>
       <c r="D4" t="n">
-        <v>9.75</v>
+        <v>12.5</v>
       </c>
       <c s="2" r="E4" t="n">
-        <v>40944.96875</v>
+        <v>40942.229166666664</v>
       </c>
       <c s="2" r="F4" t="n">
-        <v>40946.833333333336</v>
+        <v>40942.322916666664</v>
       </c>
       <c r="G4" t="n">
-        <v>35100000000000</v>
+        <v>45000000000000</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -507,1537 +507,1537 @@
         <v>4</v>
       </c>
       <c s="2" r="B5" t="n">
+        <v>40942.052083333336</v>
+      </c>
+      <c s="2" r="C5" t="n">
+        <v>40942.895833333336</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20.25</v>
+      </c>
+      <c s="2" r="E5" t="n">
         <v>40942.322916666664</v>
       </c>
-      <c s="2" r="C5" t="n">
-        <v>40942.8125</v>
-      </c>
-      <c r="D5" t="n">
-        <v>11.75</v>
-      </c>
-      <c s="2" r="E5" t="n">
-        <v>40962.875</v>
-      </c>
       <c s="2" r="F5" t="n">
-        <v>40963.15625</v>
+        <v>40942.895833333336</v>
       </c>
       <c r="G5" t="n">
-        <v>42300000000000</v>
+        <v>72900000000000</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c s="1" r="A6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c s="2" r="B6" t="n">
         <v>40944.416666666664</v>
       </c>
       <c s="2" r="C6" t="n">
-        <v>40944.822916666664</v>
+        <v>40944.895833333336</v>
       </c>
       <c r="D6" t="n">
-        <v>9.75</v>
+        <v>11.5</v>
       </c>
       <c s="2" r="E6" t="n">
         <v>40976.6875</v>
       </c>
       <c s="2" r="F6" t="n">
-        <v>40976.822916666664</v>
+        <v>40976.854166666664</v>
       </c>
       <c r="G6" t="n">
-        <v>35100000000000</v>
+        <v>41400000000000</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c s="1" r="A7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c s="2" r="B7" t="n">
-        <v>40944.96875</v>
+        <v>40944.958333333336</v>
       </c>
       <c s="2" r="C7" t="n">
-        <v>40946.833333333336</v>
+        <v>40947.0</v>
       </c>
       <c r="D7" t="n">
-        <v>44.75</v>
+        <v>49.0</v>
       </c>
       <c s="2" r="E7" t="n">
         <v>40977.25</v>
       </c>
       <c s="2" r="F7" t="n">
-        <v>40977.541666666664</v>
+        <v>40977.583333333336</v>
       </c>
       <c r="G7" t="n">
-        <v>161100000000000</v>
+        <v>176400000000000</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c s="1" r="A8" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c s="2" r="B8" t="n">
-        <v>40962.875</v>
+        <v>40962.864583333336</v>
       </c>
       <c s="2" r="C8" t="n">
-        <v>40963.15625</v>
+        <v>40963.21875</v>
       </c>
       <c r="D8" t="n">
-        <v>6.75</v>
+        <v>8.5</v>
       </c>
       <c s="2" r="E8" t="n">
-        <v>40984.427083333336</v>
+        <v>40984.416666666664</v>
       </c>
       <c s="2" r="F8" t="n">
-        <v>40984.59375</v>
+        <v>40984.6875</v>
       </c>
       <c r="G8" t="n">
-        <v>24300000000000</v>
+        <v>30600000000000</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c s="1" r="A9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c s="2" r="B9" t="n">
         <v>40976.6875</v>
       </c>
       <c s="2" r="C9" t="n">
-        <v>40976.822916666664</v>
+        <v>40976.854166666664</v>
       </c>
       <c r="D9" t="n">
-        <v>3.25</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E9" t="n">
         <v>40985.489583333336</v>
       </c>
       <c s="2" r="F9" t="n">
-        <v>40985.71875</v>
+        <v>40985.739583333336</v>
       </c>
       <c r="G9" t="n">
-        <v>11700000000000</v>
+        <v>14400000000000</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c s="1" r="A10" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c s="2" r="B10" t="n">
         <v>40977.25</v>
       </c>
       <c s="2" r="C10" t="n">
-        <v>40977.541666666664</v>
+        <v>40977.583333333336</v>
       </c>
       <c r="D10" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c s="2" r="E10" t="n">
         <v>40989.84375</v>
       </c>
       <c s="2" r="F10" t="n">
-        <v>40990.09375</v>
+        <v>40990.145833333336</v>
       </c>
       <c r="G10" t="n">
-        <v>25200000000000</v>
+        <v>28800000000000</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c s="1" r="A11" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c s="2" r="B11" t="n">
-        <v>40984.427083333336</v>
+        <v>40984.416666666664</v>
       </c>
       <c s="2" r="C11" t="n">
-        <v>40984.59375</v>
+        <v>40984.6875</v>
       </c>
       <c r="D11" t="n">
-        <v>4.0</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E11" t="n">
-        <v>40990.90625</v>
+        <v>40990.21875</v>
       </c>
       <c s="2" r="F11" t="n">
-        <v>40991.260416666664</v>
+        <v>40990.302083333336</v>
       </c>
       <c r="G11" t="n">
-        <v>14400000000000</v>
+        <v>23400000000000</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c s="1" r="A12" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c s="2" r="B12" t="n">
         <v>40985.489583333336</v>
       </c>
       <c s="2" r="C12" t="n">
-        <v>40985.71875</v>
+        <v>40985.739583333336</v>
       </c>
       <c r="D12" t="n">
-        <v>5.5</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E12" t="n">
-        <v>40993.145833333336</v>
+        <v>40990.90625</v>
       </c>
       <c s="2" r="F12" t="n">
-        <v>40993.854166666664</v>
+        <v>40991.322916666664</v>
       </c>
       <c r="G12" t="n">
-        <v>19800000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c s="1" r="A13" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c s="2" r="B13" t="n">
         <v>40989.84375</v>
       </c>
       <c s="2" r="C13" t="n">
-        <v>40990.09375</v>
+        <v>40990.145833333336</v>
       </c>
       <c r="D13" t="n">
-        <v>6.0</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E13" t="n">
-        <v>41037.197916666664</v>
+        <v>40993.145833333336</v>
       </c>
       <c s="2" r="F13" t="n">
-        <v>41037.322916666664</v>
+        <v>40993.947916666664</v>
       </c>
       <c r="G13" t="n">
-        <v>21600000000000</v>
+        <v>26100000000000</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c s="1" r="A14" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c s="2" r="B14" t="n">
-        <v>40990.90625</v>
+        <v>40990.21875</v>
       </c>
       <c s="2" r="C14" t="n">
-        <v>40991.260416666664</v>
+        <v>40990.302083333336</v>
       </c>
       <c r="D14" t="n">
-        <v>8.5</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E14" t="n">
-        <v>41051.78125</v>
+        <v>41031.677083333336</v>
       </c>
       <c s="2" r="F14" t="n">
-        <v>41052.083333333336</v>
+        <v>41031.75</v>
       </c>
       <c r="G14" t="n">
-        <v>30600000000000</v>
+        <v>7200000000000</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c s="1" r="A15" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c s="2" r="B15" t="n">
-        <v>40993.145833333336</v>
+        <v>40990.90625</v>
       </c>
       <c s="2" r="C15" t="n">
-        <v>40993.854166666664</v>
+        <v>40991.322916666664</v>
       </c>
       <c r="D15" t="n">
-        <v>17.0</v>
+        <v>10.0</v>
       </c>
       <c s="2" r="E15" t="n">
-        <v>41052.333333333336</v>
+        <v>41037.197916666664</v>
       </c>
       <c s="2" r="F15" t="n">
-        <v>41053.479166666664</v>
+        <v>41037.333333333336</v>
       </c>
       <c r="G15" t="n">
-        <v>61200000000000</v>
+        <v>36000000000000</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c s="1" r="A16" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c s="2" r="B16" t="n">
-        <v>41037.197916666664</v>
+        <v>40993.145833333336</v>
       </c>
       <c s="2" r="C16" t="n">
-        <v>41037.322916666664</v>
+        <v>40993.947916666664</v>
       </c>
       <c r="D16" t="n">
-        <v>3.0</v>
+        <v>19.25</v>
       </c>
       <c s="2" r="E16" t="n">
-        <v>41053.854166666664</v>
+        <v>41051.78125</v>
       </c>
       <c s="2" r="F16" t="n">
-        <v>41054.65625</v>
+        <v>41052.125</v>
       </c>
       <c r="G16" t="n">
-        <v>10800000000000</v>
+        <v>69300000000000</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c s="1" r="A17" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c s="2" r="B17" t="n">
-        <v>41051.78125</v>
+        <v>41031.677083333336</v>
       </c>
       <c s="2" r="C17" t="n">
-        <v>41052.083333333336</v>
+        <v>41031.75</v>
       </c>
       <c r="D17" t="n">
-        <v>7.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E17" t="n">
-        <v>41055.0625</v>
+        <v>41052.322916666664</v>
       </c>
       <c s="2" r="F17" t="n">
-        <v>41055.645833333336</v>
+        <v>41053.583333333336</v>
       </c>
       <c r="G17" t="n">
-        <v>26100000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c s="1" r="A18" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c s="2" r="B18" t="n">
-        <v>41052.333333333336</v>
+        <v>41037.197916666664</v>
       </c>
       <c s="2" r="C18" t="n">
-        <v>41053.479166666664</v>
+        <v>41037.333333333336</v>
       </c>
       <c r="D18" t="n">
-        <v>27.5</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E18" t="n">
-        <v>41063.4375</v>
+        <v>41053.833333333336</v>
       </c>
       <c s="2" r="F18" t="n">
-        <v>41063.84375</v>
+        <v>41054.708333333336</v>
       </c>
       <c r="G18" t="n">
-        <v>99000000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c s="1" r="A19" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c s="2" r="B19" t="n">
-        <v>41053.854166666664</v>
+        <v>41051.78125</v>
       </c>
       <c s="2" r="C19" t="n">
-        <v>41054.65625</v>
+        <v>41052.125</v>
       </c>
       <c r="D19" t="n">
-        <v>19.25</v>
+        <v>8.25</v>
       </c>
       <c s="2" r="E19" t="n">
-        <v>41064.010416666664</v>
+        <v>41055.0625</v>
       </c>
       <c s="2" r="F19" t="n">
-        <v>41064.46875</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="G19" t="n">
-        <v>69300000000000</v>
+        <v>29700000000000</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c s="1" r="A20" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c s="2" r="B20" t="n">
-        <v>41055.0625</v>
+        <v>41052.322916666664</v>
       </c>
       <c s="2" r="C20" t="n">
-        <v>41055.645833333336</v>
+        <v>41053.583333333336</v>
       </c>
       <c r="D20" t="n">
-        <v>14.0</v>
+        <v>30.25</v>
       </c>
       <c s="2" r="E20" t="n">
-        <v>41064.604166666664</v>
+        <v>41063.427083333336</v>
       </c>
       <c s="2" r="F20" t="n">
-        <v>41065.770833333336</v>
+        <v>41063.885416666664</v>
       </c>
       <c r="G20" t="n">
-        <v>50400000000000</v>
+        <v>108900000000000</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c s="1" r="A21" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c s="2" r="B21" t="n">
-        <v>41063.4375</v>
+        <v>41053.833333333336</v>
       </c>
       <c s="2" r="C21" t="n">
-        <v>41063.84375</v>
+        <v>41054.708333333336</v>
       </c>
       <c r="D21" t="n">
-        <v>9.75</v>
+        <v>21.0</v>
       </c>
       <c s="2" r="E21" t="n">
-        <v>41066.885416666664</v>
+        <v>41064.010416666664</v>
       </c>
       <c s="2" r="F21" t="n">
-        <v>41067.020833333336</v>
+        <v>41064.46875</v>
       </c>
       <c r="G21" t="n">
-        <v>35100000000000</v>
+        <v>75600000000000</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c s="1" r="A22" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c s="2" r="B22" t="n">
-        <v>41064.010416666664</v>
+        <v>41055.0625</v>
       </c>
       <c s="2" r="C22" t="n">
-        <v>41064.46875</v>
+        <v>41055.708333333336</v>
       </c>
       <c r="D22" t="n">
-        <v>11.0</v>
+        <v>15.5</v>
       </c>
       <c s="2" r="E22" t="n">
-        <v>41067.333333333336</v>
+        <v>41064.604166666664</v>
       </c>
       <c s="2" r="F22" t="n">
-        <v>41067.614583333336</v>
+        <v>41065.895833333336</v>
       </c>
       <c r="G22" t="n">
-        <v>39600000000000</v>
+        <v>55800000000000</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c s="1" r="A23" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c s="2" r="B23" t="n">
-        <v>41064.604166666664</v>
+        <v>41063.427083333336</v>
       </c>
       <c s="2" r="C23" t="n">
-        <v>41065.770833333336</v>
+        <v>41063.885416666664</v>
       </c>
       <c r="D23" t="n">
-        <v>28.0</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E23" t="n">
-        <v>41098.083333333336</v>
+        <v>41066.885416666664</v>
       </c>
       <c s="2" r="F23" t="n">
-        <v>41098.229166666664</v>
+        <v>41067.270833333336</v>
       </c>
       <c r="G23" t="n">
-        <v>100800000000000</v>
+        <v>39600000000000</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c s="1" r="A24" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c s="2" r="B24" t="n">
-        <v>41066.885416666664</v>
+        <v>41064.010416666664</v>
       </c>
       <c s="2" r="C24" t="n">
-        <v>41067.020833333336</v>
+        <v>41064.46875</v>
       </c>
       <c r="D24" t="n">
-        <v>3.25</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E24" t="n">
-        <v>41130.145833333336</v>
+        <v>41067.3125</v>
       </c>
       <c s="2" r="F24" t="n">
-        <v>41130.364583333336</v>
+        <v>41067.729166666664</v>
       </c>
       <c r="G24" t="n">
-        <v>11700000000000</v>
+        <v>39600000000000</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c s="1" r="A25" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c s="2" r="B25" t="n">
-        <v>41067.333333333336</v>
+        <v>41064.604166666664</v>
       </c>
       <c s="2" r="C25" t="n">
-        <v>41067.614583333336</v>
+        <v>41065.895833333336</v>
       </c>
       <c r="D25" t="n">
-        <v>6.75</v>
+        <v>31.0</v>
       </c>
       <c s="2" r="E25" t="n">
-        <v>41153.479166666664</v>
+        <v>41098.083333333336</v>
       </c>
       <c s="2" r="F25" t="n">
-        <v>41155.15625</v>
+        <v>41098.25</v>
       </c>
       <c r="G25" t="n">
-        <v>24300000000000</v>
+        <v>111600000000000</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c s="1" r="A26" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c s="2" r="B26" t="n">
-        <v>41098.083333333336</v>
+        <v>41066.885416666664</v>
       </c>
       <c s="2" r="C26" t="n">
-        <v>41098.229166666664</v>
+        <v>41067.270833333336</v>
       </c>
       <c r="D26" t="n">
-        <v>3.5</v>
+        <v>9.25</v>
       </c>
       <c s="2" r="E26" t="n">
-        <v>41316.875</v>
+        <v>41117.09375</v>
       </c>
       <c s="2" r="F26" t="n">
-        <v>41317.458333333336</v>
+        <v>41117.1875</v>
       </c>
       <c r="G26" t="n">
-        <v>12600000000000</v>
+        <v>33300000000000</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c s="1" r="A27" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c s="2" r="B27" t="n">
-        <v>41130.145833333336</v>
+        <v>41067.3125</v>
       </c>
       <c s="2" r="C27" t="n">
-        <v>41130.364583333336</v>
+        <v>41067.729166666664</v>
       </c>
       <c r="D27" t="n">
-        <v>5.25</v>
+        <v>10.0</v>
       </c>
       <c s="2" r="E27" t="n">
-        <v>41338.78125</v>
+        <v>41117.854166666664</v>
       </c>
       <c s="2" r="F27" t="n">
-        <v>41339.041666666664</v>
+        <v>41117.927083333336</v>
       </c>
       <c r="G27" t="n">
-        <v>18900000000000</v>
+        <v>36000000000000</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c s="1" r="A28" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c s="2" r="B28" t="n">
-        <v>41153.479166666664</v>
+        <v>41098.083333333336</v>
       </c>
       <c s="2" r="C28" t="n">
-        <v>41155.15625</v>
+        <v>41098.25</v>
       </c>
       <c r="D28" t="n">
-        <v>40.25</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E28" t="n">
-        <v>41339.385416666664</v>
+        <v>41130.145833333336</v>
       </c>
       <c s="2" r="F28" t="n">
-        <v>41339.895833333336</v>
+        <v>41130.395833333336</v>
       </c>
       <c r="G28" t="n">
-        <v>144900000000000</v>
+        <v>14400000000000</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c s="1" r="A29" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c s="2" r="B29" t="n">
-        <v>41316.875</v>
+        <v>41117.09375</v>
       </c>
       <c s="2" r="C29" t="n">
-        <v>41317.458333333336</v>
+        <v>41117.1875</v>
       </c>
       <c r="D29" t="n">
-        <v>14.0</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E29" t="n">
-        <v>41340.604166666664</v>
+        <v>41153.479166666664</v>
       </c>
       <c s="2" r="F29" t="n">
-        <v>41341.760416666664</v>
+        <v>41155.270833333336</v>
       </c>
       <c r="G29" t="n">
-        <v>50400000000000</v>
+        <v>8100000000000</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c s="1" r="A30" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c s="2" r="B30" t="n">
-        <v>41338.78125</v>
+        <v>41117.854166666664</v>
       </c>
       <c s="2" r="C30" t="n">
-        <v>41339.041666666664</v>
+        <v>41117.927083333336</v>
       </c>
       <c r="D30" t="n">
-        <v>6.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E30" t="n">
-        <v>41344.104166666664</v>
+        <v>41316.875</v>
       </c>
       <c s="2" r="F30" t="n">
-        <v>41344.625</v>
+        <v>41317.53125</v>
       </c>
       <c r="G30" t="n">
-        <v>22500000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c s="1" r="A31" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c s="2" r="B31" t="n">
-        <v>41339.385416666664</v>
+        <v>41130.145833333336</v>
       </c>
       <c s="2" r="C31" t="n">
-        <v>41339.895833333336</v>
+        <v>41130.395833333336</v>
       </c>
       <c r="D31" t="n">
-        <v>12.25</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E31" t="n">
-        <v>41354.552083333336</v>
+        <v>41338.78125</v>
       </c>
       <c s="2" r="F31" t="n">
-        <v>41354.635416666664</v>
+        <v>41339.083333333336</v>
       </c>
       <c r="G31" t="n">
-        <v>44100000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c s="1" r="A32" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c s="2" r="B32" t="n">
-        <v>41340.604166666664</v>
+        <v>41153.479166666664</v>
       </c>
       <c s="2" r="C32" t="n">
-        <v>41341.760416666664</v>
+        <v>41155.270833333336</v>
       </c>
       <c r="D32" t="n">
-        <v>27.75</v>
+        <v>43.0</v>
       </c>
       <c s="2" r="E32" t="n">
-        <v>41380.46875</v>
+        <v>41339.385416666664</v>
       </c>
       <c s="2" r="F32" t="n">
-        <v>41380.875</v>
+        <v>41339.916666666664</v>
       </c>
       <c r="G32" t="n">
-        <v>99900000000000</v>
+        <v>154800000000000</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c s="1" r="A33" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c s="2" r="B33" t="n">
-        <v>41344.104166666664</v>
+        <v>41316.875</v>
       </c>
       <c s="2" r="C33" t="n">
-        <v>41344.625</v>
+        <v>41317.53125</v>
       </c>
       <c r="D33" t="n">
-        <v>12.5</v>
+        <v>15.75</v>
       </c>
       <c s="2" r="E33" t="n">
-        <v>41381.010416666664</v>
+        <v>41340.604166666664</v>
       </c>
       <c s="2" r="F33" t="n">
-        <v>41381.604166666664</v>
+        <v>41341.84375</v>
       </c>
       <c r="G33" t="n">
-        <v>45000000000000</v>
+        <v>56700000000000</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c s="1" r="A34" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c s="2" r="B34" t="n">
-        <v>41354.552083333336</v>
+        <v>41338.78125</v>
       </c>
       <c s="2" r="C34" t="n">
-        <v>41354.635416666664</v>
+        <v>41339.083333333336</v>
       </c>
       <c r="D34" t="n">
-        <v>2.0</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E34" t="n">
-        <v>41384.197916666664</v>
+        <v>41344.09375</v>
       </c>
       <c s="2" r="F34" t="n">
-        <v>41384.552083333336</v>
+        <v>41344.791666666664</v>
       </c>
       <c r="G34" t="n">
-        <v>7200000000000</v>
+        <v>26100000000000</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c s="1" r="A35" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c s="2" r="B35" t="n">
-        <v>41380.46875</v>
+        <v>41339.385416666664</v>
       </c>
       <c s="2" r="C35" t="n">
-        <v>41380.875</v>
+        <v>41339.916666666664</v>
       </c>
       <c r="D35" t="n">
-        <v>9.75</v>
+        <v>12.75</v>
       </c>
       <c s="2" r="E35" t="n">
-        <v>41387.5625</v>
+        <v>41354.552083333336</v>
       </c>
       <c s="2" r="F35" t="n">
-        <v>41388.25</v>
+        <v>41354.645833333336</v>
       </c>
       <c r="G35" t="n">
-        <v>35100000000000</v>
+        <v>45900000000000</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c s="1" r="A36" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c s="2" r="B36" t="n">
-        <v>41381.010416666664</v>
+        <v>41340.604166666664</v>
       </c>
       <c s="2" r="C36" t="n">
-        <v>41381.604166666664</v>
+        <v>41341.84375</v>
       </c>
       <c r="D36" t="n">
-        <v>14.25</v>
+        <v>29.75</v>
       </c>
       <c s="2" r="E36" t="n">
-        <v>41392.427083333336</v>
+        <v>41356.458333333336</v>
       </c>
       <c s="2" r="F36" t="n">
-        <v>41392.59375</v>
+        <v>41356.53125</v>
       </c>
       <c r="G36" t="n">
-        <v>51300000000000</v>
+        <v>107100000000000</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c s="1" r="A37" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c s="2" r="B37" t="n">
-        <v>41384.197916666664</v>
+        <v>41344.09375</v>
       </c>
       <c s="2" r="C37" t="n">
-        <v>41384.552083333336</v>
+        <v>41344.791666666664</v>
       </c>
       <c r="D37" t="n">
-        <v>8.5</v>
+        <v>16.75</v>
       </c>
       <c s="2" r="E37" t="n">
-        <v>41392.84375</v>
+        <v>41380.458333333336</v>
       </c>
       <c s="2" r="F37" t="n">
-        <v>41393.125</v>
+        <v>41380.90625</v>
       </c>
       <c r="G37" t="n">
-        <v>30600000000000</v>
+        <v>60300000000000</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c s="1" r="A38" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c s="2" r="B38" t="n">
-        <v>41387.5625</v>
+        <v>41354.552083333336</v>
       </c>
       <c s="2" r="C38" t="n">
-        <v>41388.25</v>
+        <v>41354.645833333336</v>
       </c>
       <c r="D38" t="n">
-        <v>16.5</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E38" t="n">
-        <v>41394.625</v>
+        <v>41381.0</v>
       </c>
       <c s="2" r="F38" t="n">
-        <v>41395.59375</v>
+        <v>41381.697916666664</v>
       </c>
       <c r="G38" t="n">
-        <v>59400000000000</v>
+        <v>8100000000000</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c s="1" r="A39" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c s="2" r="B39" t="n">
-        <v>41392.427083333336</v>
+        <v>41356.458333333336</v>
       </c>
       <c s="2" r="C39" t="n">
-        <v>41392.59375</v>
+        <v>41356.53125</v>
       </c>
       <c r="D39" t="n">
-        <v>4.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E39" t="n">
-        <v>41430.25</v>
+        <v>41384.1875</v>
       </c>
       <c s="2" r="F39" t="n">
-        <v>41431.145833333336</v>
+        <v>41384.604166666664</v>
       </c>
       <c r="G39" t="n">
-        <v>14400000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c s="1" r="A40" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c s="2" r="B40" t="n">
-        <v>41392.84375</v>
+        <v>41380.458333333336</v>
       </c>
       <c s="2" r="C40" t="n">
-        <v>41393.125</v>
+        <v>41380.90625</v>
       </c>
       <c r="D40" t="n">
-        <v>6.75</v>
+        <v>10.75</v>
       </c>
       <c s="2" r="E40" t="n">
-        <v>41441.135416666664</v>
+        <v>41387.5625</v>
       </c>
       <c s="2" r="F40" t="n">
-        <v>41441.385416666664</v>
+        <v>41388.3125</v>
       </c>
       <c r="G40" t="n">
-        <v>24300000000000</v>
+        <v>38700000000000</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c s="1" r="A41" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c s="2" r="B41" t="n">
-        <v>41394.625</v>
+        <v>41381.0</v>
       </c>
       <c s="2" r="C41" t="n">
-        <v>41395.59375</v>
+        <v>41381.697916666664</v>
       </c>
       <c r="D41" t="n">
-        <v>23.25</v>
+        <v>16.75</v>
       </c>
       <c s="2" r="E41" t="n">
-        <v>41472.958333333336</v>
+        <v>41392.427083333336</v>
       </c>
       <c s="2" r="F41" t="n">
-        <v>41473.427083333336</v>
+        <v>41392.625</v>
       </c>
       <c r="G41" t="n">
-        <v>83700000000000</v>
+        <v>60300000000000</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c s="1" r="A42" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c s="2" r="B42" t="n">
-        <v>41430.25</v>
+        <v>41384.1875</v>
       </c>
       <c s="2" r="C42" t="n">
-        <v>41431.145833333336</v>
+        <v>41384.604166666664</v>
       </c>
       <c r="D42" t="n">
-        <v>21.5</v>
+        <v>10.0</v>
       </c>
       <c s="2" r="E42" t="n">
-        <v>41474.385416666664</v>
+        <v>41392.84375</v>
       </c>
       <c s="2" r="F42" t="n">
-        <v>41474.604166666664</v>
+        <v>41393.166666666664</v>
       </c>
       <c r="G42" t="n">
-        <v>77400000000000</v>
+        <v>36000000000000</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c s="1" r="A43" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c s="2" r="B43" t="n">
-        <v>41441.135416666664</v>
+        <v>41387.5625</v>
       </c>
       <c s="2" r="C43" t="n">
-        <v>41441.385416666664</v>
+        <v>41388.3125</v>
       </c>
       <c r="D43" t="n">
-        <v>6.0</v>
+        <v>18.0</v>
       </c>
       <c s="2" r="E43" t="n">
-        <v>41474.635416666664</v>
+        <v>41394.625</v>
       </c>
       <c s="2" r="F43" t="n">
-        <v>41475.614583333336</v>
+        <v>41395.65625</v>
       </c>
       <c r="G43" t="n">
-        <v>21600000000000</v>
+        <v>64800000000000</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c s="1" r="A44" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c s="2" r="B44" t="n">
-        <v>41472.958333333336</v>
+        <v>41392.427083333336</v>
       </c>
       <c s="2" r="C44" t="n">
-        <v>41473.427083333336</v>
+        <v>41392.625</v>
       </c>
       <c r="D44" t="n">
-        <v>11.25</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E44" t="n">
-        <v>41492.0</v>
+        <v>41405.604166666664</v>
       </c>
       <c s="2" r="F44" t="n">
-        <v>41492.197916666664</v>
+        <v>41405.677083333336</v>
       </c>
       <c r="G44" t="n">
-        <v>40500000000000</v>
+        <v>17100000000000</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c s="1" r="A45" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c s="2" r="B45" t="n">
-        <v>41474.385416666664</v>
+        <v>41392.84375</v>
       </c>
       <c s="2" r="C45" t="n">
-        <v>41474.604166666664</v>
+        <v>41393.166666666664</v>
       </c>
       <c r="D45" t="n">
-        <v>5.25</v>
+        <v>7.75</v>
       </c>
       <c s="2" r="E45" t="n">
-        <v>41496.1875</v>
+        <v>41430.239583333336</v>
       </c>
       <c s="2" r="F45" t="n">
-        <v>41497.0</v>
+        <v>41431.208333333336</v>
       </c>
       <c r="G45" t="n">
-        <v>18900000000000</v>
+        <v>27900000000000</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c s="1" r="A46" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c s="2" r="B46" t="n">
-        <v>41474.635416666664</v>
+        <v>41394.625</v>
       </c>
       <c s="2" r="C46" t="n">
-        <v>41475.614583333336</v>
+        <v>41395.65625</v>
       </c>
       <c r="D46" t="n">
-        <v>23.5</v>
+        <v>24.75</v>
       </c>
       <c s="2" r="E46" t="n">
-        <v>41501.791666666664</v>
+        <v>41441.135416666664</v>
       </c>
       <c s="2" r="F46" t="n">
-        <v>41501.9375</v>
+        <v>41441.40625</v>
       </c>
       <c r="G46" t="n">
-        <v>84600000000000</v>
+        <v>89100000000000</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c s="1" r="A47" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c s="2" r="B47" t="n">
-        <v>41492.0</v>
+        <v>41405.604166666664</v>
       </c>
       <c s="2" r="C47" t="n">
-        <v>41492.197916666664</v>
+        <v>41405.677083333336</v>
       </c>
       <c r="D47" t="n">
-        <v>4.75</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E47" t="n">
-        <v>41502.333333333336</v>
+        <v>41472.145833333336</v>
       </c>
       <c s="2" r="F47" t="n">
-        <v>41504.583333333336</v>
+        <v>41472.229166666664</v>
       </c>
       <c r="G47" t="n">
-        <v>17100000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c s="1" r="A48" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c s="2" r="B48" t="n">
-        <v>41496.1875</v>
+        <v>41430.239583333336</v>
       </c>
       <c s="2" r="C48" t="n">
-        <v>41497.0</v>
+        <v>41431.208333333336</v>
       </c>
       <c r="D48" t="n">
-        <v>19.5</v>
+        <v>23.25</v>
       </c>
       <c s="2" r="E48" t="n">
-        <v>41505.28125</v>
+        <v>41472.958333333336</v>
       </c>
       <c s="2" r="F48" t="n">
-        <v>41505.854166666664</v>
+        <v>41473.46875</v>
       </c>
       <c r="G48" t="n">
-        <v>70200000000000</v>
+        <v>83700000000000</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c s="1" r="A49" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c s="2" r="B49" t="n">
-        <v>41501.791666666664</v>
+        <v>41441.135416666664</v>
       </c>
       <c s="2" r="C49" t="n">
-        <v>41501.9375</v>
+        <v>41441.40625</v>
       </c>
       <c r="D49" t="n">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E49" t="n">
-        <v>41518.197916666664</v>
+        <v>41474.364583333336</v>
       </c>
       <c s="2" r="F49" t="n">
-        <v>41518.270833333336</v>
+        <v>41474.625</v>
       </c>
       <c r="G49" t="n">
-        <v>12600000000000</v>
+        <v>23400000000000</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c s="1" r="A50" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c s="2" r="B50" t="n">
-        <v>41502.333333333336</v>
+        <v>41472.145833333336</v>
       </c>
       <c s="2" r="C50" t="n">
-        <v>41504.583333333336</v>
+        <v>41472.229166666664</v>
       </c>
       <c r="D50" t="n">
-        <v>54.0</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E50" t="n">
-        <v>41518.354166666664</v>
+        <v>41474.625</v>
       </c>
       <c s="2" r="F50" t="n">
-        <v>41518.583333333336</v>
+        <v>41475.666666666664</v>
       </c>
       <c r="G50" t="n">
-        <v>194400000000000</v>
+        <v>7200000000000</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c s="1" r="A51" t="n">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c s="2" r="B51" t="n">
-        <v>41505.28125</v>
+        <v>41472.958333333336</v>
       </c>
       <c s="2" r="C51" t="n">
-        <v>41505.854166666664</v>
+        <v>41473.46875</v>
       </c>
       <c r="D51" t="n">
-        <v>13.75</v>
+        <v>12.25</v>
       </c>
       <c s="2" r="E51" t="n">
-        <v>41684.625</v>
+        <v>41496.1875</v>
       </c>
       <c s="2" r="F51" t="n">
-        <v>41684.822916666664</v>
+        <v>41497.052083333336</v>
       </c>
       <c r="G51" t="n">
-        <v>49500000000000</v>
+        <v>44100000000000</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c s="1" r="A52" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c s="2" r="B52" t="n">
-        <v>41518.197916666664</v>
+        <v>41474.364583333336</v>
       </c>
       <c s="2" r="C52" t="n">
-        <v>41518.270833333336</v>
+        <v>41475.666666666664</v>
       </c>
       <c r="D52" t="n">
-        <v>1.75</v>
+        <v>31.25</v>
       </c>
       <c s="2" r="E52" t="n">
-        <v>41690.46875</v>
+        <v>41501.791666666664</v>
       </c>
       <c s="2" r="F52" t="n">
-        <v>41690.75</v>
+        <v>41501.947916666664</v>
       </c>
       <c r="G52" t="n">
-        <v>6300000000000</v>
+        <v>112500000000000</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c s="1" r="A53" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c s="2" r="B53" t="n">
-        <v>41518.354166666664</v>
+        <v>41491.989583333336</v>
       </c>
       <c s="2" r="C53" t="n">
-        <v>41518.583333333336</v>
+        <v>41492.229166666664</v>
       </c>
       <c r="D53" t="n">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c s="2" r="E53" t="n">
-        <v>41691.479166666664</v>
+        <v>41502.333333333336</v>
       </c>
       <c s="2" r="F53" t="n">
-        <v>41692.145833333336</v>
+        <v>41504.677083333336</v>
       </c>
       <c r="G53" t="n">
-        <v>19800000000000</v>
+        <v>20700000000000</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c s="1" r="A54" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c s="2" r="B54" t="n">
-        <v>41684.625</v>
+        <v>41496.1875</v>
       </c>
       <c s="2" r="C54" t="n">
-        <v>41684.822916666664</v>
+        <v>41497.052083333336</v>
       </c>
       <c r="D54" t="n">
-        <v>4.75</v>
+        <v>20.75</v>
       </c>
       <c s="2" r="E54" t="n">
-        <v>41695.885416666664</v>
+        <v>41505.28125</v>
       </c>
       <c s="2" r="F54" t="n">
-        <v>41696.697916666664</v>
+        <v>41505.979166666664</v>
       </c>
       <c r="G54" t="n">
-        <v>17100000000000</v>
+        <v>74700000000000</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c s="1" r="A55" t="n">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c s="2" r="B55" t="n">
-        <v>41690.46875</v>
+        <v>41501.791666666664</v>
       </c>
       <c s="2" r="C55" t="n">
-        <v>41690.75</v>
+        <v>41501.947916666664</v>
       </c>
       <c r="D55" t="n">
-        <v>6.75</v>
+        <v>3.75</v>
       </c>
       <c s="2" r="E55" t="n">
-        <v>41697.083333333336</v>
+        <v>41518.197916666664</v>
       </c>
       <c s="2" r="F55" t="n">
-        <v>41697.572916666664</v>
+        <v>41518.28125</v>
       </c>
       <c r="G55" t="n">
-        <v>24300000000000</v>
+        <v>13500000000000</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c s="1" r="A56" t="n">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c s="2" r="B56" t="n">
-        <v>41691.479166666664</v>
+        <v>41502.333333333336</v>
       </c>
       <c s="2" r="C56" t="n">
-        <v>41692.145833333336</v>
+        <v>41504.677083333336</v>
       </c>
       <c r="D56" t="n">
-        <v>16.0</v>
+        <v>56.25</v>
       </c>
       <c s="2" r="E56" t="n">
-        <v>41697.677083333336</v>
+        <v>41518.354166666664</v>
       </c>
       <c s="2" r="F56" t="n">
-        <v>41698.010416666664</v>
+        <v>41518.635416666664</v>
       </c>
       <c r="G56" t="n">
-        <v>57600000000000</v>
+        <v>202500000000000</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c s="1" r="A57" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c s="2" r="B57" t="n">
-        <v>41695.885416666664</v>
+        <v>41505.28125</v>
       </c>
       <c s="2" r="C57" t="n">
-        <v>41696.697916666664</v>
+        <v>41505.979166666664</v>
       </c>
       <c r="D57" t="n">
-        <v>19.5</v>
+        <v>16.75</v>
       </c>
       <c s="2" r="E57" t="n">
-        <v>41704.822916666664</v>
+        <v>41684.614583333336</v>
       </c>
       <c s="2" r="F57" t="n">
-        <v>41705.197916666664</v>
+        <v>41684.84375</v>
       </c>
       <c r="G57" t="n">
-        <v>70200000000000</v>
+        <v>60300000000000</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c s="1" r="A58" t="n">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c s="2" r="B58" t="n">
-        <v>41697.083333333336</v>
+        <v>41518.197916666664</v>
       </c>
       <c s="2" r="C58" t="n">
-        <v>41697.572916666664</v>
+        <v>41518.28125</v>
       </c>
       <c r="D58" t="n">
-        <v>11.75</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E58" t="n">
-        <v>41711.520833333336</v>
+        <v>41685.375</v>
       </c>
       <c s="2" r="F58" t="n">
-        <v>41711.635416666664</v>
+        <v>41685.479166666664</v>
       </c>
       <c r="G58" t="n">
-        <v>42300000000000</v>
+        <v>7200000000000</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c s="1" r="A59" t="n">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c s="2" r="B59" t="n">
-        <v>41697.677083333336</v>
+        <v>41518.354166666664</v>
       </c>
       <c s="2" r="C59" t="n">
-        <v>41698.010416666664</v>
+        <v>41518.635416666664</v>
       </c>
       <c r="D59" t="n">
-        <v>8.0</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E59" t="n">
-        <v>41711.666666666664</v>
+        <v>41688.760416666664</v>
       </c>
       <c s="2" r="F59" t="n">
-        <v>41711.791666666664</v>
+        <v>41688.833333333336</v>
       </c>
       <c r="G59" t="n">
-        <v>28800000000000</v>
+        <v>24300000000000</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c s="1" r="A60" t="n">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c s="2" r="B60" t="n">
-        <v>41704.822916666664</v>
+        <v>41684.614583333336</v>
       </c>
       <c s="2" r="C60" t="n">
-        <v>41705.197916666664</v>
+        <v>41684.84375</v>
       </c>
       <c r="D60" t="n">
-        <v>9.0</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E60" t="n">
-        <v>41711.833333333336</v>
+        <v>41690.46875</v>
       </c>
       <c s="2" r="F60" t="n">
-        <v>41711.947916666664</v>
+        <v>41690.791666666664</v>
       </c>
       <c r="G60" t="n">
-        <v>32400000000000</v>
+        <v>19800000000000</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c s="1" r="A61" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c s="2" r="B61" t="n">
-        <v>41711.520833333336</v>
+        <v>41685.375</v>
       </c>
       <c s="2" r="C61" t="n">
-        <v>41711.635416666664</v>
+        <v>41685.479166666664</v>
       </c>
       <c r="D61" t="n">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c s="2" r="E61" t="n">
-        <v>41712.020833333336</v>
+        <v>41691.479166666664</v>
       </c>
       <c s="2" r="F61" t="n">
-        <v>41712.354166666664</v>
+        <v>41692.239583333336</v>
       </c>
       <c r="G61" t="n">
-        <v>9900000000000</v>
+        <v>9000000000000</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c s="1" r="A62" t="n">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c s="2" r="B62" t="n">
-        <v>41711.666666666664</v>
+        <v>41688.760416666664</v>
       </c>
       <c s="2" r="C62" t="n">
-        <v>41711.791666666664</v>
+        <v>41688.833333333336</v>
       </c>
       <c r="D62" t="n">
-        <v>3.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E62" t="n">
-        <v>41735.520833333336</v>
+        <v>41692.322916666664</v>
       </c>
       <c s="2" r="F62" t="n">
-        <v>41735.989583333336</v>
+        <v>41692.40625</v>
       </c>
       <c r="G62" t="n">
-        <v>10800000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c s="1" r="A63" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c s="2" r="B63" t="n">
-        <v>41711.833333333336</v>
+        <v>41690.46875</v>
       </c>
       <c s="2" r="C63" t="n">
-        <v>41711.947916666664</v>
+        <v>41690.791666666664</v>
       </c>
       <c r="D63" t="n">
-        <v>2.75</v>
+        <v>7.75</v>
       </c>
       <c s="2" r="E63" t="n">
-        <v>41737.604166666664</v>
+        <v>41694.229166666664</v>
       </c>
       <c s="2" r="F63" t="n">
-        <v>41737.770833333336</v>
+        <v>41694.302083333336</v>
       </c>
       <c r="G63" t="n">
-        <v>9900000000000</v>
+        <v>27900000000000</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c s="1" r="A64" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c s="2" r="B64" t="n">
-        <v>41712.020833333336</v>
+        <v>41691.479166666664</v>
       </c>
       <c s="2" r="C64" t="n">
-        <v>41712.354166666664</v>
+        <v>41692.239583333336</v>
       </c>
       <c r="D64" t="n">
-        <v>8.0</v>
+        <v>18.25</v>
       </c>
       <c s="2" r="E64" t="n">
-        <v>41738.989583333336</v>
+        <v>41695.885416666664</v>
       </c>
       <c s="2" r="F64" t="n">
-        <v>41739.15625</v>
+        <v>41696.8125</v>
       </c>
       <c r="G64" t="n">
-        <v>28800000000000</v>
+        <v>65700000000000</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c s="1" r="A65" t="n">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c s="2" r="B65" t="n">
-        <v>41735.520833333336</v>
+        <v>41692.322916666664</v>
       </c>
       <c s="2" r="C65" t="n">
-        <v>41735.989583333336</v>
+        <v>41692.40625</v>
       </c>
       <c r="D65" t="n">
-        <v>11.25</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E65" t="n">
-        <v>41747.791666666664</v>
+        <v>41697.083333333336</v>
       </c>
       <c s="2" r="F65" t="n">
-        <v>41747.979166666664</v>
+        <v>41698.09375</v>
       </c>
       <c r="G65" t="n">
-        <v>40500000000000</v>
+        <v>7200000000000</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c s="1" r="A66" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c s="2" r="B66" t="n">
-        <v>41737.604166666664</v>
+        <v>41694.229166666664</v>
       </c>
       <c s="2" r="C66" t="n">
-        <v>41737.770833333336</v>
+        <v>41694.302083333336</v>
       </c>
       <c r="D66" t="n">
-        <v>4.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E66" t="n">
-        <v>41748.28125</v>
+        <v>41704.802083333336</v>
       </c>
       <c s="2" r="F66" t="n">
-        <v>41748.9375</v>
+        <v>41705.239583333336</v>
       </c>
       <c r="G66" t="n">
-        <v>14400000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c s="1" r="A67" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c s="2" r="B67" t="n">
-        <v>41738.989583333336</v>
+        <v>41695.885416666664</v>
       </c>
       <c s="2" r="C67" t="n">
-        <v>41739.15625</v>
+        <v>41696.8125</v>
       </c>
       <c r="D67" t="n">
-        <v>4.0</v>
+        <v>22.25</v>
       </c>
       <c s="2" r="E67" t="n">
-        <v>41748.9375</v>
+        <v>41711.520833333336</v>
       </c>
       <c s="2" r="F67" t="n">
-        <v>41749.40625</v>
+        <v>41711.65625</v>
       </c>
       <c r="G67" t="n">
-        <v>14400000000000</v>
+        <v>80100000000000</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c s="1" r="A68" t="n">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c s="2" r="B68" t="n">
-        <v>41747.791666666664</v>
+        <v>41697.083333333336</v>
       </c>
       <c s="2" r="C68" t="n">
-        <v>41747.979166666664</v>
+        <v>41698.09375</v>
       </c>
       <c r="D68" t="n">
-        <v>4.5</v>
+        <v>24.25</v>
       </c>
       <c s="2" r="E68" t="n">
-        <v>41756.489583333336</v>
+        <v>41711.666666666664</v>
       </c>
       <c s="2" r="F68" t="n">
-        <v>41756.822916666664</v>
+        <v>41712.0</v>
       </c>
       <c r="G68" t="n">
-        <v>16200000000000</v>
+        <v>87300000000000</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c s="1" r="A69" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c s="2" r="B69" t="n">
-        <v>41748.28125</v>
+        <v>41704.802083333336</v>
       </c>
       <c s="2" r="C69" t="n">
-        <v>41749.40625</v>
+        <v>41705.239583333336</v>
       </c>
       <c r="D69" t="n">
-        <v>27.0</v>
+        <v>10.5</v>
       </c>
       <c s="2" r="E69" t="n">
-        <v>41757.385416666664</v>
+        <v>41712.020833333336</v>
       </c>
       <c s="2" r="F69" t="n">
-        <v>41757.53125</v>
+        <v>41712.40625</v>
       </c>
       <c r="G69" t="n">
-        <v>97200000000000</v>
+        <v>37800000000000</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c s="1" r="A70" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c s="2" r="B70" t="n">
-        <v>41754.65625</v>
+        <v>41711.520833333336</v>
       </c>
       <c s="2" r="C70" t="n">
-        <v>41754.802083333336</v>
+        <v>41711.65625</v>
       </c>
       <c r="D70" t="n">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E70" t="n">
-        <v>41757.885416666664</v>
+        <v>41712.75</v>
       </c>
       <c s="2" r="F70" t="n">
-        <v>41758.5625</v>
+        <v>41712.822916666664</v>
       </c>
       <c r="G70" t="n">
-        <v>12600000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c s="1" r="A71" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c s="2" r="B71" t="n">
-        <v>41756.489583333336</v>
+        <v>41711.666666666664</v>
       </c>
       <c s="2" r="C71" t="n">
-        <v>41756.822916666664</v>
+        <v>41712.0</v>
       </c>
       <c r="D71" t="n">
         <v>8.0</v>
       </c>
       <c s="2" r="E71" t="n">
-        <v>41759.489583333336</v>
+        <v>41730.364583333336</v>
       </c>
       <c s="2" r="F71" t="n">
-        <v>41760.197916666664</v>
+        <v>41730.4375</v>
       </c>
       <c r="G71" t="n">
         <v>28800000000000</v>
@@ -2045,1686 +2045,1088 @@
     </row>
     <row r="72" spans="1:7">
       <c s="1" r="A72" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c s="2" r="B72" t="n">
-        <v>41757.385416666664</v>
+        <v>41712.020833333336</v>
       </c>
       <c s="2" r="C72" t="n">
-        <v>41757.53125</v>
+        <v>41712.40625</v>
       </c>
       <c r="D72" t="n">
-        <v>3.5</v>
+        <v>9.25</v>
       </c>
       <c s="2" r="E72" t="n">
-        <v>41778.5625</v>
+        <v>41735.520833333336</v>
       </c>
       <c s="2" r="F72" t="n">
-        <v>41778.677083333336</v>
+        <v>41736.197916666664</v>
       </c>
       <c r="G72" t="n">
-        <v>12600000000000</v>
+        <v>33300000000000</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c s="1" r="A73" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c s="2" r="B73" t="n">
-        <v>41757.885416666664</v>
+        <v>41712.75</v>
       </c>
       <c s="2" r="C73" t="n">
-        <v>41758.5625</v>
+        <v>41712.822916666664</v>
       </c>
       <c r="D73" t="n">
-        <v>16.25</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E73" t="n">
-        <v>41779.041666666664</v>
+        <v>41737.604166666664</v>
       </c>
       <c s="2" r="F73" t="n">
-        <v>41779.1875</v>
+        <v>41737.791666666664</v>
       </c>
       <c r="G73" t="n">
-        <v>58500000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c s="1" r="A74" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c s="2" r="B74" t="n">
-        <v>41759.489583333336</v>
+        <v>41730.364583333336</v>
       </c>
       <c s="2" r="C74" t="n">
-        <v>41760.197916666664</v>
+        <v>41730.4375</v>
       </c>
       <c r="D74" t="n">
-        <v>17.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E74" t="n">
-        <v>41781.5625</v>
+        <v>41738.979166666664</v>
       </c>
       <c s="2" r="F74" t="n">
-        <v>41782.104166666664</v>
+        <v>41739.197916666664</v>
       </c>
       <c r="G74" t="n">
-        <v>61200000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c s="1" r="A75" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c s="2" r="B75" t="n">
-        <v>41778.5625</v>
+        <v>41735.520833333336</v>
       </c>
       <c s="2" r="C75" t="n">
-        <v>41778.677083333336</v>
+        <v>41736.197916666664</v>
       </c>
       <c r="D75" t="n">
-        <v>2.75</v>
+        <v>16.25</v>
       </c>
       <c s="2" r="E75" t="n">
-        <v>41795.802083333336</v>
+        <v>41740.40625</v>
       </c>
       <c s="2" r="F75" t="n">
-        <v>41796.604166666664</v>
+        <v>41740.5</v>
       </c>
       <c r="G75" t="n">
-        <v>9900000000000</v>
+        <v>58500000000000</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c s="1" r="A76" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c s="2" r="B76" t="n">
-        <v>41779.041666666664</v>
+        <v>41737.604166666664</v>
       </c>
       <c s="2" r="C76" t="n">
-        <v>41779.1875</v>
+        <v>41737.791666666664</v>
       </c>
       <c r="D76" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c s="2" r="E76" t="n">
-        <v>41807.072916666664</v>
+        <v>41746.625</v>
       </c>
       <c s="2" r="F76" t="n">
-        <v>41807.354166666664</v>
+        <v>41746.697916666664</v>
       </c>
       <c r="G76" t="n">
-        <v>12600000000000</v>
+        <v>16200000000000</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c s="1" r="A77" t="n">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c s="2" r="B77" t="n">
-        <v>41781.5625</v>
+        <v>41738.979166666664</v>
       </c>
       <c s="2" r="C77" t="n">
-        <v>41782.104166666664</v>
+        <v>41739.197916666664</v>
       </c>
       <c r="D77" t="n">
-        <v>13.0</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E77" t="n">
-        <v>41823.4375</v>
+        <v>41747.78125</v>
       </c>
       <c s="2" r="F77" t="n">
-        <v>41823.8125</v>
+        <v>41748.010416666664</v>
       </c>
       <c r="G77" t="n">
-        <v>46800000000000</v>
+        <v>18900000000000</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c s="1" r="A78" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c s="2" r="B78" t="n">
-        <v>41795.802083333336</v>
+        <v>41740.40625</v>
       </c>
       <c s="2" r="C78" t="n">
-        <v>41796.604166666664</v>
+        <v>41740.5</v>
       </c>
       <c r="D78" t="n">
-        <v>19.25</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E78" t="n">
-        <v>41825.25</v>
+        <v>41748.28125</v>
       </c>
       <c s="2" r="F78" t="n">
-        <v>41825.729166666664</v>
+        <v>41749.489583333336</v>
       </c>
       <c r="G78" t="n">
-        <v>69300000000000</v>
+        <v>8100000000000</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c s="1" r="A79" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c s="2" r="B79" t="n">
-        <v>41807.072916666664</v>
+        <v>41746.625</v>
       </c>
       <c s="2" r="C79" t="n">
-        <v>41807.354166666664</v>
+        <v>41746.697916666664</v>
       </c>
       <c r="D79" t="n">
-        <v>6.75</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E79" t="n">
-        <v>41826.84375</v>
+        <v>41754.645833333336</v>
       </c>
       <c s="2" r="F79" t="n">
-        <v>41826.979166666664</v>
+        <v>41755.020833333336</v>
       </c>
       <c r="G79" t="n">
-        <v>24300000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c s="1" r="A80" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c s="2" r="B80" t="n">
-        <v>41823.4375</v>
+        <v>41747.78125</v>
       </c>
       <c s="2" r="C80" t="n">
-        <v>41823.8125</v>
+        <v>41748.010416666664</v>
       </c>
       <c r="D80" t="n">
-        <v>9.0</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E80" t="n">
-        <v>41849.25</v>
+        <v>41755.458333333336</v>
       </c>
       <c s="2" r="F80" t="n">
-        <v>41853.125</v>
+        <v>41755.53125</v>
       </c>
       <c r="G80" t="n">
-        <v>32400000000000</v>
+        <v>19800000000000</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c s="1" r="A81" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c s="2" r="B81" t="n">
-        <v>41825.25</v>
+        <v>41748.28125</v>
       </c>
       <c s="2" r="C81" t="n">
-        <v>41825.729166666664</v>
+        <v>41749.489583333336</v>
       </c>
       <c r="D81" t="n">
-        <v>11.5</v>
+        <v>29.0</v>
       </c>
       <c s="2" r="E81" t="n">
-        <v>41853.385416666664</v>
+        <v>41756.479166666664</v>
       </c>
       <c s="2" r="F81" t="n">
-        <v>41853.458333333336</v>
+        <v>41756.90625</v>
       </c>
       <c r="G81" t="n">
-        <v>41400000000000</v>
+        <v>104400000000000</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c s="1" r="A82" t="n">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c s="2" r="B82" t="n">
-        <v>41826.84375</v>
+        <v>41754.645833333336</v>
       </c>
       <c s="2" r="C82" t="n">
-        <v>41826.979166666664</v>
+        <v>41755.020833333336</v>
       </c>
       <c r="D82" t="n">
-        <v>3.25</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E82" t="n">
-        <v>41853.541666666664</v>
+        <v>41757.385416666664</v>
       </c>
       <c s="2" r="F82" t="n">
-        <v>41854.53125</v>
+        <v>41757.583333333336</v>
       </c>
       <c r="G82" t="n">
-        <v>11700000000000</v>
+        <v>32400000000000</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c s="1" r="A83" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c s="2" r="B83" t="n">
-        <v>41849.25</v>
+        <v>41755.458333333336</v>
       </c>
       <c s="2" r="C83" t="n">
-        <v>41853.125</v>
+        <v>41755.53125</v>
       </c>
       <c r="D83" t="n">
-        <v>93.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E83" t="n">
-        <v>41927.53125</v>
+        <v>41757.885416666664</v>
       </c>
       <c s="2" r="F83" t="n">
-        <v>41927.677083333336</v>
+        <v>41758.708333333336</v>
       </c>
       <c r="G83" t="n">
-        <v>334800000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c s="1" r="A84" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c s="2" r="B84" t="n">
-        <v>41853.385416666664</v>
+        <v>41756.479166666664</v>
       </c>
       <c s="2" r="C84" t="n">
-        <v>41853.458333333336</v>
+        <v>41756.90625</v>
       </c>
       <c r="D84" t="n">
-        <v>1.75</v>
+        <v>10.25</v>
       </c>
       <c s="2" r="E84" t="n">
-        <v>41927.739583333336</v>
+        <v>41758.708333333336</v>
       </c>
       <c s="2" r="F84" t="n">
-        <v>41928.041666666664</v>
+        <v>41758.802083333336</v>
       </c>
       <c r="G84" t="n">
-        <v>6300000000000</v>
+        <v>36900000000000</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c s="1" r="A85" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c s="2" r="B85" t="n">
-        <v>41853.541666666664</v>
+        <v>41757.385416666664</v>
       </c>
       <c s="2" r="C85" t="n">
-        <v>41854.53125</v>
+        <v>41757.583333333336</v>
       </c>
       <c r="D85" t="n">
-        <v>23.75</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E85" t="n">
-        <v>41945.15625</v>
+        <v>41758.802083333336</v>
       </c>
       <c s="2" r="F85" t="n">
-        <v>41945.354166666664</v>
+        <v>41758.9375</v>
       </c>
       <c r="G85" t="n">
-        <v>85500000000000</v>
+        <v>17100000000000</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c s="1" r="A86" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c s="2" r="B86" t="n">
-        <v>41927.53125</v>
+        <v>41757.885416666664</v>
       </c>
       <c s="2" r="C86" t="n">
-        <v>41927.677083333336</v>
+        <v>41758.9375</v>
       </c>
       <c r="D86" t="n">
-        <v>3.5</v>
+        <v>25.25</v>
       </c>
       <c s="2" r="E86" t="n">
-        <v>41946.71875</v>
+        <v>41779.041666666664</v>
       </c>
       <c s="2" r="F86" t="n">
-        <v>41947.114583333336</v>
+        <v>41779.208333333336</v>
       </c>
       <c r="G86" t="n">
-        <v>12600000000000</v>
+        <v>90900000000000</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c s="1" r="A87" t="n">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c s="2" r="B87" t="n">
-        <v>41927.739583333336</v>
+        <v>41759.489583333336</v>
       </c>
       <c s="2" r="C87" t="n">
-        <v>41928.041666666664</v>
+        <v>41760.333333333336</v>
       </c>
       <c r="D87" t="n">
-        <v>7.25</v>
+        <v>20.25</v>
       </c>
       <c s="2" r="E87" t="n">
-        <v>41955.395833333336</v>
+        <v>41781.5625</v>
       </c>
       <c s="2" r="F87" t="n">
-        <v>41955.479166666664</v>
+        <v>41782.177083333336</v>
       </c>
       <c r="G87" t="n">
-        <v>26100000000000</v>
+        <v>72900000000000</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c s="1" r="A88" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c s="2" r="B88" t="n">
-        <v>41945.15625</v>
+        <v>41778.5625</v>
       </c>
       <c s="2" r="C88" t="n">
-        <v>41945.354166666664</v>
+        <v>41778.697916666664</v>
       </c>
       <c r="D88" t="n">
-        <v>4.75</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E88" t="n">
-        <v>41955.729166666664</v>
+        <v>41782.333333333336</v>
       </c>
       <c s="2" r="F88" t="n">
-        <v>41955.979166666664</v>
+        <v>41782.53125</v>
       </c>
       <c r="G88" t="n">
-        <v>17100000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c s="1" r="A89" t="n">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c s="2" r="B89" t="n">
-        <v>41946.71875</v>
+        <v>41779.041666666664</v>
       </c>
       <c s="2" r="C89" t="n">
-        <v>41947.114583333336</v>
+        <v>41779.208333333336</v>
       </c>
       <c r="D89" t="n">
-        <v>9.5</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E89" t="n">
-        <v>41959.0</v>
+        <v>41782.979166666664</v>
       </c>
       <c s="2" r="F89" t="n">
-        <v>41959.520833333336</v>
+        <v>41783.25</v>
       </c>
       <c r="G89" t="n">
-        <v>34200000000000</v>
+        <v>14400000000000</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c s="1" r="A90" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c s="2" r="B90" t="n">
-        <v>41955.395833333336</v>
+        <v>41781.5625</v>
       </c>
       <c s="2" r="C90" t="n">
-        <v>41955.479166666664</v>
+        <v>41782.177083333336</v>
       </c>
       <c r="D90" t="n">
-        <v>2.0</v>
+        <v>14.75</v>
       </c>
       <c s="2" r="E90" t="n">
-        <v>41961.770833333336</v>
+        <v>41783.375</v>
       </c>
       <c s="2" r="F90" t="n">
-        <v>41962.020833333336</v>
+        <v>41783.447916666664</v>
       </c>
       <c r="G90" t="n">
-        <v>7200000000000</v>
+        <v>53100000000000</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c s="1" r="A91" t="n">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c s="2" r="B91" t="n">
-        <v>41955.729166666664</v>
+        <v>41782.333333333336</v>
       </c>
       <c s="2" r="C91" t="n">
-        <v>41955.979166666664</v>
+        <v>41782.53125</v>
       </c>
       <c r="D91" t="n">
-        <v>6.0</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E91" t="n">
-        <v>41962.822916666664</v>
+        <v>41788.59375</v>
       </c>
       <c s="2" r="F91" t="n">
-        <v>41962.96875</v>
+        <v>41788.729166666664</v>
       </c>
       <c r="G91" t="n">
-        <v>21600000000000</v>
+        <v>17100000000000</v>
       </c>
     </row>
     <row r="92" spans="1:7">
       <c s="1" r="A92" t="n">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c s="2" r="B92" t="n">
-        <v>41959.0</v>
+        <v>41782.979166666664</v>
       </c>
       <c s="2" r="C92" t="n">
-        <v>41959.520833333336</v>
+        <v>41783.25</v>
       </c>
       <c r="D92" t="n">
-        <v>12.5</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E92" t="n">
-        <v>41965.8125</v>
+        <v>41795.791666666664</v>
       </c>
       <c s="2" r="F92" t="n">
-        <v>41966.6875</v>
+        <v>41796.645833333336</v>
       </c>
       <c r="G92" t="n">
-        <v>45000000000000</v>
+        <v>23400000000000</v>
       </c>
     </row>
     <row r="93" spans="1:7">
       <c s="1" r="A93" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c s="2" r="B93" t="n">
-        <v>41961.770833333336</v>
+        <v>41783.375</v>
       </c>
       <c s="2" r="C93" t="n">
-        <v>41962.020833333336</v>
+        <v>41783.447916666664</v>
       </c>
       <c r="D93" t="n">
-        <v>6.0</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E93" t="n">
-        <v>41967.90625</v>
+        <v>41807.041666666664</v>
       </c>
       <c s="2" r="F93" t="n">
-        <v>41968.145833333336</v>
+        <v>41807.40625</v>
       </c>
       <c r="G93" t="n">
-        <v>21600000000000</v>
+        <v>6300000000000</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c s="1" r="A94" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c s="2" r="B94" t="n">
-        <v>41962.822916666664</v>
+        <v>41788.59375</v>
       </c>
       <c s="2" r="C94" t="n">
-        <v>41962.96875</v>
+        <v>41788.729166666664</v>
       </c>
       <c r="D94" t="n">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E94" t="n">
-        <v>41977.84375</v>
+        <v>41823.4375</v>
       </c>
       <c s="2" r="F94" t="n">
-        <v>41978.666666666664</v>
+        <v>41823.833333333336</v>
       </c>
       <c r="G94" t="n">
-        <v>12600000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="95" spans="1:7">
       <c s="1" r="A95" t="n">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c s="2" r="B95" t="n">
-        <v>41965.8125</v>
+        <v>41795.791666666664</v>
       </c>
       <c s="2" r="C95" t="n">
-        <v>41966.6875</v>
+        <v>41796.645833333336</v>
       </c>
       <c r="D95" t="n">
-        <v>21.0</v>
+        <v>20.5</v>
       </c>
       <c s="2" r="E95" t="n">
-        <v>41982.427083333336</v>
+        <v>41825.25</v>
       </c>
       <c s="2" r="F95" t="n">
-        <v>41982.927083333336</v>
+        <v>41825.760416666664</v>
       </c>
       <c r="G95" t="n">
-        <v>75600000000000</v>
+        <v>73800000000000</v>
       </c>
     </row>
     <row r="96" spans="1:7">
       <c s="1" r="A96" t="n">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c s="2" r="B96" t="n">
-        <v>41967.90625</v>
+        <v>41807.041666666664</v>
       </c>
       <c s="2" r="C96" t="n">
-        <v>41968.145833333336</v>
+        <v>41807.40625</v>
       </c>
       <c r="D96" t="n">
-        <v>5.75</v>
+        <v>8.75</v>
       </c>
       <c s="2" r="E96" t="n">
-        <v>41992.020833333336</v>
+        <v>41826.84375</v>
       </c>
       <c s="2" r="F96" t="n">
-        <v>41992.59375</v>
+        <v>41827.0</v>
       </c>
       <c r="G96" t="n">
-        <v>20700000000000</v>
+        <v>31500000000000</v>
       </c>
     </row>
     <row r="97" spans="1:7">
       <c s="1" r="A97" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c s="2" r="B97" t="n">
-        <v>41977.84375</v>
+        <v>41823.4375</v>
       </c>
       <c s="2" r="C97" t="n">
-        <v>41978.666666666664</v>
+        <v>41823.833333333336</v>
       </c>
       <c r="D97" t="n">
-        <v>19.75</v>
+        <v>9.5</v>
       </c>
       <c s="2" r="E97" t="n">
-        <v>41992.614583333336</v>
+        <v>41849.25</v>
       </c>
       <c s="2" r="F97" t="n">
-        <v>41992.833333333336</v>
+        <v>41853.364583333336</v>
       </c>
       <c r="G97" t="n">
-        <v>71100000000000</v>
+        <v>34200000000000</v>
       </c>
     </row>
     <row r="98" spans="1:7">
       <c s="1" r="A98" t="n">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c s="2" r="B98" t="n">
-        <v>41982.427083333336</v>
+        <v>41825.25</v>
       </c>
       <c s="2" r="C98" t="n">
-        <v>41982.927083333336</v>
+        <v>41825.760416666664</v>
       </c>
       <c r="D98" t="n">
-        <v>12.0</v>
+        <v>12.25</v>
       </c>
       <c s="2" r="E98" t="n">
-        <v>41994.020833333336</v>
+        <v>41853.364583333336</v>
       </c>
       <c s="2" r="F98" t="n">
-        <v>41994.385416666664</v>
+        <v>41854.6875</v>
       </c>
       <c r="G98" t="n">
-        <v>43200000000000</v>
+        <v>44100000000000</v>
       </c>
     </row>
     <row r="99" spans="1:7">
       <c s="1" r="A99" t="n">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c s="2" r="B99" t="n">
-        <v>41992.020833333336</v>
+        <v>41826.84375</v>
       </c>
       <c s="2" r="C99" t="n">
-        <v>41992.59375</v>
+        <v>41827.0</v>
       </c>
       <c r="D99" t="n">
-        <v>13.75</v>
+        <v>3.75</v>
       </c>
       <c s="2" r="E99" t="n">
-        <v>41994.40625</v>
+        <v>41927.739583333336</v>
       </c>
       <c s="2" r="F99" t="n">
-        <v>41996.020833333336</v>
+        <v>41928.083333333336</v>
       </c>
       <c r="G99" t="n">
-        <v>49500000000000</v>
+        <v>13500000000000</v>
       </c>
     </row>
     <row r="100" spans="1:7">
       <c s="1" r="A100" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c s="2" r="B100" t="n">
-        <v>41992.614583333336</v>
+        <v>41849.25</v>
       </c>
       <c s="2" r="C100" t="n">
-        <v>41992.833333333336</v>
+        <v>41854.6875</v>
       </c>
       <c r="D100" t="n">
-        <v>5.25</v>
+        <v>130.5</v>
       </c>
       <c s="2" r="E100" t="n">
-        <v>42005.354166666664</v>
+        <v>41945.145833333336</v>
       </c>
       <c s="2" r="F100" t="n">
-        <v>42005.854166666664</v>
+        <v>41945.364583333336</v>
       </c>
       <c r="G100" t="n">
-        <v>18900000000000</v>
+        <v>469800000000000</v>
       </c>
     </row>
     <row r="101" spans="1:7">
       <c s="1" r="A101" t="n">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c s="2" r="B101" t="n">
-        <v>41994.020833333336</v>
+        <v>41927.53125</v>
       </c>
       <c s="2" r="C101" t="n">
-        <v>41994.385416666664</v>
+        <v>41927.6875</v>
       </c>
       <c r="D101" t="n">
-        <v>8.75</v>
+        <v>3.75</v>
       </c>
       <c s="2" r="E101" t="n">
-        <v>42006.5625</v>
+        <v>41946.71875</v>
       </c>
       <c s="2" r="F101" t="n">
-        <v>42006.791666666664</v>
+        <v>41947.15625</v>
       </c>
       <c r="G101" t="n">
-        <v>31500000000000</v>
+        <v>13500000000000</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c s="1" r="A102" t="n">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c s="2" r="B102" t="n">
-        <v>41994.40625</v>
+        <v>41927.739583333336</v>
       </c>
       <c s="2" r="C102" t="n">
-        <v>41996.020833333336</v>
+        <v>41928.083333333336</v>
       </c>
       <c r="D102" t="n">
-        <v>38.75</v>
+        <v>8.25</v>
       </c>
       <c s="2" r="E102" t="n">
-        <v>42008.8125</v>
+        <v>41955.395833333336</v>
       </c>
       <c s="2" r="F102" t="n">
-        <v>42008.916666666664</v>
+        <v>41955.489583333336</v>
       </c>
       <c r="G102" t="n">
-        <v>139500000000000</v>
+        <v>29700000000000</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c s="1" r="A103" t="n">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c s="2" r="B103" t="n">
-        <v>42005.354166666664</v>
+        <v>41945.145833333336</v>
       </c>
       <c s="2" r="C103" t="n">
-        <v>42005.854166666664</v>
+        <v>41945.364583333336</v>
       </c>
       <c r="D103" t="n">
-        <v>12.0</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E103" t="n">
-        <v>42009.135416666664</v>
+        <v>41955.71875</v>
       </c>
       <c s="2" r="F103" t="n">
-        <v>42009.3125</v>
+        <v>41956.020833333336</v>
       </c>
       <c r="G103" t="n">
-        <v>43200000000000</v>
+        <v>18900000000000</v>
       </c>
     </row>
     <row r="104" spans="1:7">
       <c s="1" r="A104" t="n">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c s="2" r="B104" t="n">
-        <v>42006.5625</v>
+        <v>41946.71875</v>
       </c>
       <c s="2" r="C104" t="n">
-        <v>42006.791666666664</v>
+        <v>41947.15625</v>
       </c>
       <c r="D104" t="n">
-        <v>5.5</v>
+        <v>10.5</v>
       </c>
       <c s="2" r="E104" t="n">
-        <v>42013.489583333336</v>
+        <v>41959.0</v>
       </c>
       <c s="2" r="F104" t="n">
-        <v>42014.375</v>
+        <v>41959.572916666664</v>
       </c>
       <c r="G104" t="n">
-        <v>19800000000000</v>
+        <v>37800000000000</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c s="1" r="A105" t="n">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c s="2" r="B105" t="n">
-        <v>42008.8125</v>
+        <v>41955.395833333336</v>
       </c>
       <c s="2" r="C105" t="n">
-        <v>42008.916666666664</v>
+        <v>41955.489583333336</v>
       </c>
       <c r="D105" t="n">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E105" t="n">
-        <v>42024.416666666664</v>
+        <v>41961.770833333336</v>
       </c>
       <c s="2" r="F105" t="n">
-        <v>42024.916666666664</v>
+        <v>41962.072916666664</v>
       </c>
       <c r="G105" t="n">
-        <v>9000000000000</v>
+        <v>8100000000000</v>
       </c>
     </row>
     <row r="106" spans="1:7">
       <c s="1" r="A106" t="n">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c s="2" r="B106" t="n">
-        <v>42009.135416666664</v>
+        <v>41955.71875</v>
       </c>
       <c s="2" r="C106" t="n">
-        <v>42009.3125</v>
+        <v>41956.020833333336</v>
       </c>
       <c r="D106" t="n">
-        <v>4.25</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E106" t="n">
-        <v>42025.21875</v>
+        <v>41962.791666666664</v>
       </c>
       <c s="2" r="F106" t="n">
-        <v>42026.010416666664</v>
+        <v>41963.041666666664</v>
       </c>
       <c r="G106" t="n">
-        <v>15300000000000</v>
+        <v>26100000000000</v>
       </c>
     </row>
     <row r="107" spans="1:7">
       <c s="1" r="A107" t="n">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c s="2" r="B107" t="n">
-        <v>42013.489583333336</v>
+        <v>41959.0</v>
       </c>
       <c s="2" r="C107" t="n">
-        <v>42014.375</v>
+        <v>41959.572916666664</v>
       </c>
       <c r="D107" t="n">
-        <v>21.25</v>
+        <v>13.75</v>
       </c>
       <c s="2" r="E107" t="n">
-        <v>42031.09375</v>
+        <v>41965.8125</v>
       </c>
       <c s="2" r="F107" t="n">
-        <v>42031.302083333336</v>
+        <v>41966.729166666664</v>
       </c>
       <c r="G107" t="n">
-        <v>76500000000000</v>
+        <v>49500000000000</v>
       </c>
     </row>
     <row r="108" spans="1:7">
       <c s="1" r="A108" t="n">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c s="2" r="B108" t="n">
-        <v>42024.416666666664</v>
+        <v>41961.770833333336</v>
       </c>
       <c s="2" r="C108" t="n">
-        <v>42024.916666666664</v>
+        <v>41962.072916666664</v>
       </c>
       <c r="D108" t="n">
-        <v>12.0</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E108" t="n">
-        <v>42033.65625</v>
+        <v>41967.885416666664</v>
       </c>
       <c s="2" r="F108" t="n">
-        <v>42034.9375</v>
+        <v>41968.1875</v>
       </c>
       <c r="G108" t="n">
-        <v>43200000000000</v>
+        <v>26100000000000</v>
       </c>
     </row>
     <row r="109" spans="1:7">
       <c s="1" r="A109" t="n">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c s="2" r="B109" t="n">
-        <v>42025.21875</v>
+        <v>41962.791666666664</v>
       </c>
       <c s="2" r="C109" t="n">
-        <v>42026.010416666664</v>
+        <v>41963.041666666664</v>
       </c>
       <c r="D109" t="n">
-        <v>19.0</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E109" t="n">
-        <v>42034.96875</v>
+        <v>41977.84375</v>
       </c>
       <c s="2" r="F109" t="n">
-        <v>42035.416666666664</v>
+        <v>41978.697916666664</v>
       </c>
       <c r="G109" t="n">
-        <v>68400000000000</v>
+        <v>21600000000000</v>
       </c>
     </row>
     <row r="110" spans="1:7">
       <c s="1" r="A110" t="n">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c s="2" r="B110" t="n">
-        <v>42031.09375</v>
+        <v>41965.8125</v>
       </c>
       <c s="2" r="C110" t="n">
-        <v>42031.302083333336</v>
+        <v>41966.729166666664</v>
       </c>
       <c r="D110" t="n">
-        <v>5.0</v>
+        <v>22.0</v>
       </c>
       <c s="2" r="E110" t="n">
-        <v>42035.520833333336</v>
+        <v>41982.427083333336</v>
       </c>
       <c s="2" r="F110" t="n">
-        <v>42036.770833333336</v>
+        <v>41983.03125</v>
       </c>
       <c r="G110" t="n">
-        <v>18000000000000</v>
+        <v>79200000000000</v>
       </c>
     </row>
     <row r="111" spans="1:7">
       <c s="1" r="A111" t="n">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c s="2" r="B111" t="n">
-        <v>42033.65625</v>
+        <v>41967.885416666664</v>
       </c>
       <c s="2" r="C111" t="n">
-        <v>42034.9375</v>
+        <v>41968.1875</v>
       </c>
       <c r="D111" t="n">
-        <v>30.75</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E111" t="n">
-        <v>42036.770833333336</v>
+        <v>41992.010416666664</v>
       </c>
       <c s="2" r="F111" t="n">
-        <v>42036.864583333336</v>
+        <v>41992.885416666664</v>
       </c>
       <c r="G111" t="n">
-        <v>110700000000000</v>
+        <v>26100000000000</v>
       </c>
     </row>
     <row r="112" spans="1:7">
       <c s="1" r="A112" t="n">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c s="2" r="B112" t="n">
-        <v>42034.96875</v>
+        <v>41977.84375</v>
       </c>
       <c s="2" r="C112" t="n">
-        <v>42035.416666666664</v>
+        <v>41978.697916666664</v>
       </c>
       <c r="D112" t="n">
-        <v>10.75</v>
+        <v>20.5</v>
       </c>
       <c s="2" r="E112" t="n">
-        <v>42043.395833333336</v>
+        <v>41994.020833333336</v>
       </c>
       <c s="2" r="F112" t="n">
-        <v>42043.9375</v>
+        <v>41996.09375</v>
       </c>
       <c r="G112" t="n">
-        <v>38700000000000</v>
+        <v>73800000000000</v>
       </c>
     </row>
     <row r="113" spans="1:7">
       <c s="1" r="A113" t="n">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c s="2" r="B113" t="n">
-        <v>42035.520833333336</v>
+        <v>41982.427083333336</v>
       </c>
       <c s="2" r="C113" t="n">
-        <v>42036.864583333336</v>
+        <v>41983.03125</v>
       </c>
       <c r="D113" t="n">
-        <v>32.25</v>
+        <v>14.5</v>
       </c>
       <c s="2" r="E113" t="n">
-        <v>42044.9375</v>
+        <v>42005.354166666664</v>
       </c>
       <c s="2" r="F113" t="n">
-        <v>42045.697916666664</v>
+        <v>42005.895833333336</v>
       </c>
       <c r="G113" t="n">
-        <v>116100000000000</v>
+        <v>52200000000000</v>
       </c>
     </row>
     <row r="114" spans="1:7">
       <c s="1" r="A114" t="n">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c s="2" r="B114" t="n">
-        <v>42040.53125</v>
+        <v>41992.010416666664</v>
       </c>
       <c s="2" r="C114" t="n">
-        <v>42040.791666666664</v>
+        <v>41992.885416666664</v>
       </c>
       <c r="D114" t="n">
-        <v>6.25</v>
+        <v>21.0</v>
       </c>
       <c s="2" r="E114" t="n">
-        <v>42051.15625</v>
+        <v>42006.5625</v>
       </c>
       <c s="2" r="F114" t="n">
-        <v>42051.239583333336</v>
+        <v>42006.854166666664</v>
       </c>
       <c r="G114" t="n">
-        <v>22500000000000</v>
+        <v>75600000000000</v>
       </c>
     </row>
     <row r="115" spans="1:7">
       <c s="1" r="A115" t="n">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c s="2" r="B115" t="n">
-        <v>42043.395833333336</v>
+        <v>41994.020833333336</v>
       </c>
       <c s="2" r="C115" t="n">
-        <v>42043.9375</v>
+        <v>41996.09375</v>
       </c>
       <c r="D115" t="n">
-        <v>13.0</v>
+        <v>49.75</v>
       </c>
       <c s="2" r="E115" t="n">
-        <v>42051.270833333336</v>
+        <v>42008.8125</v>
       </c>
       <c s="2" r="F115" t="n">
-        <v>42051.604166666664</v>
+        <v>42008.947916666664</v>
       </c>
       <c r="G115" t="n">
-        <v>46800000000000</v>
+        <v>179100000000000</v>
       </c>
     </row>
     <row r="116" spans="1:7">
       <c s="1" r="A116" t="n">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c s="2" r="B116" t="n">
-        <v>42044.9375</v>
+        <v>42005.354166666664</v>
       </c>
       <c s="2" r="C116" t="n">
-        <v>42045.697916666664</v>
+        <v>42005.895833333336</v>
       </c>
       <c r="D116" t="n">
-        <v>18.25</v>
+        <v>13.0</v>
       </c>
       <c s="2" r="E116" t="n">
-        <v>42051.6875</v>
+        <v>42009.125</v>
       </c>
       <c s="2" r="F116" t="n">
-        <v>42051.78125</v>
+        <v>42009.364583333336</v>
       </c>
       <c r="G116" t="n">
-        <v>65700000000000</v>
+        <v>46800000000000</v>
       </c>
     </row>
     <row r="117" spans="1:7">
       <c s="1" r="A117" t="n">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c s="2" r="B117" t="n">
-        <v>42051.15625</v>
+        <v>42006.5625</v>
       </c>
       <c s="2" r="C117" t="n">
-        <v>42051.239583333336</v>
+        <v>42006.854166666664</v>
       </c>
       <c r="D117" t="n">
-        <v>2.0</v>
-      </c>
-      <c s="2" r="E117" t="n">
-        <v>42052.125</v>
-      </c>
-      <c s="2" r="F117" t="n">
-        <v>42052.21875</v>
+        <v>7.0</v>
       </c>
       <c r="G117" t="n">
-        <v>7200000000000</v>
+        <v>25200000000000</v>
       </c>
     </row>
     <row r="118" spans="1:7">
       <c s="1" r="A118" t="n">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c s="2" r="B118" t="n">
-        <v>42051.270833333336</v>
+        <v>42008.8125</v>
       </c>
       <c s="2" r="C118" t="n">
-        <v>42051.604166666664</v>
+        <v>42008.947916666664</v>
       </c>
       <c r="D118" t="n">
-        <v>8.0</v>
-      </c>
-      <c s="2" r="E118" t="n">
-        <v>42056.75</v>
-      </c>
-      <c s="2" r="F118" t="n">
-        <v>42056.895833333336</v>
+        <v>3.25</v>
       </c>
       <c r="G118" t="n">
-        <v>28800000000000</v>
+        <v>11700000000000</v>
       </c>
     </row>
     <row r="119" spans="1:7">
       <c s="1" r="A119" t="n">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c s="2" r="B119" t="n">
-        <v>42051.6875</v>
+        <v>42009.125</v>
       </c>
       <c s="2" r="C119" t="n">
-        <v>42051.78125</v>
+        <v>42009.364583333336</v>
       </c>
       <c r="D119" t="n">
-        <v>2.25</v>
-      </c>
-      <c s="2" r="E119" t="n">
-        <v>42057.052083333336</v>
-      </c>
-      <c s="2" r="F119" t="n">
-        <v>42057.677083333336</v>
+        <v>5.75</v>
       </c>
       <c r="G119" t="n">
-        <v>8100000000000</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c s="1" r="A120" t="n">
-        <v>121</v>
-      </c>
-      <c s="2" r="B120" t="n">
-        <v>42052.125</v>
-      </c>
-      <c s="2" r="C120" t="n">
-        <v>42052.21875</v>
-      </c>
-      <c r="D120" t="n">
-        <v>2.25</v>
-      </c>
-      <c s="2" r="E120" t="n">
-        <v>42079.916666666664</v>
-      </c>
-      <c s="2" r="F120" t="n">
-        <v>42080.229166666664</v>
-      </c>
-      <c r="G120" t="n">
-        <v>8100000000000</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7">
-      <c s="1" r="A121" t="n">
-        <v>122</v>
-      </c>
-      <c s="2" r="B121" t="n">
-        <v>42056.75</v>
-      </c>
-      <c s="2" r="C121" t="n">
-        <v>42056.895833333336</v>
-      </c>
-      <c r="D121" t="n">
-        <v>3.5</v>
-      </c>
-      <c s="2" r="E121" t="n">
-        <v>42085.4375</v>
-      </c>
-      <c s="2" r="F121" t="n">
-        <v>42085.645833333336</v>
-      </c>
-      <c r="G121" t="n">
-        <v>12600000000000</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7">
-      <c s="1" r="A122" t="n">
-        <v>123</v>
-      </c>
-      <c s="2" r="B122" t="n">
-        <v>42057.052083333336</v>
-      </c>
-      <c s="2" r="C122" t="n">
-        <v>42057.677083333336</v>
-      </c>
-      <c r="D122" t="n">
-        <v>15.0</v>
-      </c>
-      <c s="2" r="E122" t="n">
-        <v>42087.0</v>
-      </c>
-      <c s="2" r="F122" t="n">
-        <v>42087.177083333336</v>
-      </c>
-      <c r="G122" t="n">
-        <v>54000000000000</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7">
-      <c s="1" r="A123" t="n">
-        <v>124</v>
-      </c>
-      <c s="2" r="B123" t="n">
-        <v>42079.916666666664</v>
-      </c>
-      <c s="2" r="C123" t="n">
-        <v>42080.229166666664</v>
-      </c>
-      <c r="D123" t="n">
-        <v>7.5</v>
-      </c>
-      <c s="2" r="E123" t="n">
-        <v>42088.5</v>
-      </c>
-      <c s="2" r="F123" t="n">
-        <v>42089.083333333336</v>
-      </c>
-      <c r="G123" t="n">
-        <v>27000000000000</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7">
-      <c s="1" r="A124" t="n">
-        <v>125</v>
-      </c>
-      <c s="2" r="B124" t="n">
-        <v>42085.4375</v>
-      </c>
-      <c s="2" r="C124" t="n">
-        <v>42085.645833333336</v>
-      </c>
-      <c r="D124" t="n">
-        <v>5.0</v>
-      </c>
-      <c s="2" r="E124" t="n">
-        <v>42089.739583333336</v>
-      </c>
-      <c s="2" r="F124" t="n">
-        <v>42090.145833333336</v>
-      </c>
-      <c r="G124" t="n">
-        <v>18000000000000</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7">
-      <c s="1" r="A125" t="n">
-        <v>126</v>
-      </c>
-      <c s="2" r="B125" t="n">
-        <v>42087.0</v>
-      </c>
-      <c s="2" r="C125" t="n">
-        <v>42087.177083333336</v>
-      </c>
-      <c r="D125" t="n">
-        <v>4.25</v>
-      </c>
-      <c s="2" r="E125" t="n">
-        <v>42092.96875</v>
-      </c>
-      <c s="2" r="F125" t="n">
-        <v>42093.083333333336</v>
-      </c>
-      <c r="G125" t="n">
-        <v>15300000000000</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7">
-      <c s="1" r="A126" t="n">
-        <v>127</v>
-      </c>
-      <c s="2" r="B126" t="n">
-        <v>42088.5</v>
-      </c>
-      <c s="2" r="C126" t="n">
-        <v>42089.083333333336</v>
-      </c>
-      <c r="D126" t="n">
-        <v>14.0</v>
-      </c>
-      <c s="2" r="E126" t="n">
-        <v>42095.489583333336</v>
-      </c>
-      <c s="2" r="F126" t="n">
-        <v>42095.822916666664</v>
-      </c>
-      <c r="G126" t="n">
-        <v>50400000000000</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7">
-      <c s="1" r="A127" t="n">
-        <v>128</v>
-      </c>
-      <c s="2" r="B127" t="n">
-        <v>42089.739583333336</v>
-      </c>
-      <c s="2" r="C127" t="n">
-        <v>42090.145833333336</v>
-      </c>
-      <c r="D127" t="n">
-        <v>9.75</v>
-      </c>
-      <c s="2" r="E127" t="n">
-        <v>42096.729166666664</v>
-      </c>
-      <c s="2" r="F127" t="n">
-        <v>42097.260416666664</v>
-      </c>
-      <c r="G127" t="n">
-        <v>35100000000000</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7">
-      <c s="1" r="A128" t="n">
-        <v>129</v>
-      </c>
-      <c s="2" r="B128" t="n">
-        <v>42092.96875</v>
-      </c>
-      <c s="2" r="C128" t="n">
-        <v>42093.083333333336</v>
-      </c>
-      <c r="D128" t="n">
-        <v>2.75</v>
-      </c>
-      <c s="2" r="E128" t="n">
-        <v>42097.260416666664</v>
-      </c>
-      <c s="2" r="F128" t="n">
-        <v>42097.333333333336</v>
-      </c>
-      <c r="G128" t="n">
-        <v>9900000000000</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7">
-      <c s="1" r="A129" t="n">
-        <v>130</v>
-      </c>
-      <c s="2" r="B129" t="n">
-        <v>42095.489583333336</v>
-      </c>
-      <c s="2" r="C129" t="n">
-        <v>42095.822916666664</v>
-      </c>
-      <c r="D129" t="n">
-        <v>8.0</v>
-      </c>
-      <c s="2" r="E129" t="n">
-        <v>42116.739583333336</v>
-      </c>
-      <c s="2" r="F129" t="n">
-        <v>42117.697916666664</v>
-      </c>
-      <c r="G129" t="n">
-        <v>28800000000000</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7">
-      <c s="1" r="A130" t="n">
-        <v>131</v>
-      </c>
-      <c s="2" r="B130" t="n">
-        <v>42096.729166666664</v>
-      </c>
-      <c s="2" r="C130" t="n">
-        <v>42097.333333333336</v>
-      </c>
-      <c r="D130" t="n">
-        <v>14.5</v>
-      </c>
-      <c s="2" r="E130" t="n">
-        <v>42118.510416666664</v>
-      </c>
-      <c s="2" r="F130" t="n">
-        <v>42118.645833333336</v>
-      </c>
-      <c r="G130" t="n">
-        <v>52200000000000</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7">
-      <c s="1" r="A131" t="n">
-        <v>133</v>
-      </c>
-      <c s="2" r="B131" t="n">
-        <v>42112.458333333336</v>
-      </c>
-      <c s="2" r="C131" t="n">
-        <v>42112.875</v>
-      </c>
-      <c r="D131" t="n">
-        <v>10.0</v>
-      </c>
-      <c s="2" r="E131" t="n">
-        <v>42128.0</v>
-      </c>
-      <c s="2" r="F131" t="n">
-        <v>42128.59375</v>
-      </c>
-      <c r="G131" t="n">
-        <v>36000000000000</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7">
-      <c s="1" r="A132" t="n">
-        <v>134</v>
-      </c>
-      <c s="2" r="B132" t="n">
-        <v>42116.739583333336</v>
-      </c>
-      <c s="2" r="C132" t="n">
-        <v>42117.697916666664</v>
-      </c>
-      <c r="D132" t="n">
-        <v>23.0</v>
-      </c>
-      <c s="2" r="E132" t="n">
-        <v>42130.541666666664</v>
-      </c>
-      <c s="2" r="F132" t="n">
-        <v>42130.791666666664</v>
-      </c>
-      <c r="G132" t="n">
-        <v>82800000000000</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7">
-      <c s="1" r="A133" t="n">
-        <v>135</v>
-      </c>
-      <c s="2" r="B133" t="n">
-        <v>42118.510416666664</v>
-      </c>
-      <c s="2" r="C133" t="n">
-        <v>42118.645833333336</v>
-      </c>
-      <c r="D133" t="n">
-        <v>3.25</v>
-      </c>
-      <c s="2" r="E133" t="n">
-        <v>42130.875</v>
-      </c>
-      <c s="2" r="F133" t="n">
-        <v>42131.489583333336</v>
-      </c>
-      <c r="G133" t="n">
-        <v>11700000000000</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7">
-      <c s="1" r="A134" t="n">
-        <v>136</v>
-      </c>
-      <c s="2" r="B134" t="n">
-        <v>42128.0</v>
-      </c>
-      <c s="2" r="C134" t="n">
-        <v>42128.59375</v>
-      </c>
-      <c r="D134" t="n">
-        <v>14.25</v>
-      </c>
-      <c s="2" r="E134" t="n">
-        <v>42131.489583333336</v>
-      </c>
-      <c s="2" r="F134" t="n">
-        <v>42132.416666666664</v>
-      </c>
-      <c r="G134" t="n">
-        <v>51300000000000</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7">
-      <c s="1" r="A135" t="n">
-        <v>137</v>
-      </c>
-      <c s="2" r="B135" t="n">
-        <v>42130.541666666664</v>
-      </c>
-      <c s="2" r="C135" t="n">
-        <v>42130.791666666664</v>
-      </c>
-      <c r="D135" t="n">
-        <v>6.0</v>
-      </c>
-      <c s="2" r="E135" t="n">
-        <v>42139.697916666664</v>
-      </c>
-      <c s="2" r="F135" t="n">
-        <v>42139.864583333336</v>
-      </c>
-      <c r="G135" t="n">
-        <v>21600000000000</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7">
-      <c s="1" r="A136" t="n">
-        <v>138</v>
-      </c>
-      <c s="2" r="B136" t="n">
-        <v>42130.875</v>
-      </c>
-      <c s="2" r="C136" t="n">
-        <v>42132.416666666664</v>
-      </c>
-      <c r="D136" t="n">
-        <v>37.0</v>
-      </c>
-      <c s="2" r="E136" t="n">
-        <v>42140.979166666664</v>
-      </c>
-      <c s="2" r="F136" t="n">
-        <v>42142.177083333336</v>
-      </c>
-      <c r="G136" t="n">
-        <v>133200000000000</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7">
-      <c s="1" r="A137" t="n">
-        <v>140</v>
-      </c>
-      <c s="2" r="B137" t="n">
-        <v>42135.989583333336</v>
-      </c>
-      <c s="2" r="C137" t="n">
-        <v>42136.177083333336</v>
-      </c>
-      <c r="D137" t="n">
-        <v>4.5</v>
-      </c>
-      <c s="2" r="E137" t="n">
-        <v>42145.9375</v>
-      </c>
-      <c s="2" r="F137" t="n">
-        <v>42148.0625</v>
-      </c>
-      <c r="G137" t="n">
-        <v>16200000000000</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7">
-      <c s="1" r="A138" t="n">
-        <v>141</v>
-      </c>
-      <c s="2" r="B138" t="n">
-        <v>42139.697916666664</v>
-      </c>
-      <c s="2" r="C138" t="n">
-        <v>42139.864583333336</v>
-      </c>
-      <c r="D138" t="n">
-        <v>4.0</v>
-      </c>
-      <c s="2" r="E138" t="n">
-        <v>42148.604166666664</v>
-      </c>
-      <c s="2" r="F138" t="n">
-        <v>42149.21875</v>
-      </c>
-      <c r="G138" t="n">
-        <v>14400000000000</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7">
-      <c s="1" r="A139" t="n">
-        <v>142</v>
-      </c>
-      <c s="2" r="B139" t="n">
-        <v>42140.979166666664</v>
-      </c>
-      <c s="2" r="C139" t="n">
-        <v>42142.177083333336</v>
-      </c>
-      <c r="D139" t="n">
-        <v>28.75</v>
-      </c>
-      <c s="2" r="E139" t="n">
-        <v>42149.541666666664</v>
-      </c>
-      <c s="2" r="F139" t="n">
-        <v>42150.104166666664</v>
-      </c>
-      <c r="G139" t="n">
-        <v>103500000000000</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7">
-      <c s="1" r="A140" t="n">
-        <v>143</v>
-      </c>
-      <c s="2" r="B140" t="n">
-        <v>42145.9375</v>
-      </c>
-      <c s="2" r="C140" t="n">
-        <v>42148.0625</v>
-      </c>
-      <c r="D140" t="n">
-        <v>51.0</v>
-      </c>
-      <c s="2" r="E140" t="n">
-        <v>42167.375</v>
-      </c>
-      <c s="2" r="F140" t="n">
-        <v>42169.177083333336</v>
-      </c>
-      <c r="G140" t="n">
-        <v>183600000000000</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7">
-      <c s="1" r="A141" t="n">
-        <v>144</v>
-      </c>
-      <c s="2" r="B141" t="n">
-        <v>42148.604166666664</v>
-      </c>
-      <c s="2" r="C141" t="n">
-        <v>42149.21875</v>
-      </c>
-      <c r="D141" t="n">
-        <v>14.75</v>
-      </c>
-      <c s="2" r="E141" t="n">
-        <v>42170.322916666664</v>
-      </c>
-      <c s="2" r="F141" t="n">
-        <v>42170.854166666664</v>
-      </c>
-      <c r="G141" t="n">
-        <v>53100000000000</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7">
-      <c s="1" r="A142" t="n">
-        <v>145</v>
-      </c>
-      <c s="2" r="B142" t="n">
-        <v>42149.541666666664</v>
-      </c>
-      <c s="2" r="C142" t="n">
-        <v>42150.104166666664</v>
-      </c>
-      <c r="D142" t="n">
-        <v>13.5</v>
-      </c>
-      <c s="2" r="E142" t="n">
-        <v>42173.010416666664</v>
-      </c>
-      <c s="2" r="F142" t="n">
-        <v>42173.96875</v>
-      </c>
-      <c r="G142" t="n">
-        <v>48600000000000</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7">
-      <c s="1" r="A143" t="n">
-        <v>146</v>
-      </c>
-      <c s="2" r="B143" t="n">
-        <v>42167.375</v>
-      </c>
-      <c s="2" r="C143" t="n">
-        <v>42169.177083333336</v>
-      </c>
-      <c r="D143" t="n">
-        <v>43.25</v>
-      </c>
-      <c r="G143" t="n">
-        <v>155700000000000</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7">
-      <c s="1" r="A144" t="n">
-        <v>147</v>
-      </c>
-      <c s="2" r="B144" t="n">
-        <v>42170.322916666664</v>
-      </c>
-      <c s="2" r="C144" t="n">
-        <v>42170.854166666664</v>
-      </c>
-      <c r="D144" t="n">
-        <v>12.75</v>
-      </c>
-      <c r="G144" t="n">
-        <v>45900000000000</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7">
-      <c s="1" r="A145" t="n">
-        <v>148</v>
-      </c>
-      <c s="2" r="B145" t="n">
-        <v>42173.010416666664</v>
-      </c>
-      <c s="2" r="C145" t="n">
-        <v>42173.96875</v>
-      </c>
-      <c r="D145" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="G145" t="n">
-        <v>82800000000000</v>
+        <v>20700000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>